<commit_message>
Created general layout and added some initial parts of the work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D4F6E1-35B3-9D47-8EFD-F43C366863C1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C315B1-2624-5646-B753-4446A1673C73}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="68720" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Original" sheetId="7" r:id="rId1"/>
-    <sheet name="Original - Old" sheetId="1" r:id="rId2"/>
-    <sheet name="Interim Report - Old" sheetId="3" r:id="rId3"/>
-    <sheet name="Dissertation - Old" sheetId="4" r:id="rId4"/>
+    <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
+    <sheet name="Dissertation - Old" sheetId="4" r:id="rId2"/>
+    <sheet name="Original - Old" sheetId="1" r:id="rId3"/>
+    <sheet name="Interim Report - Old" sheetId="3" r:id="rId4"/>
     <sheet name="Dissertation to print - Old" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="60">
   <si>
     <t>Week</t>
   </si>
@@ -173,13 +173,63 @@
   </si>
   <si>
     <t>G53DIA Coursework</t>
+  </si>
+  <si>
+    <t>12th October
+Project Proposal - Soft</t>
+  </si>
+  <si>
+    <t>SET/SEM Questionaires</t>
+  </si>
+  <si>
+    <t>Create Git repository</t>
+  </si>
+  <si>
+    <t>Set up LaTeX files</t>
+  </si>
+  <si>
+    <t>Start of Autumn Semester</t>
+  </si>
+  <si>
+    <t>Start of Spring Semester</t>
+  </si>
+  <si>
+    <t>Research Paper</t>
+  </si>
+  <si>
+    <t>Basic Reasearch into competition - Not sure what to call this</t>
+  </si>
+  <si>
+    <t>7th December
+Interim Report - 10%</t>
+  </si>
+  <si>
+    <t>12th April
+Dissertation - 75%</t>
+  </si>
+  <si>
+    <t>16/17th May
+Presentation - 15%</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Interrim Report - Break this down?</t>
+  </si>
+  <si>
+    <t>Create Demo for Presentation</t>
+  </si>
+  <si>
+    <t>23rd October
+Revised Project Proposal - 0%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -216,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,8 +309,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8BEFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -373,11 +429,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -435,6 +540,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,6 +576,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFD8BEFF"/>
       <color rgb="FFD883FF"/>
     </mruColors>
   </colors>
@@ -720,16 +854,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AL70"/>
+  <dimension ref="A1:AL63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="31.83203125" customWidth="1"/>
     <col min="2" max="11" width="9.1640625" customWidth="1"/>
@@ -738,7 +869,613 @@
     <col min="36" max="36" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="125" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" s="1" customFormat="1" ht="119">
+      <c r="A1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="40"/>
+      <c r="F1" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="17" thickBot="1">
+      <c r="A2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="47">
+        <v>43367</v>
+      </c>
+      <c r="C2" s="47">
+        <v>43374</v>
+      </c>
+      <c r="D2" s="47">
+        <v>43381</v>
+      </c>
+      <c r="E2" s="47">
+        <v>43388</v>
+      </c>
+      <c r="F2" s="49">
+        <v>43395</v>
+      </c>
+      <c r="G2" s="47">
+        <v>43402</v>
+      </c>
+      <c r="H2" s="47">
+        <v>43409</v>
+      </c>
+      <c r="I2" s="47">
+        <v>43416</v>
+      </c>
+      <c r="J2" s="47">
+        <v>43423</v>
+      </c>
+      <c r="K2" s="47">
+        <v>43430</v>
+      </c>
+      <c r="L2" s="49">
+        <v>43437</v>
+      </c>
+      <c r="M2" s="47">
+        <v>43444</v>
+      </c>
+      <c r="N2" s="47">
+        <v>43451</v>
+      </c>
+      <c r="O2" s="47">
+        <v>43458</v>
+      </c>
+      <c r="P2" s="47">
+        <v>43465</v>
+      </c>
+      <c r="Q2" s="47">
+        <v>43472</v>
+      </c>
+      <c r="R2" s="47">
+        <v>43479</v>
+      </c>
+      <c r="S2" s="47">
+        <v>43486</v>
+      </c>
+      <c r="T2" s="47">
+        <v>43493</v>
+      </c>
+      <c r="U2" s="47">
+        <v>43500</v>
+      </c>
+      <c r="V2" s="47">
+        <v>43507</v>
+      </c>
+      <c r="W2" s="47">
+        <v>43514</v>
+      </c>
+      <c r="X2" s="47">
+        <v>43521</v>
+      </c>
+      <c r="Y2" s="47">
+        <v>43528</v>
+      </c>
+      <c r="Z2" s="47">
+        <v>43535</v>
+      </c>
+      <c r="AA2" s="47">
+        <v>43542</v>
+      </c>
+      <c r="AB2" s="47">
+        <v>43549</v>
+      </c>
+      <c r="AC2" s="47">
+        <v>43556</v>
+      </c>
+      <c r="AD2" s="49">
+        <v>43563</v>
+      </c>
+      <c r="AE2" s="47">
+        <v>43570</v>
+      </c>
+      <c r="AF2" s="47">
+        <v>43577</v>
+      </c>
+      <c r="AG2" s="47">
+        <v>43584</v>
+      </c>
+      <c r="AH2" s="47">
+        <v>43591</v>
+      </c>
+      <c r="AI2" s="47">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="17" thickTop="1">
+      <c r="A3" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="AD3" s="50"/>
+      <c r="AF3" s="28"/>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="AD4" s="50"/>
+      <c r="AF4" s="28"/>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="51"/>
+      <c r="L5" s="50"/>
+      <c r="AD5" s="50"/>
+      <c r="AF5" s="28"/>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" s="45"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="52"/>
+      <c r="L6" s="50"/>
+      <c r="AD6" s="50"/>
+      <c r="AF6" s="28"/>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="50"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="51"/>
+      <c r="AD7" s="50"/>
+      <c r="AF7" s="28"/>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" s="45"/>
+      <c r="F8" s="50"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="52"/>
+      <c r="AD8" s="50"/>
+      <c r="AF8" s="28"/>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" s="45"/>
+      <c r="F9" s="50"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="52"/>
+      <c r="AD9" s="50"/>
+      <c r="AF9" s="28"/>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="50"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="9"/>
+      <c r="AD10" s="50"/>
+      <c r="AF10" s="28"/>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="51"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="28"/>
+    </row>
+    <row r="12" spans="1:35">
+      <c r="A12" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="AD12" s="50"/>
+      <c r="AF12" s="28"/>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="F13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="AD13" s="50"/>
+      <c r="AF13" s="28"/>
+    </row>
+    <row r="14" spans="1:35">
+      <c r="A14" s="60"/>
+      <c r="F14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="AD14" s="50"/>
+      <c r="AF14" s="28"/>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="A15" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="AD15" s="50"/>
+      <c r="AF15" s="28"/>
+    </row>
+    <row r="16" spans="1:35">
+      <c r="A16" s="60"/>
+      <c r="F16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="AD16" s="50"/>
+      <c r="AF16" s="28"/>
+    </row>
+    <row r="17" spans="1:38">
+      <c r="A17" s="60"/>
+      <c r="F17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="AD17" s="50"/>
+      <c r="AF17" s="28"/>
+    </row>
+    <row r="18" spans="1:38">
+      <c r="A18" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="AD18" s="50"/>
+      <c r="AF18" s="28"/>
+    </row>
+    <row r="19" spans="1:38">
+      <c r="A19" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="AD19" s="50"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="59"/>
+      <c r="AH19" s="59"/>
+    </row>
+    <row r="20" spans="1:38">
+      <c r="A20" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="AD20" s="50"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="59"/>
+      <c r="AH20" s="59"/>
+    </row>
+    <row r="21" spans="1:38">
+      <c r="A21" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="AD21" s="50"/>
+      <c r="AF21" s="28"/>
+      <c r="AI21" s="59"/>
+    </row>
+    <row r="22" spans="1:38">
+      <c r="A22" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="AD22" s="50"/>
+      <c r="AF22" s="28"/>
+    </row>
+    <row r="23" spans="1:38">
+      <c r="A23" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="F23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="AD23" s="50"/>
+      <c r="AF23" s="28"/>
+    </row>
+    <row r="24" spans="1:38">
+      <c r="A24" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="F24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="AD24" s="50"/>
+      <c r="AF24" s="28"/>
+    </row>
+    <row r="25" spans="1:38">
+      <c r="A25" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="AB25" s="24"/>
+      <c r="AC25" s="24"/>
+      <c r="AD25" s="50"/>
+      <c r="AF25" s="28"/>
+      <c r="AI25" s="12"/>
+    </row>
+    <row r="26" spans="1:38">
+      <c r="A26" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="AD26" s="50"/>
+      <c r="AF26" s="28"/>
+    </row>
+    <row r="27" spans="1:38">
+      <c r="A27" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="F27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="AD27" s="50"/>
+      <c r="AF27" s="28"/>
+    </row>
+    <row r="28" spans="1:38" s="28" customFormat="1">
+      <c r="A28" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28" s="50"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28" s="50"/>
+      <c r="M28"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+      <c r="AB28"/>
+      <c r="AC28"/>
+      <c r="AD28" s="50"/>
+      <c r="AE28"/>
+      <c r="AL28" s="39"/>
+    </row>
+    <row r="29" spans="1:38" s="28" customFormat="1">
+      <c r="A29" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29" s="50"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29" s="50"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+      <c r="Z29"/>
+      <c r="AA29"/>
+      <c r="AB29"/>
+      <c r="AC29"/>
+      <c r="AD29" s="50"/>
+      <c r="AE29"/>
+    </row>
+    <row r="30" spans="1:38" s="28" customFormat="1">
+      <c r="A30" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30" s="50"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30" s="50"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+      <c r="AB30" s="9"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="52"/>
+      <c r="AE30" s="8"/>
+      <c r="AF30" s="62"/>
+      <c r="AG30" s="62"/>
+      <c r="AH30" s="62"/>
+    </row>
+    <row r="31" spans="1:38" s="28" customFormat="1"/>
+    <row r="32" spans="1:38" s="28" customFormat="1"/>
+    <row r="33" s="28" customFormat="1"/>
+    <row r="34" s="28" customFormat="1"/>
+    <row r="35" s="28" customFormat="1"/>
+    <row r="36" s="28" customFormat="1"/>
+    <row r="37" s="28" customFormat="1"/>
+    <row r="38" s="28" customFormat="1"/>
+    <row r="39" s="28" customFormat="1"/>
+    <row r="40" s="28" customFormat="1"/>
+    <row r="41" s="28" customFormat="1"/>
+    <row r="42" s="28" customFormat="1"/>
+    <row r="43" s="28" customFormat="1"/>
+    <row r="44" s="28" customFormat="1"/>
+    <row r="45" s="28" customFormat="1"/>
+    <row r="46" s="28" customFormat="1"/>
+    <row r="47" s="28" customFormat="1"/>
+    <row r="48" s="28" customFormat="1"/>
+    <row r="49" spans="1:1" s="28" customFormat="1"/>
+    <row r="50" spans="1:1" s="28" customFormat="1"/>
+    <row r="51" spans="1:1" s="28" customFormat="1"/>
+    <row r="52" spans="1:1" s="28" customFormat="1"/>
+    <row r="53" spans="1:1" s="28" customFormat="1"/>
+    <row r="54" spans="1:1" s="28" customFormat="1"/>
+    <row r="55" spans="1:1" s="28" customFormat="1"/>
+    <row r="56" spans="1:1" s="28" customFormat="1"/>
+    <row r="57" spans="1:1" s="28" customFormat="1"/>
+    <row r="58" spans="1:1" s="28" customFormat="1"/>
+    <row r="59" spans="1:1" s="28" customFormat="1"/>
+    <row r="60" spans="1:1" s="28" customFormat="1"/>
+    <row r="61" spans="1:1">
+      <c r="A61" s="28"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="28"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AL70"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="28" customWidth="1"/>
+    <col min="13" max="35" width="9.1640625" customWidth="1"/>
+    <col min="36" max="36" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="125">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -790,7 +1527,7 @@
       </c>
       <c r="AJ1" s="40"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -898,14 +1635,14 @@
       </c>
       <c r="AJ2" s="15"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="5"/>
       <c r="AF3" s="5"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -914,7 +1651,7 @@
       <c r="L4" s="5"/>
       <c r="AF4" s="5"/>
     </row>
-    <row r="5" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="17" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -924,7 +1661,7 @@
       <c r="L5" s="5"/>
       <c r="AF5" s="5"/>
     </row>
-    <row r="6" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="17" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -935,7 +1672,7 @@
       <c r="L6" s="26"/>
       <c r="AF6" s="5"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -958,7 +1695,7 @@
       <c r="AA7" s="7"/>
       <c r="AF7" s="5"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -969,14 +1706,14 @@
       <c r="AE8" s="7"/>
       <c r="AF8" s="5"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="5"/>
       <c r="AF9" s="5"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -984,7 +1721,7 @@
       <c r="L10" s="5"/>
       <c r="AF10" s="5"/>
     </row>
-    <row r="11" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" ht="17" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -992,7 +1729,7 @@
       <c r="L11" s="5"/>
       <c r="AF11" s="5"/>
     </row>
-    <row r="12" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="17" thickBot="1">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1001,7 +1738,7 @@
       <c r="L12" s="5"/>
       <c r="AF12" s="5"/>
     </row>
-    <row r="13" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" ht="17" thickBot="1">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -1011,7 +1748,7 @@
       <c r="M13" s="23"/>
       <c r="AF13" s="5"/>
     </row>
-    <row r="14" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" ht="17" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -1023,14 +1760,14 @@
       <c r="X14" s="23"/>
       <c r="AF14" s="5"/>
     </row>
-    <row r="15" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" ht="17" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="L15" s="5"/>
       <c r="AF15" s="5"/>
     </row>
-    <row r="16" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" ht="17" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1040,7 +1777,7 @@
       <c r="L16" s="5"/>
       <c r="AF16" s="5"/>
     </row>
-    <row r="17" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="17" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -1050,7 +1787,7 @@
       <c r="L17" s="5"/>
       <c r="AF17" s="5"/>
     </row>
-    <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="17" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1059,7 +1796,7 @@
       <c r="M18" s="20"/>
       <c r="AF18" s="5"/>
     </row>
-    <row r="19" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="17" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1070,7 +1807,7 @@
       <c r="N19" s="22"/>
       <c r="AF19" s="5"/>
     </row>
-    <row r="20" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="17" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -1083,7 +1820,7 @@
       <c r="Q20" s="24"/>
       <c r="AF20" s="5"/>
     </row>
-    <row r="21" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="17" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1099,7 +1836,7 @@
       <c r="U21" s="22"/>
       <c r="AF21" s="5"/>
     </row>
-    <row r="22" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="17" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
@@ -1113,7 +1850,7 @@
       <c r="Q22" s="29"/>
       <c r="AF22" s="5"/>
     </row>
-    <row r="23" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="17" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
@@ -1127,7 +1864,7 @@
       <c r="Z23" s="38"/>
       <c r="AF23" s="5"/>
     </row>
-    <row r="24" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="17" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
@@ -1143,7 +1880,7 @@
       <c r="AC24" s="9"/>
       <c r="AF24" s="5"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35">
       <c r="A25" s="6" t="s">
         <v>39</v>
       </c>
@@ -1152,7 +1889,7 @@
       <c r="U25" s="9"/>
       <c r="AF25" s="5"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -1161,7 +1898,7 @@
       <c r="AG26" s="31"/>
       <c r="AH26" s="31"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35">
       <c r="A27" s="5" t="s">
         <v>41</v>
       </c>
@@ -1169,14 +1906,14 @@
       <c r="AF27" s="5"/>
       <c r="AI27" s="31"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L28" s="5"/>
       <c r="AF28" s="5"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35">
       <c r="A29" s="5" t="s">
         <v>22</v>
       </c>
@@ -1185,7 +1922,7 @@
       <c r="L29" s="5"/>
       <c r="AF29" s="5"/>
     </row>
-    <row r="30" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="17" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
@@ -1196,7 +1933,7 @@
       <c r="S30" s="9"/>
       <c r="AF30" s="5"/>
     </row>
-    <row r="31" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="17" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
@@ -1209,14 +1946,14 @@
       <c r="AC31" s="35"/>
       <c r="AF31" s="5"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35">
       <c r="A32" s="6" t="s">
         <v>11</v>
       </c>
       <c r="L32" s="5"/>
       <c r="AF32" s="5"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
@@ -1224,7 +1961,7 @@
       <c r="L33" s="5"/>
       <c r="AF33" s="5"/>
     </row>
-    <row r="34" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" s="28" customFormat="1">
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
@@ -1261,7 +1998,7 @@
       <c r="AF34" s="5"/>
       <c r="AL34" s="39"/>
     </row>
-    <row r="35" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A35" s="5" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +2034,7 @@
       <c r="AE35"/>
       <c r="AF35" s="5"/>
     </row>
-    <row r="36" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A36" s="5" t="s">
         <v>44</v>
       </c>
@@ -1333,7 +2070,7 @@
       <c r="AE36"/>
       <c r="AF36" s="5"/>
     </row>
-    <row r="37" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" s="28" customFormat="1">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -1369,43 +2106,43 @@
       <c r="AE37" s="8"/>
       <c r="AF37" s="5"/>
     </row>
-    <row r="38" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" s="28" customFormat="1"/>
+    <row r="39" spans="1:38" s="28" customFormat="1"/>
+    <row r="40" spans="1:38" s="28" customFormat="1"/>
+    <row r="41" spans="1:38" s="28" customFormat="1"/>
+    <row r="42" spans="1:38" s="28" customFormat="1"/>
+    <row r="43" spans="1:38" s="28" customFormat="1"/>
+    <row r="44" spans="1:38" s="28" customFormat="1"/>
+    <row r="45" spans="1:38" s="28" customFormat="1"/>
+    <row r="46" spans="1:38" s="28" customFormat="1"/>
+    <row r="47" spans="1:38" s="28" customFormat="1"/>
+    <row r="48" spans="1:38" s="28" customFormat="1"/>
+    <row r="49" s="28" customFormat="1"/>
+    <row r="50" s="28" customFormat="1"/>
+    <row r="51" s="28" customFormat="1"/>
+    <row r="52" s="28" customFormat="1"/>
+    <row r="53" s="28" customFormat="1"/>
+    <row r="54" s="28" customFormat="1"/>
+    <row r="55" s="28" customFormat="1"/>
+    <row r="56" s="28" customFormat="1"/>
+    <row r="57" s="28" customFormat="1"/>
+    <row r="58" s="28" customFormat="1"/>
+    <row r="59" s="28" customFormat="1"/>
+    <row r="60" s="28" customFormat="1"/>
+    <row r="61" s="28" customFormat="1"/>
+    <row r="62" s="28" customFormat="1"/>
+    <row r="63" s="28" customFormat="1"/>
+    <row r="64" s="28" customFormat="1"/>
+    <row r="65" spans="1:1" s="28" customFormat="1"/>
+    <row r="66" spans="1:1" s="28" customFormat="1"/>
+    <row r="67" spans="1:1" s="28" customFormat="1"/>
+    <row r="68" spans="1:1">
       <c r="A68" s="28"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" s="28"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" s="28"/>
     </row>
   </sheetData>
@@ -1414,7 +2151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH43"/>
   <sheetViews>
@@ -1425,13 +2162,13 @@
       <selection pane="bottomRight" activeCell="O21" sqref="O21:Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="34" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" ht="131" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" s="1" customFormat="1" ht="131">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1454,7 +2191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1556,19 +2293,19 @@
       </c>
       <c r="AH2" s="2"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1576,14 +2313,14 @@
       <c r="D5" s="9"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -1605,7 +2342,7 @@
       <c r="Z7" s="9"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -1614,30 +2351,30 @@
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -1646,7 +2383,7 @@
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -1655,25 +2392,25 @@
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1681,7 +2418,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1690,7 +2427,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -1700,7 +2437,7 @@
       <c r="N20" s="10"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31">
       <c r="A21" s="5" t="s">
         <v>29</v>
       </c>
@@ -1713,14 +2450,14 @@
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31">
       <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
@@ -1730,7 +2467,7 @@
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31">
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
@@ -1741,21 +2478,21 @@
       <c r="Y24" s="10"/>
       <c r="Z24" s="10"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31">
       <c r="A25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T25" s="9"/>
       <c r="U25" s="9"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31">
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
@@ -1764,18 +2501,18 @@
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31">
       <c r="A28" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="8"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -1785,14 +2522,14 @@
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31">
       <c r="A31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31">
       <c r="A32" s="5" t="s">
         <v>16</v>
       </c>
@@ -1801,37 +2538,37 @@
       <c r="AD32" s="8"/>
       <c r="AE32" s="8"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="5"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="5"/>
     </row>
   </sheetData>
@@ -1841,7 +2578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
@@ -1852,7 +2589,7 @@
       <selection pane="bottomRight" activeCell="Y26" sqref="Y26:Z26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="11" width="7.5" customWidth="1"/>
@@ -1860,7 +2597,7 @@
     <col min="13" max="34" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="131" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="131">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1883,7 +2620,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1993,13 +2730,13 @@
         <v>43241</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -2007,7 +2744,7 @@
       <c r="D4" s="7"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="17" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -2016,7 +2753,7 @@
       <c r="E5" s="7"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="17" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -2026,7 +2763,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -2048,7 +2785,7 @@
       <c r="Z7" s="9"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -2058,27 +2795,27 @@
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="11"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" ht="17" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="11"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="17" thickBot="1">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -2086,7 +2823,7 @@
       <c r="I12" s="23"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" ht="17" thickBot="1">
       <c r="A13" s="28" t="s">
         <v>38</v>
       </c>
@@ -2095,7 +2832,7 @@
       <c r="J13" s="23"/>
       <c r="M13" s="23"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36">
       <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
@@ -2105,7 +2842,7 @@
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -2115,13 +2852,13 @@
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
     </row>
-    <row r="16" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" ht="17" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="17" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -2130,7 +2867,7 @@
       <c r="H17" s="20"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="17" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -2139,7 +2876,7 @@
       <c r="I18" s="22"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="17" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -2147,7 +2884,7 @@
       <c r="J19" s="19"/>
       <c r="M19" s="20"/>
     </row>
-    <row r="20" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="17" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -2157,7 +2894,7 @@
       <c r="M20" s="21"/>
       <c r="N20" s="22"/>
     </row>
-    <row r="21" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="17" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -2169,7 +2906,7 @@
       <c r="P21" s="22"/>
       <c r="Q21" s="24"/>
     </row>
-    <row r="22" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="17" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2182,7 +2919,7 @@
       <c r="Q22" s="30"/>
       <c r="S22" s="19"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35">
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
@@ -2195,7 +2932,7 @@
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -2203,7 +2940,7 @@
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35">
       <c r="A25" s="5" t="s">
         <v>34</v>
       </c>
@@ -2214,7 +2951,7 @@
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35">
       <c r="A26" s="5" t="s">
         <v>36</v>
       </c>
@@ -2226,7 +2963,7 @@
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35">
       <c r="A27" s="6" t="s">
         <v>39</v>
       </c>
@@ -2234,7 +2971,7 @@
       <c r="T27" s="9"/>
       <c r="U27" s="9"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35">
       <c r="A28" s="5" t="s">
         <v>42</v>
       </c>
@@ -2242,20 +2979,20 @@
       <c r="AG28" s="31"/>
       <c r="AH28" s="31"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35">
       <c r="A29" s="5" t="s">
         <v>41</v>
       </c>
       <c r="L29" s="5"/>
       <c r="AI29" s="31"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35">
       <c r="A30" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35">
       <c r="A31" s="5" t="s">
         <v>22</v>
       </c>
@@ -2263,7 +3000,7 @@
       <c r="G31" s="12"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35">
       <c r="A32" s="5" t="s">
         <v>27</v>
       </c>
@@ -2273,20 +3010,20 @@
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31">
       <c r="A33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31">
       <c r="A34" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="8"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" s="28" customFormat="1">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -2321,7 +3058,7 @@
       <c r="AD35"/>
       <c r="AE35"/>
     </row>
-    <row r="36" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" s="28" customFormat="1">
       <c r="A36" s="5" t="s">
         <v>13</v>
       </c>
@@ -2356,7 +3093,7 @@
       <c r="AD36"/>
       <c r="AE36"/>
     </row>
-    <row r="37" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" s="28" customFormat="1">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -2391,739 +3128,43 @@
       <c r="AD37" s="8"/>
       <c r="AE37" s="8"/>
     </row>
-    <row r="38" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" s="28" customFormat="1"/>
+    <row r="39" spans="1:31" s="28" customFormat="1"/>
+    <row r="40" spans="1:31" s="28" customFormat="1"/>
+    <row r="41" spans="1:31" s="28" customFormat="1"/>
+    <row r="42" spans="1:31" s="28" customFormat="1"/>
+    <row r="43" spans="1:31" s="28" customFormat="1"/>
+    <row r="44" spans="1:31" s="28" customFormat="1"/>
+    <row r="45" spans="1:31" s="28" customFormat="1"/>
+    <row r="46" spans="1:31" s="28" customFormat="1"/>
+    <row r="47" spans="1:31" s="28" customFormat="1"/>
+    <row r="48" spans="1:31" s="28" customFormat="1"/>
+    <row r="49" s="28" customFormat="1"/>
+    <row r="50" s="28" customFormat="1"/>
+    <row r="51" s="28" customFormat="1"/>
+    <row r="52" s="28" customFormat="1"/>
+    <row r="53" s="28" customFormat="1"/>
+    <row r="54" s="28" customFormat="1"/>
+    <row r="55" s="28" customFormat="1"/>
+    <row r="56" s="28" customFormat="1"/>
+    <row r="57" s="28" customFormat="1"/>
+    <row r="58" s="28" customFormat="1"/>
+    <row r="59" s="28" customFormat="1"/>
+    <row r="60" s="28" customFormat="1"/>
+    <row r="61" s="28" customFormat="1"/>
+    <row r="62" s="28" customFormat="1"/>
+    <row r="63" s="28" customFormat="1"/>
+    <row r="64" s="28" customFormat="1"/>
+    <row r="65" spans="1:1" s="28" customFormat="1"/>
+    <row r="66" spans="1:1" s="28" customFormat="1"/>
+    <row r="67" spans="1:1" s="28" customFormat="1"/>
+    <row r="68" spans="1:1">
       <c r="A68" s="28"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" s="28"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AL70"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="28" customWidth="1"/>
-    <col min="13" max="35" width="9.1640625" customWidth="1"/>
-    <col min="36" max="36" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="125" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ1" s="40"/>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="15">
-        <v>43003</v>
-      </c>
-      <c r="C2" s="15">
-        <v>43010</v>
-      </c>
-      <c r="D2" s="15">
-        <v>43017</v>
-      </c>
-      <c r="E2" s="15">
-        <v>43024</v>
-      </c>
-      <c r="F2" s="15">
-        <v>43031</v>
-      </c>
-      <c r="G2" s="15">
-        <v>43038</v>
-      </c>
-      <c r="H2" s="15">
-        <v>43045</v>
-      </c>
-      <c r="I2" s="15">
-        <v>43052</v>
-      </c>
-      <c r="J2" s="15">
-        <v>43059</v>
-      </c>
-      <c r="K2" s="15">
-        <v>43066</v>
-      </c>
-      <c r="L2" s="41">
-        <v>43073</v>
-      </c>
-      <c r="M2" s="15">
-        <v>43080</v>
-      </c>
-      <c r="N2" s="15">
-        <v>43087</v>
-      </c>
-      <c r="O2" s="15">
-        <v>43094</v>
-      </c>
-      <c r="P2" s="15">
-        <v>43101</v>
-      </c>
-      <c r="Q2" s="15">
-        <v>43108</v>
-      </c>
-      <c r="R2" s="15">
-        <v>43115</v>
-      </c>
-      <c r="S2" s="15">
-        <v>43122</v>
-      </c>
-      <c r="T2" s="15">
-        <v>43129</v>
-      </c>
-      <c r="U2" s="15">
-        <v>43136</v>
-      </c>
-      <c r="V2" s="15">
-        <v>43143</v>
-      </c>
-      <c r="W2" s="15">
-        <v>43150</v>
-      </c>
-      <c r="X2" s="15">
-        <v>43157</v>
-      </c>
-      <c r="Y2" s="15">
-        <v>43164</v>
-      </c>
-      <c r="Z2" s="15">
-        <v>43171</v>
-      </c>
-      <c r="AA2" s="15">
-        <v>43178</v>
-      </c>
-      <c r="AB2" s="15">
-        <v>43185</v>
-      </c>
-      <c r="AC2" s="15">
-        <v>43192</v>
-      </c>
-      <c r="AD2" s="15">
-        <v>43199</v>
-      </c>
-      <c r="AE2" s="15">
-        <v>43206</v>
-      </c>
-      <c r="AF2" s="41">
-        <v>43213</v>
-      </c>
-      <c r="AG2" s="15">
-        <v>43220</v>
-      </c>
-      <c r="AH2" s="15">
-        <v>43227</v>
-      </c>
-      <c r="AI2" s="15">
-        <v>43234</v>
-      </c>
-      <c r="AJ2" s="15"/>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="AF3" s="5"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="L4" s="5"/>
-      <c r="AF4" s="5"/>
-    </row>
-    <row r="5" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="7"/>
-      <c r="L5" s="5"/>
-      <c r="AF5" s="5"/>
-    </row>
-    <row r="6" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="26"/>
-      <c r="AF6" s="5"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="7"/>
-      <c r="AF7" s="5"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="5"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="5"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="AF9" s="5"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="L10" s="5"/>
-      <c r="AF10" s="5"/>
-    </row>
-    <row r="11" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="L11" s="5"/>
-      <c r="AF11" s="5"/>
-    </row>
-    <row r="12" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="23"/>
-      <c r="L12" s="5"/>
-      <c r="AF12" s="5"/>
-    </row>
-    <row r="13" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="AF13" s="5"/>
-    </row>
-    <row r="14" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="5"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="X14" s="23"/>
-      <c r="AF14" s="5"/>
-    </row>
-    <row r="15" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" s="5"/>
-      <c r="AF15" s="5"/>
-    </row>
-    <row r="16" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="20"/>
-      <c r="L16" s="5"/>
-      <c r="AF16" s="5"/>
-    </row>
-    <row r="17" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="L17" s="5"/>
-      <c r="AF17" s="5"/>
-    </row>
-    <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="19"/>
-      <c r="M18" s="20"/>
-      <c r="AF18" s="5"/>
-    </row>
-    <row r="19" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="22"/>
-      <c r="AF19" s="5"/>
-    </row>
-    <row r="20" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="27"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="24"/>
-      <c r="AF20" s="5"/>
-    </row>
-    <row r="21" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="Q21" s="30"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="22"/>
-      <c r="AF21" s="5"/>
-    </row>
-    <row r="22" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="AF22" s="5"/>
-    </row>
-    <row r="23" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L23" s="5"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="21"/>
-      <c r="Z23" s="38"/>
-      <c r="AF23" s="5"/>
-    </row>
-    <row r="24" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24" s="5"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="Y24" s="24"/>
-      <c r="Z24" s="21"/>
-      <c r="AA24" s="22"/>
-      <c r="AB24" s="9"/>
-      <c r="AC24" s="9"/>
-      <c r="AF24" s="5"/>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" s="5"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="AF25" s="5"/>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="5"/>
-      <c r="AF26" s="5"/>
-      <c r="AG26" s="31"/>
-      <c r="AH26" s="31"/>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L27" s="5"/>
-      <c r="AF27" s="5"/>
-      <c r="AI27" s="31"/>
-    </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L28" s="5"/>
-      <c r="AF28" s="5"/>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="L29" s="5"/>
-      <c r="AF29" s="5"/>
-    </row>
-    <row r="30" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" s="5"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="AF30" s="5"/>
-    </row>
-    <row r="31" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L31" s="5"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="AB31" s="34"/>
-      <c r="AC31" s="35"/>
-      <c r="AF31" s="5"/>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32" s="5"/>
-      <c r="AF32" s="5"/>
-    </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="L33" s="5"/>
-      <c r="AF33" s="5"/>
-    </row>
-    <row r="34" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34" s="5"/>
-      <c r="M34"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-      <c r="AF34" s="5"/>
-      <c r="AL34" s="39"/>
-    </row>
-    <row r="35" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35" s="5"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35" s="5"/>
-    </row>
-    <row r="36" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36" s="5"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36" s="36"/>
-      <c r="W36" s="37"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36" s="36"/>
-      <c r="AB36" s="37"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-      <c r="AF36" s="5"/>
-    </row>
-    <row r="37" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37" s="5"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37" s="8"/>
-      <c r="AC37" s="8"/>
-      <c r="AD37" s="8"/>
-      <c r="AE37" s="8"/>
-      <c r="AF37" s="5"/>
-    </row>
-    <row r="38" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="28"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="28"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" s="28"/>
     </row>
   </sheetData>
@@ -3136,11 +3177,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AL220"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:M111"/>
+    <sheetView zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="31.83203125" customWidth="1"/>
     <col min="2" max="11" width="9.1640625" customWidth="1"/>
@@ -3149,7 +3190,7 @@
     <col min="36" max="36" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="88" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="88">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -3174,7 +3215,7 @@
       </c>
       <c r="AJ1" s="40"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3213,13 +3254,13 @@
       </c>
       <c r="AJ2" s="15"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -3227,7 +3268,7 @@
       <c r="D4" s="7"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="17" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -3236,7 +3277,7 @@
       <c r="E5" s="7"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="17" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -3246,40 +3287,40 @@
       <c r="K6" s="7"/>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="11"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" ht="17" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="11"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="17" thickBot="1">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -3287,7 +3328,7 @@
       <c r="I12" s="23"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" ht="17" thickBot="1">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -3296,19 +3337,19 @@
       <c r="J13" s="23"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" ht="17" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" ht="17" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -3317,7 +3358,7 @@
       <c r="H16" s="20"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="17" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -3326,7 +3367,7 @@
       <c r="I17" s="22"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="17" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -3334,7 +3375,7 @@
       <c r="J18" s="19"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -3343,7 +3384,7 @@
       <c r="K19" s="24"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3352,7 +3393,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
@@ -3360,7 +3401,7 @@
       <c r="K21" s="9"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
@@ -3368,43 +3409,43 @@
       <c r="K22" s="9"/>
       <c r="L22" s="27"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="6" t="s">
         <v>39</v>
       </c>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="5" t="s">
         <v>41</v>
       </c>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="5" t="s">
         <v>22</v>
       </c>
@@ -3412,32 +3453,32 @@
       <c r="G29" s="12"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
         <v>11</v>
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="8"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" s="28" customFormat="1">
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
@@ -3454,7 +3495,7 @@
       <c r="L34" s="5"/>
       <c r="AL34" s="39"/>
     </row>
-    <row r="35" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" s="28" customFormat="1">
       <c r="A35" s="5" t="s">
         <v>13</v>
       </c>
@@ -3470,7 +3511,7 @@
       <c r="K35"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" s="28" customFormat="1">
       <c r="A36" s="5" t="s">
         <v>44</v>
       </c>
@@ -3486,7 +3527,7 @@
       <c r="K36"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" s="28" customFormat="1">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -3502,7 +3543,7 @@
       <c r="K37"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:38" s="28" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" s="28" customFormat="1" ht="17">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -3518,7 +3559,7 @@
       <c r="K38" s="40"/>
       <c r="L38" s="40"/>
     </row>
-    <row r="39" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" s="28" customFormat="1">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -3556,7 +3597,7 @@
         <v>43150</v>
       </c>
     </row>
-    <row r="40" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" s="28" customFormat="1">
       <c r="A40" s="6" t="s">
         <v>7</v>
       </c>
@@ -3572,7 +3613,7 @@
       <c r="K40"/>
       <c r="L40"/>
     </row>
-    <row r="41" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" s="28" customFormat="1">
       <c r="A41" s="5" t="s">
         <v>14</v>
       </c>
@@ -3588,7 +3629,7 @@
       <c r="K41"/>
       <c r="L41"/>
     </row>
-    <row r="42" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" s="28" customFormat="1">
       <c r="A42" s="5" t="s">
         <v>21</v>
       </c>
@@ -3604,7 +3645,7 @@
       <c r="K42"/>
       <c r="L42"/>
     </row>
-    <row r="43" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" s="28" customFormat="1">
       <c r="A43" s="5" t="s">
         <v>18</v>
       </c>
@@ -3620,7 +3661,7 @@
       <c r="K43"/>
       <c r="L43"/>
     </row>
-    <row r="44" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" s="28" customFormat="1">
       <c r="A44" s="5" t="s">
         <v>35</v>
       </c>
@@ -3636,7 +3677,7 @@
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
     </row>
-    <row r="45" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" s="28" customFormat="1">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -3652,7 +3693,7 @@
       <c r="K45"/>
       <c r="L45"/>
     </row>
-    <row r="46" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" s="28" customFormat="1">
       <c r="A46" s="6" t="s">
         <v>9</v>
       </c>
@@ -3668,7 +3709,7 @@
       <c r="K46"/>
       <c r="L46"/>
     </row>
-    <row r="47" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" s="28" customFormat="1">
       <c r="A47" s="5" t="s">
         <v>31</v>
       </c>
@@ -3684,7 +3725,7 @@
       <c r="K47"/>
       <c r="L47"/>
     </row>
-    <row r="48" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" s="28" customFormat="1">
       <c r="A48" s="5" t="s">
         <v>32</v>
       </c>
@@ -3700,7 +3741,7 @@
       <c r="K48"/>
       <c r="L48"/>
     </row>
-    <row r="49" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A49" s="5" t="s">
         <v>23</v>
       </c>
@@ -3716,7 +3757,7 @@
       <c r="K49"/>
       <c r="L49"/>
     </row>
-    <row r="50" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A50" s="5" t="s">
         <v>38</v>
       </c>
@@ -3732,7 +3773,7 @@
       <c r="K50"/>
       <c r="L50"/>
     </row>
-    <row r="51" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" s="28" customFormat="1">
       <c r="A51" s="5" t="s">
         <v>33</v>
       </c>
@@ -3748,7 +3789,7 @@
       <c r="K51"/>
       <c r="L51"/>
     </row>
-    <row r="52" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" s="28" customFormat="1">
       <c r="A52" s="6" t="s">
         <v>8</v>
       </c>
@@ -3764,7 +3805,7 @@
       <c r="K52"/>
       <c r="L52"/>
     </row>
-    <row r="53" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" s="28" customFormat="1">
       <c r="A53" s="5" t="s">
         <v>19</v>
       </c>
@@ -3780,7 +3821,7 @@
       <c r="K53"/>
       <c r="L53"/>
     </row>
-    <row r="54" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A54" s="5" t="s">
         <v>37</v>
       </c>
@@ -3796,7 +3837,7 @@
       <c r="K54"/>
       <c r="L54"/>
     </row>
-    <row r="55" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A55" s="5" t="s">
         <v>23</v>
       </c>
@@ -3812,7 +3853,7 @@
       <c r="K55"/>
       <c r="L55"/>
     </row>
-    <row r="56" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A56" s="5" t="s">
         <v>25</v>
       </c>
@@ -3828,7 +3869,7 @@
       <c r="K56"/>
       <c r="L56"/>
     </row>
-    <row r="57" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A57" s="5" t="s">
         <v>26</v>
       </c>
@@ -3844,7 +3885,7 @@
       <c r="K57"/>
       <c r="L57"/>
     </row>
-    <row r="58" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" s="28" customFormat="1" ht="17" thickBot="1">
       <c r="A58" s="5" t="s">
         <v>24</v>
       </c>
@@ -3860,7 +3901,7 @@
       <c r="K58"/>
       <c r="L58"/>
     </row>
-    <row r="59" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" s="28" customFormat="1">
       <c r="A59" s="5" t="s">
         <v>29</v>
       </c>
@@ -3876,7 +3917,7 @@
       <c r="K59"/>
       <c r="L59"/>
     </row>
-    <row r="60" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" s="28" customFormat="1">
       <c r="A60" s="5" t="s">
         <v>34</v>
       </c>
@@ -3892,7 +3933,7 @@
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" s="28" customFormat="1">
       <c r="A61" s="5" t="s">
         <v>36</v>
       </c>
@@ -3908,7 +3949,7 @@
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
     </row>
-    <row r="62" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" s="28" customFormat="1">
       <c r="A62" s="6" t="s">
         <v>39</v>
       </c>
@@ -3924,7 +3965,7 @@
       <c r="K62"/>
       <c r="L62"/>
     </row>
-    <row r="63" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" s="28" customFormat="1">
       <c r="A63" s="5" t="s">
         <v>42</v>
       </c>
@@ -3940,7 +3981,7 @@
       <c r="K63"/>
       <c r="L63"/>
     </row>
-    <row r="64" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" s="28" customFormat="1">
       <c r="A64" s="5" t="s">
         <v>41</v>
       </c>
@@ -3956,7 +3997,7 @@
       <c r="K64"/>
       <c r="L64"/>
     </row>
-    <row r="65" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="28" customFormat="1">
       <c r="A65" s="6" t="s">
         <v>10</v>
       </c>
@@ -3972,7 +4013,7 @@
       <c r="K65"/>
       <c r="L65"/>
     </row>
-    <row r="66" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="28" customFormat="1">
       <c r="A66" s="5" t="s">
         <v>22</v>
       </c>
@@ -3988,7 +4029,7 @@
       <c r="K66"/>
       <c r="L66"/>
     </row>
-    <row r="67" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="28" customFormat="1">
       <c r="A67" s="5" t="s">
         <v>27</v>
       </c>
@@ -4004,7 +4045,7 @@
       <c r="K67"/>
       <c r="L67"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13">
       <c r="A68" s="5" t="s">
         <v>43</v>
       </c>
@@ -4014,19 +4055,19 @@
       <c r="H68" s="9"/>
       <c r="L68"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13">
       <c r="A69" s="6" t="s">
         <v>11</v>
       </c>
       <c r="L69"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13">
       <c r="A70" s="5" t="s">
         <v>12</v>
       </c>
       <c r="L70"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13">
       <c r="A71" s="5" t="s">
         <v>15</v>
       </c>
@@ -4036,7 +4077,7 @@
       <c r="F71" s="8"/>
       <c r="L71"/>
     </row>
-    <row r="72" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="17" thickBot="1">
       <c r="A72" s="5" t="s">
         <v>13</v>
       </c>
@@ -4044,7 +4085,7 @@
       <c r="H72" s="8"/>
       <c r="L72"/>
     </row>
-    <row r="73" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="17" thickBot="1">
       <c r="A73" s="5" t="s">
         <v>44</v>
       </c>
@@ -4053,12 +4094,12 @@
       <c r="K73" s="36"/>
       <c r="L73" s="37"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" ht="77" customHeight="1">
       <c r="A75" s="3" t="s">
         <v>1</v>
       </c>
@@ -4079,7 +4120,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13">
       <c r="A76" s="4" t="s">
         <v>0</v>
       </c>
@@ -4120,35 +4161,35 @@
         <v>43234</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13">
       <c r="A77" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J77" s="5"/>
       <c r="L77"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13">
       <c r="A78" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J78" s="5"/>
       <c r="L78"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13">
       <c r="A79" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J79" s="5"/>
       <c r="L79"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13">
       <c r="A80" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J80" s="5"/>
       <c r="L80"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12">
       <c r="A81" s="5" t="s">
         <v>35</v>
       </c>
@@ -4159,7 +4200,7 @@
       <c r="J81" s="5"/>
       <c r="L81"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12">
       <c r="A82" s="5" t="s">
         <v>17</v>
       </c>
@@ -4170,42 +4211,42 @@
       <c r="J82" s="5"/>
       <c r="L82"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12">
       <c r="A83" s="6" t="s">
         <v>9</v>
       </c>
       <c r="J83" s="5"/>
       <c r="L83"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12">
       <c r="A84" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J84" s="5"/>
       <c r="L84"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12">
       <c r="A85" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J85" s="5"/>
       <c r="L85"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12">
       <c r="A86" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J86" s="5"/>
       <c r="L86"/>
     </row>
-    <row r="87" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="17" thickBot="1">
       <c r="A87" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J87" s="5"/>
       <c r="L87"/>
     </row>
-    <row r="88" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="17" thickBot="1">
       <c r="A88" s="5" t="s">
         <v>33</v>
       </c>
@@ -4213,63 +4254,63 @@
       <c r="J88" s="5"/>
       <c r="L88"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12">
       <c r="A89" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J89" s="5"/>
       <c r="L89"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12">
       <c r="A90" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J90" s="5"/>
       <c r="L90"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12">
       <c r="A91" s="5" t="s">
         <v>37</v>
       </c>
       <c r="J91" s="5"/>
       <c r="L91"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12">
       <c r="A92" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J92" s="5"/>
       <c r="L92"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12">
       <c r="A93" s="5" t="s">
         <v>25</v>
       </c>
       <c r="J93" s="5"/>
       <c r="L93"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12">
       <c r="A94" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J94" s="5"/>
       <c r="L94"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12">
       <c r="A95" s="5" t="s">
         <v>24</v>
       </c>
       <c r="J95" s="5"/>
       <c r="L95"/>
     </row>
-    <row r="96" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="17" thickBot="1">
       <c r="A96" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J96" s="5"/>
       <c r="L96"/>
     </row>
-    <row r="97" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="17" thickBot="1">
       <c r="A97" s="5" t="s">
         <v>34</v>
       </c>
@@ -4279,7 +4320,7 @@
       <c r="J97" s="5"/>
       <c r="L97"/>
     </row>
-    <row r="98" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="17" thickBot="1">
       <c r="A98" s="5" t="s">
         <v>36</v>
       </c>
@@ -4291,14 +4332,14 @@
       <c r="J98" s="5"/>
       <c r="L98"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13">
       <c r="A99" s="6" t="s">
         <v>39</v>
       </c>
       <c r="J99" s="5"/>
       <c r="L99"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13">
       <c r="A100" s="5" t="s">
         <v>42</v>
       </c>
@@ -4306,7 +4347,7 @@
       <c r="K100" s="31"/>
       <c r="L100" s="31"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13">
       <c r="A101" s="5" t="s">
         <v>41</v>
       </c>
@@ -4314,28 +4355,28 @@
       <c r="L101"/>
       <c r="M101" s="31"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13">
       <c r="A102" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J102" s="5"/>
       <c r="L102"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13">
       <c r="A103" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J103" s="5"/>
       <c r="L103"/>
     </row>
-    <row r="104" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" ht="17" thickBot="1">
       <c r="A104" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J104" s="5"/>
       <c r="L104"/>
     </row>
-    <row r="105" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" ht="17" thickBot="1">
       <c r="A105" s="5" t="s">
         <v>43</v>
       </c>
@@ -4344,21 +4385,21 @@
       <c r="J105" s="5"/>
       <c r="L105"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13">
       <c r="A106" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J106" s="5"/>
       <c r="L106"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13">
       <c r="A107" s="5" t="s">
         <v>12</v>
       </c>
       <c r="J107" s="5"/>
       <c r="L107"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13">
       <c r="A108" s="5" t="s">
         <v>15</v>
       </c>
@@ -4366,7 +4407,7 @@
       <c r="K108" s="28"/>
       <c r="M108" s="28"/>
     </row>
-    <row r="109" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" ht="17" thickBot="1">
       <c r="A109" s="5" t="s">
         <v>13</v>
       </c>
@@ -4374,7 +4415,7 @@
       <c r="K109" s="28"/>
       <c r="M109" s="28"/>
     </row>
-    <row r="110" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="17" thickBot="1">
       <c r="A110" s="5" t="s">
         <v>44</v>
       </c>
@@ -4384,7 +4425,7 @@
       <c r="K110" s="28"/>
       <c r="M110" s="28"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13">
       <c r="A111" s="5" t="s">
         <v>16</v>
       </c>
@@ -4396,331 +4437,331 @@
       <c r="K111" s="28"/>
       <c r="M111" s="28"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13">
       <c r="A112" s="5"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" s="5"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" s="5"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115" s="5"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" s="5"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" s="5"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" s="5"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" s="5"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1">
       <c r="A120" s="5"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" s="5"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" s="5"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" s="5"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" s="5"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" s="5"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="5"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132" s="5"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133" s="5"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134" s="5"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135" s="5"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1">
       <c r="A136" s="5"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1">
       <c r="A137" s="5"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138" s="5"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139" s="5"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1">
       <c r="A140" s="5"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1">
       <c r="A141" s="5"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142" s="5"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1">
       <c r="A143" s="5"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1">
       <c r="A144" s="5"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1">
       <c r="A145" s="5"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1">
       <c r="A146" s="5"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1">
       <c r="A147" s="5"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1">
       <c r="A148" s="5"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1">
       <c r="A149" s="5"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1">
       <c r="A150" s="5"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1">
       <c r="A151" s="5"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1">
       <c r="A152" s="5"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1">
       <c r="A153" s="5"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1">
       <c r="A154" s="5"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1">
       <c r="A155" s="5"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1">
       <c r="A156" s="5"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1">
       <c r="A157" s="5"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1">
       <c r="A158" s="5"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1">
       <c r="A159" s="5"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1">
       <c r="A160" s="5"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1">
       <c r="A161" s="5"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1">
       <c r="A162" s="5"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1">
       <c r="A163" s="5"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1">
       <c r="A164" s="5"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1">
       <c r="A165" s="5"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1">
       <c r="A166" s="5"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1">
       <c r="A167" s="5"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1">
       <c r="A168" s="5"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1">
       <c r="A169" s="5"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1">
       <c r="A170" s="5"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1">
       <c r="A171" s="5"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1">
       <c r="A172" s="5"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1">
       <c r="A173" s="5"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1">
       <c r="A174" s="5"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1">
       <c r="A175" s="5"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1">
       <c r="A176" s="5"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1">
       <c r="A177" s="5"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1">
       <c r="A178" s="5"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1">
       <c r="A179" s="5"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1">
       <c r="A180" s="5"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1">
       <c r="A181" s="5"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1">
       <c r="A182" s="5"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1">
       <c r="A183" s="5"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1">
       <c r="A184" s="5"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1">
       <c r="A185" s="5"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1">
       <c r="A186" s="5"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1">
       <c r="A187" s="5"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1">
       <c r="A188" s="5"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1">
       <c r="A189" s="5"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1">
       <c r="A190" s="5"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1">
       <c r="A191" s="5"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1">
       <c r="A192" s="5"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1">
       <c r="A193" s="5"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1">
       <c r="A194" s="5"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1">
       <c r="A195" s="5"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1">
       <c r="A196" s="5"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1">
       <c r="A197" s="5"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1">
       <c r="A198" s="5"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1">
       <c r="A199" s="5"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1">
       <c r="A200" s="5"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1">
       <c r="A201" s="5"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1">
       <c r="A202" s="5"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1">
       <c r="A203" s="5"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1">
       <c r="A204" s="5"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1">
       <c r="A205" s="5"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1">
       <c r="A206" s="5"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1">
       <c r="A207" s="5"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1">
       <c r="A208" s="5"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1">
       <c r="A209" s="5"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1">
       <c r="A210" s="5"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1">
       <c r="A211" s="5"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1">
       <c r="A212" s="5"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1">
       <c r="A213" s="5"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1">
       <c r="A214" s="5"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1">
       <c r="A215" s="5"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1">
       <c r="A216" s="5"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1">
       <c r="A217" s="5"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1">
       <c r="A218" s="5"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1">
       <c r="A219" s="5"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1">
       <c r="A220" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Ethics Checklists to workplan deadlines
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C315B1-2624-5646-B753-4446A1673C73}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB32682-3D56-CE4D-B45F-C0B7FFD6C124}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="2820" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
@@ -221,8 +221,9 @@
     <t>Create Demo for Presentation</t>
   </si>
   <si>
-    <t>23rd October
-Revised Project Proposal - 0%</t>
+    <t>22nd October
+Project Proposal - 0%
+Preliminary Ethics Check</t>
   </si>
 </sst>
 </file>
@@ -857,7 +858,7 @@
   <dimension ref="A1:AL63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="AM4" sqref="AM4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -869,7 +870,7 @@
     <col min="36" max="36" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="119">
+    <row r="1" spans="1:35" s="1" customFormat="1" ht="131">
       <c r="A1" s="44" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added codes to each part of the workplan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB32682-3D56-CE4D-B45F-C0B7FFD6C124}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DD92B0-5C8B-FC42-A4DB-A50699FFF4CF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="2820" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="78">
   <si>
     <t>Week</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>Research Paper</t>
-  </si>
-  <si>
-    <t>Basic Reasearch into competition - Not sure what to call this</t>
   </si>
   <si>
     <t>7th December
@@ -224,6 +221,63 @@
     <t>22nd October
 Project Proposal - 0%
 Preliminary Ethics Check</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Research for Proposal</t>
   </si>
 </sst>
 </file>
@@ -317,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -479,11 +533,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -559,16 +633,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,55 +960,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AL63"/>
+  <dimension ref="A1:AM63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="28" customWidth="1"/>
-    <col min="13" max="35" width="9.1640625" customWidth="1"/>
-    <col min="36" max="36" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="9.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="28" customWidth="1"/>
+    <col min="14" max="36" width="9.1640625" customWidth="1"/>
+    <col min="37" max="37" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="131">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="131">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="C1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="48" t="s">
+        <v>58</v>
+      </c>
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
       <c r="J1" s="40"/>
       <c r="K1" s="40"/>
-      <c r="L1" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="48" t="s">
+        <v>52</v>
+      </c>
       <c r="N1" s="40"/>
       <c r="O1" s="40"/>
       <c r="P1" s="40"/>
       <c r="Q1" s="40"/>
       <c r="R1" s="40"/>
       <c r="S1" s="40"/>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="40"/>
+      <c r="U1" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="40"/>
       <c r="V1" s="40"/>
       <c r="W1" s="40"/>
       <c r="X1" s="40"/>
@@ -912,208 +1017,224 @@
       <c r="AA1" s="40"/>
       <c r="AB1" s="40"/>
       <c r="AC1" s="40"/>
-      <c r="AD1" s="48" t="s">
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="17" thickBot="1">
-      <c r="A2" s="46" t="s">
+    </row>
+    <row r="2" spans="1:36" ht="17" thickBot="1">
+      <c r="A2" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47">
+      <c r="C2" s="47">
         <v>43367</v>
       </c>
-      <c r="C2" s="47">
+      <c r="D2" s="47">
         <v>43374</v>
       </c>
-      <c r="D2" s="47">
+      <c r="E2" s="47">
         <v>43381</v>
       </c>
-      <c r="E2" s="47">
+      <c r="F2" s="47">
         <v>43388</v>
       </c>
-      <c r="F2" s="49">
+      <c r="G2" s="49">
         <v>43395</v>
       </c>
-      <c r="G2" s="47">
+      <c r="H2" s="47">
         <v>43402</v>
       </c>
-      <c r="H2" s="47">
+      <c r="I2" s="47">
         <v>43409</v>
       </c>
-      <c r="I2" s="47">
+      <c r="J2" s="47">
         <v>43416</v>
       </c>
-      <c r="J2" s="47">
+      <c r="K2" s="47">
         <v>43423</v>
       </c>
-      <c r="K2" s="47">
+      <c r="L2" s="47">
         <v>43430</v>
       </c>
-      <c r="L2" s="49">
+      <c r="M2" s="49">
         <v>43437</v>
       </c>
-      <c r="M2" s="47">
+      <c r="N2" s="47">
         <v>43444</v>
       </c>
-      <c r="N2" s="47">
+      <c r="O2" s="47">
         <v>43451</v>
       </c>
-      <c r="O2" s="47">
+      <c r="P2" s="47">
         <v>43458</v>
       </c>
-      <c r="P2" s="47">
+      <c r="Q2" s="47">
         <v>43465</v>
       </c>
-      <c r="Q2" s="47">
+      <c r="R2" s="47">
         <v>43472</v>
       </c>
-      <c r="R2" s="47">
+      <c r="S2" s="47">
         <v>43479</v>
       </c>
-      <c r="S2" s="47">
+      <c r="T2" s="47">
         <v>43486</v>
       </c>
-      <c r="T2" s="47">
+      <c r="U2" s="47">
         <v>43493</v>
       </c>
-      <c r="U2" s="47">
+      <c r="V2" s="47">
         <v>43500</v>
       </c>
-      <c r="V2" s="47">
+      <c r="W2" s="47">
         <v>43507</v>
       </c>
-      <c r="W2" s="47">
+      <c r="X2" s="47">
         <v>43514</v>
       </c>
-      <c r="X2" s="47">
+      <c r="Y2" s="47">
         <v>43521</v>
       </c>
-      <c r="Y2" s="47">
+      <c r="Z2" s="47">
         <v>43528</v>
       </c>
-      <c r="Z2" s="47">
+      <c r="AA2" s="47">
         <v>43535</v>
       </c>
-      <c r="AA2" s="47">
+      <c r="AB2" s="47">
         <v>43542</v>
       </c>
-      <c r="AB2" s="47">
+      <c r="AC2" s="47">
         <v>43549</v>
       </c>
-      <c r="AC2" s="47">
+      <c r="AD2" s="47">
         <v>43556</v>
       </c>
-      <c r="AD2" s="49">
+      <c r="AE2" s="49">
         <v>43563</v>
       </c>
-      <c r="AE2" s="47">
+      <c r="AF2" s="47">
         <v>43570</v>
       </c>
-      <c r="AF2" s="47">
+      <c r="AG2" s="47">
         <v>43577</v>
       </c>
-      <c r="AG2" s="47">
+      <c r="AH2" s="47">
         <v>43584</v>
       </c>
-      <c r="AH2" s="47">
+      <c r="AI2" s="47">
         <v>43591</v>
       </c>
-      <c r="AI2" s="47">
+      <c r="AJ2" s="47">
         <v>43598</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="17" thickTop="1">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:36" ht="17" thickTop="1">
+      <c r="A3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="AD3" s="50"/>
-      <c r="AF3" s="28"/>
-    </row>
-    <row r="4" spans="1:35">
-      <c r="A4" s="45" t="s">
+      <c r="B3" s="59"/>
+      <c r="G3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="AE3" s="50"/>
+      <c r="AG3" s="28"/>
+    </row>
+    <row r="4" spans="1:36">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="7"/>
-      <c r="F4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="AD4" s="50"/>
-      <c r="AF4" s="28"/>
-    </row>
-    <row r="5" spans="1:35">
-      <c r="A5" s="45" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="7"/>
+      <c r="G4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="AE4" s="50"/>
+      <c r="AG4" s="28"/>
+    </row>
+    <row r="5" spans="1:36">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="51"/>
-      <c r="L5" s="50"/>
-      <c r="AD5" s="50"/>
-      <c r="AF5" s="28"/>
-    </row>
-    <row r="6" spans="1:35">
-      <c r="A6" s="45"/>
-      <c r="C6" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="51"/>
+      <c r="M5" s="50"/>
+      <c r="AE5" s="50"/>
+      <c r="AG5" s="28"/>
+    </row>
+    <row r="6" spans="1:36">
+      <c r="B6" s="45"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="52"/>
-      <c r="L6" s="50"/>
-      <c r="AD6" s="50"/>
-      <c r="AF6" s="28"/>
-    </row>
-    <row r="7" spans="1:35">
-      <c r="A7" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="50"/>
-      <c r="H7" s="43"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="52"/>
+      <c r="M6" s="50"/>
+      <c r="AE6" s="50"/>
+      <c r="AG6" s="28"/>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="50"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="51"/>
-      <c r="AD7" s="50"/>
-      <c r="AF7" s="28"/>
-    </row>
-    <row r="8" spans="1:35">
-      <c r="A8" s="45"/>
-      <c r="F8" s="50"/>
-      <c r="H8" s="24"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="51"/>
+      <c r="AE7" s="50"/>
+      <c r="AG7" s="28"/>
+    </row>
+    <row r="8" spans="1:36">
+      <c r="B8" s="45"/>
+      <c r="G8" s="50"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="52"/>
-      <c r="AD8" s="50"/>
-      <c r="AF8" s="28"/>
-    </row>
-    <row r="9" spans="1:35">
-      <c r="A9" s="45"/>
-      <c r="F9" s="50"/>
-      <c r="H9" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="52"/>
+      <c r="AE8" s="50"/>
+      <c r="AG8" s="28"/>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="B9" s="45"/>
+      <c r="G9" s="50"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="52"/>
-      <c r="AD9" s="50"/>
-      <c r="AF9" s="28"/>
-    </row>
-    <row r="10" spans="1:35">
-      <c r="A10" s="45" t="s">
+      <c r="K9" s="24"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="52"/>
+      <c r="AE9" s="50"/>
+      <c r="AG9" s="28"/>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="50"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="9"/>
+      <c r="G10" s="50"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="52"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
@@ -1126,203 +1247,241 @@
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
       <c r="Y10" s="9"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="9"/>
-      <c r="AD10" s="50"/>
-      <c r="AF10" s="28"/>
-    </row>
-    <row r="11" spans="1:35">
-      <c r="A11" s="45" t="s">
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="9"/>
+      <c r="AE10" s="50"/>
+      <c r="AG10" s="28"/>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="AA11" s="7"/>
+      <c r="G11" s="50"/>
+      <c r="M11" s="50"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
-      <c r="AD11" s="51"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="28"/>
-    </row>
-    <row r="12" spans="1:35">
-      <c r="A12" s="54" t="s">
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="51"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="28"/>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="A12" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="AD12" s="50"/>
-      <c r="AF12" s="28"/>
-    </row>
-    <row r="13" spans="1:35">
-      <c r="A13" s="61" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="11"/>
+      <c r="B12" s="60"/>
+      <c r="G12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="AE12" s="50"/>
+      <c r="AG12" s="28"/>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>77</v>
+      </c>
       <c r="D13" s="11"/>
-      <c r="F13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="AD13" s="50"/>
-      <c r="AF13" s="28"/>
-    </row>
-    <row r="14" spans="1:35">
-      <c r="A14" s="60"/>
-      <c r="F14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="AD14" s="50"/>
-      <c r="AF14" s="28"/>
-    </row>
-    <row r="15" spans="1:35">
-      <c r="A15" s="55" t="s">
+      <c r="E13" s="11"/>
+      <c r="G13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="AE13" s="50"/>
+      <c r="AG13" s="28"/>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="B14" s="54"/>
+      <c r="G14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="AE14" s="50"/>
+      <c r="AG14" s="28"/>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="A15" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="AD15" s="50"/>
-      <c r="AF15" s="28"/>
-    </row>
-    <row r="16" spans="1:35">
-      <c r="A16" s="60"/>
-      <c r="F16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="AD16" s="50"/>
-      <c r="AF16" s="28"/>
-    </row>
-    <row r="17" spans="1:38">
-      <c r="A17" s="60"/>
-      <c r="F17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="AD17" s="50"/>
-      <c r="AF17" s="28"/>
-    </row>
-    <row r="18" spans="1:38">
-      <c r="A18" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="T18" s="9"/>
+      <c r="B15" s="62"/>
+      <c r="G15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="AE15" s="50"/>
+      <c r="AG15" s="28"/>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="54"/>
+      <c r="G16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="AE16" s="50"/>
+      <c r="AG16" s="28"/>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="B17" s="54"/>
+      <c r="G17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="AE17" s="50"/>
+      <c r="AG17" s="28"/>
+    </row>
+    <row r="18" spans="1:39">
+      <c r="A18" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="64"/>
+      <c r="G18" s="50"/>
+      <c r="M18" s="50"/>
       <c r="U18" s="9"/>
-      <c r="AD18" s="50"/>
-      <c r="AF18" s="28"/>
-    </row>
-    <row r="19" spans="1:38">
-      <c r="A19" s="45" t="s">
+      <c r="V18" s="9"/>
+      <c r="AE18" s="50"/>
+      <c r="AG18" s="28"/>
+    </row>
+    <row r="19" spans="1:39">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="AD19" s="50"/>
-      <c r="AF19" s="28"/>
-      <c r="AG19" s="59"/>
-      <c r="AH19" s="59"/>
-    </row>
-    <row r="20" spans="1:38">
-      <c r="A20" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="AD20" s="50"/>
-      <c r="AF20" s="28"/>
-      <c r="AG20" s="59"/>
-      <c r="AH20" s="59"/>
-    </row>
-    <row r="21" spans="1:38">
-      <c r="A21" s="45" t="s">
+      <c r="G19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="AE19" s="50"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="53"/>
+      <c r="AI19" s="53"/>
+    </row>
+    <row r="20" spans="1:39">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="AE20" s="50"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="53"/>
+      <c r="AI20" s="53"/>
+    </row>
+    <row r="21" spans="1:39">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="AD21" s="50"/>
-      <c r="AF21" s="28"/>
-      <c r="AI21" s="59"/>
-    </row>
-    <row r="22" spans="1:38">
-      <c r="A22" s="56" t="s">
+      <c r="G21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="AE21" s="50"/>
+      <c r="AG21" s="28"/>
+      <c r="AJ21" s="53"/>
+    </row>
+    <row r="22" spans="1:39">
+      <c r="A22" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="AD22" s="50"/>
-      <c r="AF22" s="28"/>
-    </row>
-    <row r="23" spans="1:38">
-      <c r="A23" s="61" t="s">
+      <c r="B22" s="66"/>
+      <c r="G22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="AE22" s="50"/>
+      <c r="AG22" s="28"/>
+    </row>
+    <row r="23" spans="1:39">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="F23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="AD23" s="50"/>
-      <c r="AF23" s="28"/>
-    </row>
-    <row r="24" spans="1:38">
-      <c r="A24" s="61" t="s">
+      <c r="D23" s="12"/>
+      <c r="G23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="AE23" s="50"/>
+      <c r="AG23" s="28"/>
+    </row>
+    <row r="24" spans="1:39">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="F24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="AD24" s="50"/>
-      <c r="AF24" s="28"/>
-    </row>
-    <row r="25" spans="1:38">
-      <c r="A25" s="45" t="s">
+      <c r="D24" s="12"/>
+      <c r="G24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="AE24" s="50"/>
+      <c r="AG24" s="28"/>
+    </row>
+    <row r="25" spans="1:39">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="L25" s="50"/>
-      <c r="P25" s="9"/>
+      <c r="G25" s="50"/>
+      <c r="M25" s="50"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
-      <c r="AB25" s="24"/>
+      <c r="T25" s="9"/>
       <c r="AC25" s="24"/>
-      <c r="AD25" s="50"/>
-      <c r="AF25" s="28"/>
-      <c r="AI25" s="12"/>
-    </row>
-    <row r="26" spans="1:38">
-      <c r="A26" s="57" t="s">
+      <c r="AD25" s="24"/>
+      <c r="AE25" s="50"/>
+      <c r="AG25" s="28"/>
+      <c r="AJ25" s="12"/>
+    </row>
+    <row r="26" spans="1:39">
+      <c r="A26" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="AD26" s="50"/>
-      <c r="AF26" s="28"/>
-    </row>
-    <row r="27" spans="1:38">
-      <c r="A27" s="45" t="s">
+      <c r="B26" s="68"/>
+      <c r="G26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="AE26" s="50"/>
+      <c r="AG26" s="28"/>
+    </row>
+    <row r="27" spans="1:39">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="F27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="AD27" s="50"/>
-      <c r="AF27" s="28"/>
-    </row>
-    <row r="28" spans="1:38" s="28" customFormat="1">
-      <c r="A28" s="45" t="s">
+      <c r="D27" s="8"/>
+      <c r="G27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="AE27" s="50"/>
+      <c r="AG27" s="28"/>
+    </row>
+    <row r="28" spans="1:39" s="28" customFormat="1">
+      <c r="A28" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28"/>
+      <c r="C28" s="9"/>
       <c r="D28"/>
       <c r="E28"/>
-      <c r="F28" s="50"/>
-      <c r="G28"/>
+      <c r="F28"/>
+      <c r="G28" s="50"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
-      <c r="L28" s="50"/>
-      <c r="M28"/>
-      <c r="N28" s="8"/>
+      <c r="L28"/>
+      <c r="M28" s="50"/>
+      <c r="N28"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
-      <c r="R28"/>
+      <c r="R28" s="8"/>
       <c r="S28"/>
       <c r="T28"/>
       <c r="U28"/>
@@ -1334,33 +1493,36 @@
       <c r="AA28"/>
       <c r="AB28"/>
       <c r="AC28"/>
-      <c r="AD28" s="50"/>
-      <c r="AE28"/>
-      <c r="AL28" s="39"/>
-    </row>
-    <row r="29" spans="1:38" s="28" customFormat="1">
-      <c r="A29" s="45" t="s">
+      <c r="AD28"/>
+      <c r="AE28" s="50"/>
+      <c r="AF28"/>
+      <c r="AM28" s="39"/>
+    </row>
+    <row r="29" spans="1:39" s="28" customFormat="1">
+      <c r="A29" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
-      <c r="F29" s="50"/>
-      <c r="G29"/>
+      <c r="F29"/>
+      <c r="G29" s="50"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
-      <c r="L29" s="50"/>
-      <c r="M29"/>
+      <c r="L29"/>
+      <c r="M29" s="50"/>
       <c r="N29"/>
       <c r="O29"/>
       <c r="P29"/>
       <c r="Q29"/>
-      <c r="R29" s="8"/>
+      <c r="R29"/>
       <c r="S29" s="8"/>
-      <c r="T29"/>
+      <c r="T29" s="8"/>
       <c r="U29"/>
       <c r="V29"/>
       <c r="W29"/>
@@ -1370,25 +1532,28 @@
       <c r="AA29"/>
       <c r="AB29"/>
       <c r="AC29"/>
-      <c r="AD29" s="50"/>
-      <c r="AE29"/>
-    </row>
-    <row r="30" spans="1:38" s="28" customFormat="1">
-      <c r="A30" s="45" t="s">
+      <c r="AD29"/>
+      <c r="AE29" s="50"/>
+      <c r="AF29"/>
+    </row>
+    <row r="30" spans="1:39" s="28" customFormat="1">
+      <c r="A30" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
-      <c r="F30" s="50"/>
-      <c r="G30"/>
+      <c r="F30"/>
+      <c r="G30" s="50"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
-      <c r="L30" s="50"/>
-      <c r="M30"/>
+      <c r="L30"/>
+      <c r="M30" s="50"/>
       <c r="N30"/>
       <c r="O30"/>
       <c r="P30"/>
@@ -1403,16 +1568,17 @@
       <c r="Y30"/>
       <c r="Z30"/>
       <c r="AA30"/>
-      <c r="AB30" s="9"/>
+      <c r="AB30"/>
       <c r="AC30" s="9"/>
-      <c r="AD30" s="52"/>
-      <c r="AE30" s="8"/>
-      <c r="AF30" s="62"/>
-      <c r="AG30" s="62"/>
-      <c r="AH30" s="62"/>
-    </row>
-    <row r="31" spans="1:38" s="28" customFormat="1"/>
-    <row r="32" spans="1:38" s="28" customFormat="1"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="52"/>
+      <c r="AF30" s="8"/>
+      <c r="AG30" s="56"/>
+      <c r="AH30" s="56"/>
+      <c r="AI30" s="56"/>
+    </row>
+    <row r="31" spans="1:39" s="28" customFormat="1"/>
+    <row r="32" spans="1:39" s="28" customFormat="1"/>
     <row r="33" s="28" customFormat="1"/>
     <row r="34" s="28" customFormat="1"/>
     <row r="35" s="28" customFormat="1"/>
@@ -1429,28 +1595,36 @@
     <row r="46" s="28" customFormat="1"/>
     <row r="47" s="28" customFormat="1"/>
     <row r="48" s="28" customFormat="1"/>
-    <row r="49" spans="1:1" s="28" customFormat="1"/>
-    <row r="50" spans="1:1" s="28" customFormat="1"/>
-    <row r="51" spans="1:1" s="28" customFormat="1"/>
-    <row r="52" spans="1:1" s="28" customFormat="1"/>
-    <row r="53" spans="1:1" s="28" customFormat="1"/>
-    <row r="54" spans="1:1" s="28" customFormat="1"/>
-    <row r="55" spans="1:1" s="28" customFormat="1"/>
-    <row r="56" spans="1:1" s="28" customFormat="1"/>
-    <row r="57" spans="1:1" s="28" customFormat="1"/>
-    <row r="58" spans="1:1" s="28" customFormat="1"/>
-    <row r="59" spans="1:1" s="28" customFormat="1"/>
-    <row r="60" spans="1:1" s="28" customFormat="1"/>
-    <row r="61" spans="1:1">
-      <c r="A61" s="28"/>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="28"/>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="28"/>
+    <row r="49" spans="2:2" s="28" customFormat="1"/>
+    <row r="50" spans="2:2" s="28" customFormat="1"/>
+    <row r="51" spans="2:2" s="28" customFormat="1"/>
+    <row r="52" spans="2:2" s="28" customFormat="1"/>
+    <row r="53" spans="2:2" s="28" customFormat="1"/>
+    <row r="54" spans="2:2" s="28" customFormat="1"/>
+    <row r="55" spans="2:2" s="28" customFormat="1"/>
+    <row r="56" spans="2:2" s="28" customFormat="1"/>
+    <row r="57" spans="2:2" s="28" customFormat="1"/>
+    <row r="58" spans="2:2" s="28" customFormat="1"/>
+    <row r="59" spans="2:2" s="28" customFormat="1"/>
+    <row r="60" spans="2:2" s="28" customFormat="1"/>
+    <row r="61" spans="2:2">
+      <c r="B61" s="28"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="28"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="28"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A26:B26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated some headings etc
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DD92B0-5C8B-FC42-A4DB-A50699FFF4CF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BC48BD-F34D-BD43-8EB3-6BBA02F373DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="2820" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="16580" windowHeight="31540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="81">
   <si>
     <t>Week</t>
   </si>
@@ -177,9 +177,6 @@
   <si>
     <t>12th October
 Project Proposal - Soft</t>
-  </si>
-  <si>
-    <t>SET/SEM Questionaires</t>
   </si>
   <si>
     <t>Create Git repository</t>
@@ -278,6 +275,18 @@
   </si>
   <si>
     <t>Research for Proposal</t>
+  </si>
+  <si>
+    <t>SET/SEM Questionaries</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>Present Presentation</t>
   </si>
 </sst>
 </file>
@@ -960,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM63"/>
+  <dimension ref="A1:AM64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -981,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40" t="s">
@@ -989,7 +998,7 @@
       </c>
       <c r="F1" s="40"/>
       <c r="G1" s="48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
@@ -997,7 +1006,7 @@
       <c r="K1" s="40"/>
       <c r="L1" s="40"/>
       <c r="M1" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N1" s="40"/>
       <c r="O1" s="40"/>
@@ -1007,7 +1016,7 @@
       <c r="S1" s="40"/>
       <c r="T1" s="40"/>
       <c r="U1" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V1" s="40"/>
       <c r="W1" s="40"/>
@@ -1019,18 +1028,18 @@
       <c r="AC1" s="40"/>
       <c r="AD1" s="40"/>
       <c r="AE1" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AF1" s="40"/>
       <c r="AH1" s="40"/>
       <c r="AI1" s="40"/>
       <c r="AJ1" s="40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="17" thickBot="1">
       <c r="A2" s="57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>0</v>
@@ -1150,7 +1159,7 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>14</v>
@@ -1164,7 +1173,7 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="45" t="s">
         <v>21</v>
@@ -1189,10 +1198,10 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="50"/>
       <c r="I7" s="43"/>
@@ -1227,7 +1236,7 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="45" t="s">
         <v>35</v>
@@ -1255,10 +1264,10 @@
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="50"/>
       <c r="M11" s="50"/>
@@ -1281,10 +1290,10 @@
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -1312,7 +1321,7 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="54"/>
       <c r="G16" s="50"/>
@@ -1329,7 +1338,7 @@
     </row>
     <row r="18" spans="1:39">
       <c r="A18" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="64"/>
       <c r="G18" s="50"/>
@@ -1341,7 +1350,7 @@
     </row>
     <row r="19" spans="1:39">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="45" t="s">
         <v>42</v>
@@ -1355,10 +1364,10 @@
     </row>
     <row r="20" spans="1:39">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="50"/>
       <c r="M20" s="50"/>
@@ -1369,7 +1378,7 @@
     </row>
     <row r="21" spans="1:39">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>41</v>
@@ -1381,23 +1390,23 @@
       <c r="AJ21" s="53"/>
     </row>
     <row r="22" spans="1:39">
-      <c r="A22" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="66"/>
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>80</v>
+      </c>
       <c r="G22" s="50"/>
       <c r="M22" s="50"/>
       <c r="AE22" s="50"/>
       <c r="AG22" s="28"/>
+      <c r="AJ22" s="53"/>
     </row>
     <row r="23" spans="1:39">
-      <c r="A23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="12"/>
+      <c r="A23" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="66"/>
       <c r="G23" s="50"/>
       <c r="M23" s="50"/>
       <c r="AE23" s="50"/>
@@ -1405,10 +1414,10 @@
     </row>
     <row r="24" spans="1:39">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="12"/>
       <c r="G24" s="50"/>
@@ -1418,94 +1427,68 @@
     </row>
     <row r="25" spans="1:39">
       <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>46</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="12"/>
       <c r="G25" s="50"/>
       <c r="M25" s="50"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="AC25" s="24"/>
-      <c r="AD25" s="24"/>
       <c r="AE25" s="50"/>
       <c r="AG25" s="28"/>
-      <c r="AJ25" s="12"/>
     </row>
     <row r="26" spans="1:39">
-      <c r="A26" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="68"/>
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>77</v>
+      </c>
       <c r="G26" s="50"/>
       <c r="M26" s="50"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="AC26" s="24"/>
+      <c r="AD26" s="24"/>
       <c r="AE26" s="50"/>
       <c r="AG26" s="28"/>
+      <c r="AJ26" s="12"/>
     </row>
     <row r="27" spans="1:39">
-      <c r="A27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
+      <c r="A27" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="68"/>
       <c r="G27" s="50"/>
       <c r="M27" s="50"/>
       <c r="AE27" s="50"/>
       <c r="AG27" s="28"/>
     </row>
-    <row r="28" spans="1:39" s="28" customFormat="1">
-      <c r="A28" s="28" t="s">
-        <v>74</v>
+    <row r="28" spans="1:39">
+      <c r="A28" t="s">
+        <v>72</v>
       </c>
       <c r="B28" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="G28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="AE28" s="50"/>
+      <c r="AG28" s="28"/>
+    </row>
+    <row r="29" spans="1:39" s="28" customFormat="1">
+      <c r="A29" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28" s="50"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28" s="50"/>
-      <c r="N28"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28"/>
-      <c r="T28"/>
-      <c r="U28"/>
-      <c r="V28"/>
-      <c r="W28"/>
-      <c r="X28"/>
-      <c r="Y28"/>
-      <c r="Z28"/>
-      <c r="AA28"/>
-      <c r="AB28"/>
-      <c r="AC28"/>
-      <c r="AD28"/>
-      <c r="AE28" s="50"/>
-      <c r="AF28"/>
-      <c r="AM28" s="39"/>
-    </row>
-    <row r="29" spans="1:39" s="28" customFormat="1">
-      <c r="A29" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29"/>
+      <c r="C29" s="9"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
@@ -1517,12 +1500,12 @@
       <c r="L29"/>
       <c r="M29" s="50"/>
       <c r="N29"/>
-      <c r="O29"/>
-      <c r="P29"/>
-      <c r="Q29"/>
-      <c r="R29"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29"/>
+      <c r="T29"/>
       <c r="U29"/>
       <c r="V29"/>
       <c r="W29"/>
@@ -1535,13 +1518,14 @@
       <c r="AD29"/>
       <c r="AE29" s="50"/>
       <c r="AF29"/>
+      <c r="AM29" s="39"/>
     </row>
     <row r="30" spans="1:39" s="28" customFormat="1">
       <c r="A30" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -1559,8 +1543,8 @@
       <c r="P30"/>
       <c r="Q30"/>
       <c r="R30"/>
-      <c r="S30"/>
-      <c r="T30"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
       <c r="U30"/>
       <c r="V30"/>
       <c r="W30"/>
@@ -1569,15 +1553,52 @@
       <c r="Z30"/>
       <c r="AA30"/>
       <c r="AB30"/>
-      <c r="AC30" s="9"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="52"/>
-      <c r="AF30" s="8"/>
-      <c r="AG30" s="56"/>
-      <c r="AH30" s="56"/>
-      <c r="AI30" s="56"/>
-    </row>
-    <row r="31" spans="1:39" s="28" customFormat="1"/>
+      <c r="AC30"/>
+      <c r="AD30"/>
+      <c r="AE30" s="50"/>
+      <c r="AF30"/>
+    </row>
+    <row r="31" spans="1:39" s="28" customFormat="1">
+      <c r="A31" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31" s="50"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31" s="50"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
+      <c r="AB31"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="52"/>
+      <c r="AF31" s="8"/>
+      <c r="AG31" s="56"/>
+      <c r="AH31" s="56"/>
+      <c r="AI31" s="56"/>
+    </row>
     <row r="32" spans="1:39" s="28" customFormat="1"/>
     <row r="33" s="28" customFormat="1"/>
     <row r="34" s="28" customFormat="1"/>
@@ -1607,14 +1628,15 @@
     <row r="58" spans="2:2" s="28" customFormat="1"/>
     <row r="59" spans="2:2" s="28" customFormat="1"/>
     <row r="60" spans="2:2" s="28" customFormat="1"/>
-    <row r="61" spans="2:2">
-      <c r="B61" s="28"/>
-    </row>
+    <row r="61" spans="2:2" s="28" customFormat="1"/>
     <row r="62" spans="2:2">
       <c r="B62" s="28"/>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="28"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1622,8 +1644,8 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
improved descriptions of work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BC48BD-F34D-BD43-8EB3-6BBA02F373DF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3264285-DB20-C947-A0F6-A7833CF6134A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="16580" windowHeight="31540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34620" yWindow="460" windowWidth="16580" windowHeight="31540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="82">
   <si>
     <t>Week</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>Presentation</t>
-  </si>
-  <si>
-    <t>Interrim Report - Break this down?</t>
   </si>
   <si>
     <t>Create Demo for Presentation</t>
@@ -232,12 +229,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -287,6 +278,18 @@
   </si>
   <si>
     <t>Present Presentation</t>
+  </si>
+  <si>
+    <t>Welcome Weeks</t>
+  </si>
+  <si>
+    <t>Project Proposal Draft</t>
+  </si>
+  <si>
+    <t>Preliminary Ethics Checklist</t>
+  </si>
+  <si>
+    <t>Break these sections down furhter</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -653,36 +656,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,13 +976,13 @@
   <dimension ref="A1:AM64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="9.1640625" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" style="28" customWidth="1"/>
     <col min="14" max="36" width="9.1640625" customWidth="1"/>
@@ -998,7 +1002,7 @@
       </c>
       <c r="F1" s="40"/>
       <c r="G1" s="48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
@@ -1039,7 +1043,7 @@
     </row>
     <row r="2" spans="1:36" ht="17" thickBot="1">
       <c r="A2" s="57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>0</v>
@@ -1159,10 +1163,10 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
@@ -1173,10 +1177,10 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1187,33 +1191,34 @@
       <c r="AG5" s="28"/>
     </row>
     <row r="6" spans="1:36">
-      <c r="B6" s="45"/>
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>80</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="52"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="51"/>
       <c r="M6" s="50"/>
       <c r="AE6" s="50"/>
       <c r="AG6" s="28"/>
     </row>
     <row r="7" spans="1:36">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="50"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="51"/>
+      <c r="B7" s="45"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="52"/>
+      <c r="M7" s="50"/>
       <c r="AE7" s="50"/>
       <c r="AG7" s="28"/>
     </row>
     <row r="8" spans="1:36">
-      <c r="B8" s="45"/>
+      <c r="B8" s="70" t="s">
+        <v>81</v>
+      </c>
       <c r="G8" s="50"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
@@ -1224,20 +1229,19 @@
       <c r="AG8" s="28"/>
     </row>
     <row r="9" spans="1:36">
-      <c r="B9" s="45"/>
+      <c r="B9" s="45" t="s">
+        <v>18</v>
+      </c>
       <c r="G9" s="50"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="52"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="51"/>
       <c r="AE9" s="50"/>
       <c r="AG9" s="28"/>
     </row>
     <row r="10" spans="1:36">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
       <c r="B10" s="45" t="s">
         <v>35</v>
       </c>
@@ -1263,9 +1267,6 @@
       <c r="AG10" s="28"/>
     </row>
     <row r="11" spans="1:36">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
       <c r="B11" s="45" t="s">
         <v>50</v>
       </c>
@@ -1279,10 +1280,10 @@
       <c r="AG11" s="28"/>
     </row>
     <row r="12" spans="1:36">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="60"/>
+      <c r="B12" s="61"/>
       <c r="G12" s="50"/>
       <c r="M12" s="50"/>
       <c r="AE12" s="50"/>
@@ -1290,10 +1291,10 @@
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -1310,10 +1311,10 @@
       <c r="AG14" s="28"/>
     </row>
     <row r="15" spans="1:36">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="62"/>
+      <c r="B15" s="63"/>
       <c r="G15" s="50"/>
       <c r="M15" s="50"/>
       <c r="AE15" s="50"/>
@@ -1321,7 +1322,7 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B16" s="54"/>
       <c r="G16" s="50"/>
@@ -1337,10 +1338,10 @@
       <c r="AG17" s="28"/>
     </row>
     <row r="18" spans="1:39">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="65"/>
       <c r="G18" s="50"/>
       <c r="M18" s="50"/>
       <c r="U18" s="9"/>
@@ -1350,7 +1351,7 @@
     </row>
     <row r="19" spans="1:39">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B19" s="45" t="s">
         <v>42</v>
@@ -1364,10 +1365,10 @@
     </row>
     <row r="20" spans="1:39">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G20" s="50"/>
       <c r="M20" s="50"/>
@@ -1378,7 +1379,7 @@
     </row>
     <row r="21" spans="1:39">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>41</v>
@@ -1391,10 +1392,10 @@
     </row>
     <row r="22" spans="1:39">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G22" s="50"/>
       <c r="M22" s="50"/>
@@ -1403,10 +1404,10 @@
       <c r="AJ22" s="53"/>
     </row>
     <row r="23" spans="1:39">
-      <c r="A23" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="66"/>
+      <c r="A23" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="67"/>
       <c r="G23" s="50"/>
       <c r="M23" s="50"/>
       <c r="AE23" s="50"/>
@@ -1414,7 +1415,7 @@
     </row>
     <row r="24" spans="1:39">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B24" s="55" t="s">
         <v>46</v>
@@ -1427,7 +1428,7 @@
     </row>
     <row r="25" spans="1:39">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" s="55" t="s">
         <v>47</v>
@@ -1440,10 +1441,10 @@
     </row>
     <row r="26" spans="1:39">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G26" s="50"/>
       <c r="M26" s="50"/>
@@ -1458,10 +1459,10 @@
       <c r="AJ26" s="12"/>
     </row>
     <row r="27" spans="1:39">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="68"/>
+      <c r="B27" s="69"/>
       <c r="G27" s="50"/>
       <c r="M27" s="50"/>
       <c r="AE27" s="50"/>
@@ -1469,10 +1470,10 @@
     </row>
     <row r="28" spans="1:39">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -1483,7 +1484,7 @@
     </row>
     <row r="29" spans="1:39" s="28" customFormat="1">
       <c r="A29" s="28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>15</v>
@@ -1522,7 +1523,7 @@
     </row>
     <row r="30" spans="1:39" s="28" customFormat="1">
       <c r="A30" s="24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B30" s="45" t="s">
         <v>13</v>
@@ -1560,7 +1561,7 @@
     </row>
     <row r="31" spans="1:39" s="28" customFormat="1">
       <c r="A31" s="24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>16</v>
@@ -1640,12 +1641,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Improved the work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3264285-DB20-C947-A0F6-A7833CF6134A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D1496F-9D89-A847-891A-002FB452B71C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34620" yWindow="460" windowWidth="16580" windowHeight="31540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="39880" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="94">
   <si>
     <t>Week</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Create Git repository</t>
   </si>
   <si>
-    <t>Set up LaTeX files</t>
-  </si>
-  <si>
     <t>Start of Autumn Semester</t>
   </si>
   <si>
@@ -196,10 +193,6 @@
   <si>
     <t>7th December
 Interim Report - 10%</t>
-  </si>
-  <si>
-    <t>12th April
-Dissertation - 75%</t>
   </si>
   <si>
     <t>16/17th May
@@ -229,6 +222,12 @@
     <t>D3</t>
   </si>
   <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -265,9 +264,6 @@
     <t>C4</t>
   </si>
   <si>
-    <t>Research for Proposal</t>
-  </si>
-  <si>
     <t>SET/SEM Questionaries</t>
   </si>
   <si>
@@ -286,10 +282,50 @@
     <t>Project Proposal Draft</t>
   </si>
   <si>
+    <t>D6</t>
+  </si>
+  <si>
     <t>Preliminary Ethics Checklist</t>
   </si>
   <si>
     <t>Break these sections down furhter</t>
+  </si>
+  <si>
+    <t>Interim Report Related Work</t>
+  </si>
+  <si>
+    <t>Interim Report Finalise</t>
+  </si>
+  <si>
+    <t>12th April
+Research Paper - 75%</t>
+  </si>
+  <si>
+    <t>Interim Report Draft</t>
+  </si>
+  <si>
+    <t>Interim Report Outline Sections</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>Develop Solution</t>
+  </si>
+  <si>
+    <t>Install LaTeX</t>
+  </si>
+  <si>
+    <t>Proposal Proposal Research</t>
+  </si>
+  <si>
+    <t>GVGAI Basic Research</t>
+  </si>
+  <si>
+    <t>GVGAI Papers for Related Works</t>
+  </si>
+  <si>
+    <t>Other Related Works</t>
   </si>
 </sst>
 </file>
@@ -627,7 +663,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -687,6 +722,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,10 +1009,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM64"/>
+  <dimension ref="A1:AM74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -990,27 +1029,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="131">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="40"/>
       <c r="E1" s="40" t="s">
         <v>45</v>
       </c>
       <c r="F1" s="40"/>
-      <c r="G1" s="48" t="s">
-        <v>56</v>
+      <c r="G1" s="47" t="s">
+        <v>54</v>
       </c>
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
       <c r="J1" s="40"/>
       <c r="K1" s="40"/>
       <c r="L1" s="40"/>
-      <c r="M1" s="48" t="s">
-        <v>51</v>
+      <c r="M1" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="N1" s="40"/>
       <c r="O1" s="40"/>
@@ -1020,7 +1059,7 @@
       <c r="S1" s="40"/>
       <c r="T1" s="40"/>
       <c r="U1" s="40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V1" s="40"/>
       <c r="W1" s="40"/>
@@ -1031,622 +1070,789 @@
       <c r="AB1" s="40"/>
       <c r="AC1" s="40"/>
       <c r="AD1" s="40"/>
-      <c r="AE1" s="48" t="s">
-        <v>52</v>
+      <c r="AE1" s="47" t="s">
+        <v>84</v>
       </c>
       <c r="AF1" s="40"/>
       <c r="AH1" s="40"/>
       <c r="AI1" s="40"/>
       <c r="AJ1" s="40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="17" thickBot="1">
-      <c r="A2" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="46">
         <v>43367</v>
       </c>
-      <c r="D2" s="47">
+      <c r="D2" s="46">
         <v>43374</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="46">
         <v>43381</v>
       </c>
-      <c r="F2" s="47">
+      <c r="F2" s="46">
         <v>43388</v>
       </c>
-      <c r="G2" s="49">
+      <c r="G2" s="48">
         <v>43395</v>
       </c>
-      <c r="H2" s="47">
+      <c r="H2" s="46">
         <v>43402</v>
       </c>
-      <c r="I2" s="47">
+      <c r="I2" s="46">
         <v>43409</v>
       </c>
-      <c r="J2" s="47">
+      <c r="J2" s="46">
         <v>43416</v>
       </c>
-      <c r="K2" s="47">
+      <c r="K2" s="46">
         <v>43423</v>
       </c>
-      <c r="L2" s="47">
+      <c r="L2" s="46">
         <v>43430</v>
       </c>
-      <c r="M2" s="49">
+      <c r="M2" s="48">
         <v>43437</v>
       </c>
-      <c r="N2" s="47">
+      <c r="N2" s="46">
         <v>43444</v>
       </c>
-      <c r="O2" s="47">
+      <c r="O2" s="46">
         <v>43451</v>
       </c>
-      <c r="P2" s="47">
+      <c r="P2" s="46">
         <v>43458</v>
       </c>
-      <c r="Q2" s="47">
+      <c r="Q2" s="46">
         <v>43465</v>
       </c>
-      <c r="R2" s="47">
+      <c r="R2" s="46">
         <v>43472</v>
       </c>
-      <c r="S2" s="47">
+      <c r="S2" s="46">
         <v>43479</v>
       </c>
-      <c r="T2" s="47">
+      <c r="T2" s="46">
         <v>43486</v>
       </c>
-      <c r="U2" s="47">
+      <c r="U2" s="46">
         <v>43493</v>
       </c>
-      <c r="V2" s="47">
+      <c r="V2" s="46">
         <v>43500</v>
       </c>
-      <c r="W2" s="47">
+      <c r="W2" s="46">
         <v>43507</v>
       </c>
-      <c r="X2" s="47">
+      <c r="X2" s="46">
         <v>43514</v>
       </c>
-      <c r="Y2" s="47">
+      <c r="Y2" s="46">
         <v>43521</v>
       </c>
-      <c r="Z2" s="47">
+      <c r="Z2" s="46">
         <v>43528</v>
       </c>
-      <c r="AA2" s="47">
+      <c r="AA2" s="46">
         <v>43535</v>
       </c>
-      <c r="AB2" s="47">
+      <c r="AB2" s="46">
         <v>43542</v>
       </c>
-      <c r="AC2" s="47">
+      <c r="AC2" s="46">
         <v>43549</v>
       </c>
-      <c r="AD2" s="47">
+      <c r="AD2" s="46">
         <v>43556</v>
       </c>
-      <c r="AE2" s="49">
+      <c r="AE2" s="48">
         <v>43563</v>
       </c>
-      <c r="AF2" s="47">
+      <c r="AF2" s="46">
         <v>43570</v>
       </c>
-      <c r="AG2" s="47">
+      <c r="AG2" s="46">
         <v>43577</v>
       </c>
-      <c r="AH2" s="47">
+      <c r="AH2" s="46">
         <v>43584</v>
       </c>
-      <c r="AI2" s="47">
+      <c r="AI2" s="46">
         <v>43591</v>
       </c>
-      <c r="AJ2" s="47">
+      <c r="AJ2" s="46">
         <v>43598</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="17" thickTop="1">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="G3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="AE3" s="50"/>
+      <c r="B3" s="58"/>
+      <c r="G3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="AE3" s="49"/>
       <c r="AG3" s="28"/>
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>78</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
-      <c r="G4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="AE4" s="50"/>
+      <c r="G4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="AE4" s="49"/>
       <c r="AG4" s="28"/>
     </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="44" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="51"/>
-      <c r="M5" s="50"/>
-      <c r="AE5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="M5" s="49"/>
+      <c r="AE5" s="49"/>
       <c r="AG5" s="28"/>
     </row>
     <row r="6" spans="1:36">
       <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>80</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="24"/>
-      <c r="G6" s="51"/>
-      <c r="M6" s="50"/>
-      <c r="AE6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="M6" s="49"/>
+      <c r="AE6" s="49"/>
       <c r="AG6" s="28"/>
     </row>
     <row r="7" spans="1:36">
-      <c r="B7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="52"/>
-      <c r="M7" s="50"/>
-      <c r="AE7" s="50"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="51"/>
+      <c r="M7" s="49"/>
+      <c r="AE7" s="49"/>
       <c r="AG7" s="28"/>
     </row>
     <row r="8" spans="1:36">
-      <c r="B8" s="70" t="s">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="51"/>
+      <c r="I8" s="7"/>
+      <c r="M8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AG8" s="28"/>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="51"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="M9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AG9" s="28"/>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="51"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="49"/>
+      <c r="AE10" s="49"/>
+      <c r="AG10" s="28"/>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="51"/>
+      <c r="M11" s="50"/>
+      <c r="AE11" s="49"/>
+      <c r="AG11" s="28"/>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="B12" s="44"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="51"/>
+      <c r="M12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AG12" s="28"/>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="B13" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="52"/>
-      <c r="AE8" s="50"/>
-      <c r="AG8" s="28"/>
-    </row>
-    <row r="9" spans="1:36">
-      <c r="B9" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="50"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="51"/>
-      <c r="AE9" s="50"/>
-      <c r="AG9" s="28"/>
-    </row>
-    <row r="10" spans="1:36">
-      <c r="B10" s="45" t="s">
+      <c r="G13" s="49"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="51"/>
+      <c r="AE13" s="49"/>
+      <c r="AG13" s="28"/>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="B14" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="9"/>
-      <c r="AE10" s="50"/>
-      <c r="AG10" s="28"/>
-    </row>
-    <row r="11" spans="1:36">
-      <c r="B11" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
-      <c r="AE11" s="51"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="28"/>
-    </row>
-    <row r="12" spans="1:36">
-      <c r="A12" s="60" t="s">
+      <c r="G14" s="49"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="9"/>
+      <c r="AE14" s="49"/>
+      <c r="AG14" s="28"/>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="B15" s="44"/>
+      <c r="G15" s="49"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AE15" s="49"/>
+      <c r="AG15" s="28"/>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="B16" s="44"/>
+      <c r="G16" s="49"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AE16" s="49"/>
+      <c r="AG16" s="28"/>
+    </row>
+    <row r="17" spans="1:36">
+      <c r="B17" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="28"/>
+    </row>
+    <row r="18" spans="1:36">
+      <c r="B18" s="44"/>
+      <c r="G18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="51"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="28"/>
+    </row>
+    <row r="19" spans="1:36">
+      <c r="A19" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="G12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="AE12" s="50"/>
-      <c r="AG12" s="28"/>
-    </row>
-    <row r="13" spans="1:36">
-      <c r="A13" t="s">
+      <c r="B19" s="60"/>
+      <c r="G19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="AE19" s="49"/>
+      <c r="AG19" s="28"/>
+    </row>
+    <row r="20" spans="1:36">
+      <c r="A20" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B20" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="G20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="AE20" s="49"/>
+      <c r="AG20" s="28"/>
+    </row>
+    <row r="21" spans="1:36">
+      <c r="B21" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="G21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="AE21" s="49"/>
+      <c r="AG21" s="28"/>
+    </row>
+    <row r="22" spans="1:36">
+      <c r="B22" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="49"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="M22" s="49"/>
+      <c r="AE22" s="49"/>
+      <c r="AG22" s="28"/>
+    </row>
+    <row r="23" spans="1:36">
+      <c r="B23" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="49"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="M23" s="49"/>
+      <c r="AE23" s="49"/>
+      <c r="AG23" s="28"/>
+    </row>
+    <row r="24" spans="1:36">
+      <c r="B24" s="53"/>
+      <c r="G24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="AE24" s="49"/>
+      <c r="AG24" s="28"/>
+    </row>
+    <row r="25" spans="1:36">
+      <c r="A25" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="62"/>
+      <c r="G25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="AE25" s="49"/>
+      <c r="AG25" s="28"/>
+    </row>
+    <row r="26" spans="1:36">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AE26" s="49"/>
+      <c r="AG26" s="28"/>
+    </row>
+    <row r="27" spans="1:36">
+      <c r="B27" s="53"/>
+      <c r="G27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="AE27" s="49"/>
+      <c r="AG27" s="28"/>
+    </row>
+    <row r="28" spans="1:36">
+      <c r="A28" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="64"/>
+      <c r="G28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="AE28" s="49"/>
+      <c r="AG28" s="28"/>
+    </row>
+    <row r="29" spans="1:36">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="AE29" s="49"/>
+      <c r="AG29" s="28"/>
+      <c r="AH29" s="52"/>
+      <c r="AI29" s="52"/>
+    </row>
+    <row r="30" spans="1:36">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="AE30" s="49"/>
+      <c r="AG30" s="28"/>
+      <c r="AH30" s="52"/>
+      <c r="AI30" s="52"/>
+    </row>
+    <row r="31" spans="1:36">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="AE31" s="49"/>
+      <c r="AG31" s="28"/>
+      <c r="AJ31" s="52"/>
+    </row>
+    <row r="32" spans="1:36">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="AE32" s="49"/>
+      <c r="AG32" s="28"/>
+      <c r="AJ32" s="52"/>
+    </row>
+    <row r="33" spans="1:39">
+      <c r="A33" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="66"/>
+      <c r="G33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="AE33" s="49"/>
+      <c r="AG33" s="28"/>
+    </row>
+    <row r="34" spans="1:39">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="G34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AG34" s="28"/>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="G35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="AE35" s="49"/>
+      <c r="AG35" s="28"/>
+    </row>
+    <row r="36" spans="1:39">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="G13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="AE13" s="50"/>
-      <c r="AG13" s="28"/>
-    </row>
-    <row r="14" spans="1:36">
-      <c r="B14" s="54"/>
-      <c r="G14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="AE14" s="50"/>
-      <c r="AG14" s="28"/>
-    </row>
-    <row r="15" spans="1:36">
-      <c r="A15" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="63"/>
-      <c r="G15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="AE15" s="50"/>
-      <c r="AG15" s="28"/>
-    </row>
-    <row r="16" spans="1:36">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="G16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="AE16" s="50"/>
-      <c r="AG16" s="28"/>
-    </row>
-    <row r="17" spans="1:39">
-      <c r="B17" s="54"/>
-      <c r="G17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="AE17" s="50"/>
-      <c r="AG17" s="28"/>
-    </row>
-    <row r="18" spans="1:39">
-      <c r="A18" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="65"/>
-      <c r="G18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="AE18" s="50"/>
-      <c r="AG18" s="28"/>
-    </row>
-    <row r="19" spans="1:39">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="AE19" s="50"/>
-      <c r="AG19" s="28"/>
-      <c r="AH19" s="53"/>
-      <c r="AI19" s="53"/>
-    </row>
-    <row r="20" spans="1:39">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="AE20" s="50"/>
-      <c r="AG20" s="28"/>
-      <c r="AH20" s="53"/>
-      <c r="AI20" s="53"/>
-    </row>
-    <row r="21" spans="1:39">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="AE21" s="50"/>
-      <c r="AG21" s="28"/>
-      <c r="AJ21" s="53"/>
-    </row>
-    <row r="22" spans="1:39">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="45" t="s">
+      <c r="G36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="AC36" s="24"/>
+      <c r="AD36" s="24"/>
+      <c r="AE36" s="49"/>
+      <c r="AG36" s="28"/>
+      <c r="AJ36" s="12"/>
+    </row>
+    <row r="37" spans="1:39">
+      <c r="A37" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="68"/>
+      <c r="G37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="AE37" s="49"/>
+      <c r="AG37" s="28"/>
+    </row>
+    <row r="38" spans="1:39">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="AE22" s="50"/>
-      <c r="AG22" s="28"/>
-      <c r="AJ22" s="53"/>
-    </row>
-    <row r="23" spans="1:39">
-      <c r="A23" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="67"/>
-      <c r="G23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="AE23" s="50"/>
-      <c r="AG23" s="28"/>
-    </row>
-    <row r="24" spans="1:39">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="G24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="AE24" s="50"/>
-      <c r="AG24" s="28"/>
-    </row>
-    <row r="25" spans="1:39">
-      <c r="A25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="12"/>
-      <c r="G25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="AE25" s="50"/>
-      <c r="AG25" s="28"/>
-    </row>
-    <row r="26" spans="1:39">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="50"/>
-      <c r="M26" s="50"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="AC26" s="24"/>
-      <c r="AD26" s="24"/>
-      <c r="AE26" s="50"/>
-      <c r="AG26" s="28"/>
-      <c r="AJ26" s="12"/>
-    </row>
-    <row r="27" spans="1:39">
-      <c r="A27" s="68" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="69"/>
-      <c r="G27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="AE27" s="50"/>
-      <c r="AG27" s="28"/>
-    </row>
-    <row r="28" spans="1:39">
-      <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="G28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="AE28" s="50"/>
-      <c r="AG28" s="28"/>
-    </row>
-    <row r="29" spans="1:39" s="28" customFormat="1">
-      <c r="A29" s="28" t="s">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="G38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="AE38" s="49"/>
+      <c r="AG38" s="28"/>
+    </row>
+    <row r="39" spans="1:39" s="28" customFormat="1">
+      <c r="A39" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29" s="50"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29" s="50"/>
-      <c r="N29"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29"/>
-      <c r="T29"/>
-      <c r="U29"/>
-      <c r="V29"/>
-      <c r="W29"/>
-      <c r="X29"/>
-      <c r="Y29"/>
-      <c r="Z29"/>
-      <c r="AA29"/>
-      <c r="AB29"/>
-      <c r="AC29"/>
-      <c r="AD29"/>
-      <c r="AE29" s="50"/>
-      <c r="AF29"/>
-      <c r="AM29" s="39"/>
-    </row>
-    <row r="30" spans="1:39" s="28" customFormat="1">
-      <c r="A30" s="24" t="s">
+      <c r="C39" s="9"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39" s="49"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39" s="49"/>
+      <c r="N39"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39"/>
+      <c r="AA39"/>
+      <c r="AB39"/>
+      <c r="AC39"/>
+      <c r="AD39"/>
+      <c r="AE39" s="49"/>
+      <c r="AF39"/>
+      <c r="AM39" s="39"/>
+    </row>
+    <row r="40" spans="1:39" s="28" customFormat="1">
+      <c r="A40" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B40" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30" s="50"/>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30" s="50"/>
-      <c r="N30"/>
-      <c r="O30"/>
-      <c r="P30"/>
-      <c r="Q30"/>
-      <c r="R30"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30"/>
-      <c r="V30"/>
-      <c r="W30"/>
-      <c r="X30"/>
-      <c r="Y30"/>
-      <c r="Z30"/>
-      <c r="AA30"/>
-      <c r="AB30"/>
-      <c r="AC30"/>
-      <c r="AD30"/>
-      <c r="AE30" s="50"/>
-      <c r="AF30"/>
-    </row>
-    <row r="31" spans="1:39" s="28" customFormat="1">
-      <c r="A31" s="24" t="s">
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40" s="49"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40" s="49"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+      <c r="AA40"/>
+      <c r="AB40"/>
+      <c r="AC40"/>
+      <c r="AD40"/>
+      <c r="AE40" s="49"/>
+      <c r="AF40"/>
+    </row>
+    <row r="41" spans="1:39" s="28" customFormat="1">
+      <c r="A41" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B41" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31" s="50"/>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31" s="50"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31"/>
-      <c r="S31"/>
-      <c r="T31"/>
-      <c r="U31"/>
-      <c r="V31"/>
-      <c r="W31"/>
-      <c r="X31"/>
-      <c r="Y31"/>
-      <c r="Z31"/>
-      <c r="AA31"/>
-      <c r="AB31"/>
-      <c r="AC31" s="9"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="52"/>
-      <c r="AF31" s="8"/>
-      <c r="AG31" s="56"/>
-      <c r="AH31" s="56"/>
-      <c r="AI31" s="56"/>
-    </row>
-    <row r="32" spans="1:39" s="28" customFormat="1"/>
-    <row r="33" s="28" customFormat="1"/>
-    <row r="34" s="28" customFormat="1"/>
-    <row r="35" s="28" customFormat="1"/>
-    <row r="36" s="28" customFormat="1"/>
-    <row r="37" s="28" customFormat="1"/>
-    <row r="38" s="28" customFormat="1"/>
-    <row r="39" s="28" customFormat="1"/>
-    <row r="40" s="28" customFormat="1"/>
-    <row r="41" s="28" customFormat="1"/>
-    <row r="42" s="28" customFormat="1"/>
-    <row r="43" s="28" customFormat="1"/>
-    <row r="44" s="28" customFormat="1"/>
-    <row r="45" s="28" customFormat="1"/>
-    <row r="46" s="28" customFormat="1"/>
-    <row r="47" s="28" customFormat="1"/>
-    <row r="48" s="28" customFormat="1"/>
-    <row r="49" spans="2:2" s="28" customFormat="1"/>
-    <row r="50" spans="2:2" s="28" customFormat="1"/>
-    <row r="51" spans="2:2" s="28" customFormat="1"/>
-    <row r="52" spans="2:2" s="28" customFormat="1"/>
-    <row r="53" spans="2:2" s="28" customFormat="1"/>
-    <row r="54" spans="2:2" s="28" customFormat="1"/>
-    <row r="55" spans="2:2" s="28" customFormat="1"/>
-    <row r="56" spans="2:2" s="28" customFormat="1"/>
-    <row r="57" spans="2:2" s="28" customFormat="1"/>
-    <row r="58" spans="2:2" s="28" customFormat="1"/>
-    <row r="59" spans="2:2" s="28" customFormat="1"/>
-    <row r="60" spans="2:2" s="28" customFormat="1"/>
-    <row r="61" spans="2:2" s="28" customFormat="1"/>
-    <row r="62" spans="2:2">
-      <c r="B62" s="28"/>
-    </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="28"/>
-    </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="28"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41" s="49"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41" s="49"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+      <c r="Z41"/>
+      <c r="AA41"/>
+      <c r="AB41"/>
+      <c r="AC41" s="9"/>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="51"/>
+      <c r="AF41" s="8"/>
+      <c r="AG41" s="55"/>
+      <c r="AH41" s="55"/>
+      <c r="AI41" s="55"/>
+    </row>
+    <row r="42" spans="1:39" s="28" customFormat="1"/>
+    <row r="43" spans="1:39" s="28" customFormat="1"/>
+    <row r="44" spans="1:39" s="28" customFormat="1"/>
+    <row r="45" spans="1:39" s="28" customFormat="1"/>
+    <row r="46" spans="1:39" s="28" customFormat="1"/>
+    <row r="47" spans="1:39" s="28" customFormat="1"/>
+    <row r="48" spans="1:39" s="28" customFormat="1"/>
+    <row r="49" s="28" customFormat="1"/>
+    <row r="50" s="28" customFormat="1"/>
+    <row r="51" s="28" customFormat="1"/>
+    <row r="52" s="28" customFormat="1"/>
+    <row r="53" s="28" customFormat="1"/>
+    <row r="54" s="28" customFormat="1"/>
+    <row r="55" s="28" customFormat="1"/>
+    <row r="56" s="28" customFormat="1"/>
+    <row r="57" s="28" customFormat="1"/>
+    <row r="58" s="28" customFormat="1"/>
+    <row r="59" s="28" customFormat="1"/>
+    <row r="60" s="28" customFormat="1"/>
+    <row r="61" s="28" customFormat="1"/>
+    <row r="62" s="28" customFormat="1"/>
+    <row r="63" s="28" customFormat="1"/>
+    <row r="64" s="28" customFormat="1"/>
+    <row r="65" spans="2:2" s="28" customFormat="1"/>
+    <row r="66" spans="2:2" s="28" customFormat="1"/>
+    <row r="67" spans="2:2" s="28" customFormat="1"/>
+    <row r="68" spans="2:2" s="28" customFormat="1"/>
+    <row r="69" spans="2:2" s="28" customFormat="1"/>
+    <row r="70" spans="2:2" s="28" customFormat="1"/>
+    <row r="71" spans="2:2" s="28" customFormat="1"/>
+    <row r="72" spans="2:2">
+      <c r="B72" s="28"/>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="28"/>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1661,7 +1867,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2353,11 +2559,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="142" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O21" sqref="O21:Q21"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2784,7 +2990,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y26" sqref="Y26:Z26"/>
+      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Created Project Proposal work plan descriptions
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D1496F-9D89-A847-891A-002FB452B71C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C71AFA-89E7-3442-8334-B1A9A5C2F024}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="39880" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="460" windowWidth="18680" windowHeight="35540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
-    <sheet name="Dissertation - Old" sheetId="4" r:id="rId2"/>
-    <sheet name="Original - Old" sheetId="1" r:id="rId3"/>
-    <sheet name="Interim Report - Old" sheetId="3" r:id="rId4"/>
-    <sheet name="Dissertation to print - Old" sheetId="5" r:id="rId5"/>
+    <sheet name="Project Proposal - to print" sheetId="8" r:id="rId2"/>
+    <sheet name="Dissertation - Old" sheetId="4" r:id="rId3"/>
+    <sheet name="Original - Old" sheetId="1" r:id="rId4"/>
+    <sheet name="Interim Report - Old" sheetId="3" r:id="rId5"/>
+    <sheet name="Dissertation to print - Old" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="98">
   <si>
     <t>Week</t>
   </si>
@@ -186,9 +187,6 @@
   </si>
   <si>
     <t>Start of Spring Semester</t>
-  </si>
-  <si>
-    <t>Research Paper</t>
   </si>
   <si>
     <t>7th December
@@ -288,9 +286,6 @@
     <t>Preliminary Ethics Checklist</t>
   </si>
   <si>
-    <t>Break these sections down furhter</t>
-  </si>
-  <si>
     <t>Interim Report Related Work</t>
   </si>
   <si>
@@ -316,9 +311,6 @@
     <t>Install LaTeX</t>
   </si>
   <si>
-    <t>Proposal Proposal Research</t>
-  </si>
-  <si>
     <t>GVGAI Basic Research</t>
   </si>
   <si>
@@ -326,6 +318,27 @@
   </si>
   <si>
     <t>Other Related Works</t>
+  </si>
+  <si>
+    <t>Presentation General Outline</t>
+  </si>
+  <si>
+    <t>Research Paper - Break down further</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>Project Proposal Research</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
   </si>
 </sst>
 </file>
@@ -605,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -681,7 +694,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -721,8 +733,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,19 +1021,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM74"/>
+  <dimension ref="A1:AM65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB15" sqref="AB15"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="9.1640625" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" style="28" customWidth="1"/>
     <col min="14" max="36" width="9.1640625" customWidth="1"/>
@@ -1041,7 +1053,7 @@
       </c>
       <c r="F1" s="40"/>
       <c r="G1" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
@@ -1049,7 +1061,7 @@
       <c r="K1" s="40"/>
       <c r="L1" s="40"/>
       <c r="M1" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N1" s="40"/>
       <c r="O1" s="40"/>
@@ -1071,18 +1083,18 @@
       <c r="AC1" s="40"/>
       <c r="AD1" s="40"/>
       <c r="AE1" s="47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AF1" s="40"/>
       <c r="AH1" s="40"/>
       <c r="AI1" s="40"/>
       <c r="AJ1" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="17" thickBot="1">
-      <c r="A2" s="56" t="s">
-        <v>55</v>
+      <c r="A2" s="55" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>0</v>
@@ -1191,10 +1203,10 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="17" thickTop="1">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="57"/>
       <c r="G3" s="49"/>
       <c r="M3" s="49"/>
       <c r="AE3" s="49"/>
@@ -1202,10 +1214,10 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
@@ -1216,7 +1228,7 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>14</v>
@@ -1231,10 +1243,10 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1245,11 +1257,17 @@
       <c r="AG6" s="28"/>
     </row>
     <row r="7" spans="1:36">
-      <c r="B7" s="44"/>
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>84</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="24"/>
       <c r="G7" s="51"/>
+      <c r="I7" s="7"/>
       <c r="M7" s="49"/>
       <c r="AE7" s="49"/>
       <c r="AG7" s="28"/>
@@ -1259,600 +1277,482 @@
         <v>59</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="24"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="51"/>
       <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="M8" s="49"/>
       <c r="AE8" s="49"/>
       <c r="AG8" s="28"/>
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="7"/>
       <c r="M9" s="49"/>
       <c r="AE9" s="49"/>
       <c r="AG9" s="28"/>
     </row>
     <row r="10" spans="1:36">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="51"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="49"/>
+      <c r="M10" s="50"/>
       <c r="AE10" s="49"/>
       <c r="AG10" s="28"/>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="51"/>
-      <c r="M11" s="50"/>
-      <c r="AE11" s="49"/>
+        <v>92</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="50"/>
+      <c r="AF11" s="9"/>
       <c r="AG11" s="28"/>
     </row>
     <row r="12" spans="1:36">
-      <c r="B12" s="44"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="51"/>
+      <c r="A12" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="59"/>
+      <c r="G12" s="49"/>
       <c r="M12" s="49"/>
       <c r="AE12" s="49"/>
       <c r="AG12" s="28"/>
     </row>
     <row r="13" spans="1:36">
-      <c r="B13" s="69" t="s">
-        <v>81</v>
-      </c>
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="49"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="51"/>
+      <c r="M13" s="49"/>
       <c r="AE13" s="49"/>
       <c r="AG13" s="28"/>
     </row>
     <row r="14" spans="1:36">
-      <c r="B14" s="44" t="s">
-        <v>35</v>
-      </c>
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
       <c r="G14" s="49"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="9"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="M14" s="49"/>
       <c r="AE14" s="49"/>
       <c r="AG14" s="28"/>
     </row>
     <row r="15" spans="1:36">
-      <c r="B15" s="44"/>
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>89</v>
+      </c>
       <c r="G15" s="49"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="M15" s="49"/>
       <c r="AE15" s="49"/>
       <c r="AG15" s="28"/>
     </row>
     <row r="16" spans="1:36">
-      <c r="B16" s="44"/>
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>90</v>
+      </c>
       <c r="G16" s="49"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="9"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="M16" s="49"/>
       <c r="AE16" s="49"/>
       <c r="AG16" s="28"/>
     </row>
-    <row r="17" spans="1:36">
-      <c r="B17" s="44" t="s">
-        <v>49</v>
-      </c>
+    <row r="17" spans="1:39">
+      <c r="A17" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="61"/>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="50"/>
-      <c r="AF17" s="9"/>
+      <c r="AE17" s="49"/>
       <c r="AG17" s="28"/>
     </row>
-    <row r="18" spans="1:36">
-      <c r="B18" s="44"/>
+    <row r="18" spans="1:39">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>86</v>
+      </c>
       <c r="G18" s="49"/>
       <c r="M18" s="49"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="51"/>
-      <c r="AF18" s="9"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AE18" s="49"/>
       <c r="AG18" s="28"/>
     </row>
-    <row r="19" spans="1:36">
-      <c r="A19" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="60"/>
+    <row r="19" spans="1:39">
+      <c r="A19" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="63"/>
       <c r="G19" s="49"/>
       <c r="M19" s="49"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
       <c r="AE19" s="49"/>
       <c r="AG19" s="28"/>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:39">
       <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>91</v>
+      </c>
       <c r="G20" s="49"/>
       <c r="M20" s="49"/>
       <c r="AE20" s="49"/>
       <c r="AG20" s="28"/>
-    </row>
-    <row r="21" spans="1:36">
-      <c r="B21" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="AH20" s="52"/>
+      <c r="AI20" s="52"/>
+    </row>
+    <row r="21" spans="1:39">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>52</v>
+      </c>
       <c r="G21" s="49"/>
       <c r="M21" s="49"/>
       <c r="AE21" s="49"/>
       <c r="AG21" s="28"/>
-    </row>
-    <row r="22" spans="1:36">
-      <c r="B22" s="54" t="s">
-        <v>92</v>
+      <c r="AH21" s="52"/>
+      <c r="AI21" s="52"/>
+    </row>
+    <row r="22" spans="1:39">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>41</v>
       </c>
       <c r="G22" s="49"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
       <c r="M22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AG22" s="28"/>
-    </row>
-    <row r="23" spans="1:36">
-      <c r="B23" s="54" t="s">
-        <v>93</v>
+      <c r="AJ22" s="52"/>
+    </row>
+    <row r="23" spans="1:39">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>75</v>
       </c>
       <c r="G23" s="49"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
       <c r="M23" s="49"/>
       <c r="AE23" s="49"/>
       <c r="AG23" s="28"/>
-    </row>
-    <row r="24" spans="1:36">
-      <c r="B24" s="53"/>
+      <c r="AJ23" s="52"/>
+    </row>
+    <row r="24" spans="1:39">
+      <c r="A24" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="65"/>
       <c r="G24" s="49"/>
       <c r="M24" s="49"/>
       <c r="AE24" s="49"/>
       <c r="AG24" s="28"/>
     </row>
-    <row r="25" spans="1:36">
-      <c r="A25" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="62"/>
+    <row r="25" spans="1:39">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="12"/>
       <c r="G25" s="49"/>
       <c r="M25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AG25" s="28"/>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:39">
       <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="54" t="s">
-        <v>88</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="12"/>
       <c r="G26" s="49"/>
       <c r="M26" s="49"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-      <c r="W26" s="10"/>
-      <c r="X26" s="10"/>
-      <c r="Y26" s="10"/>
-      <c r="Z26" s="10"/>
       <c r="AE26" s="49"/>
       <c r="AG26" s="28"/>
     </row>
-    <row r="27" spans="1:36">
-      <c r="B27" s="53"/>
+    <row r="27" spans="1:39">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="G27" s="49"/>
       <c r="M27" s="49"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="AC27" s="24"/>
+      <c r="AD27" s="24"/>
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
-    </row>
-    <row r="28" spans="1:36">
-      <c r="A28" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="64"/>
+      <c r="AJ27" s="12"/>
+    </row>
+    <row r="28" spans="1:39">
+      <c r="A28" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="67"/>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
       <c r="AE28" s="49"/>
       <c r="AG28" s="28"/>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:39">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>42</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
       <c r="AE29" s="49"/>
       <c r="AG29" s="28"/>
-      <c r="AH29" s="52"/>
-      <c r="AI29" s="52"/>
-    </row>
-    <row r="30" spans="1:36">
-      <c r="A30" t="s">
-        <v>64</v>
+    </row>
+    <row r="30" spans="1:39" s="28" customFormat="1">
+      <c r="A30" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>53</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
       <c r="G30" s="49"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
       <c r="M30" s="49"/>
+      <c r="N30"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+      <c r="AB30"/>
+      <c r="AC30"/>
+      <c r="AD30"/>
       <c r="AE30" s="49"/>
-      <c r="AG30" s="28"/>
-      <c r="AH30" s="52"/>
-      <c r="AI30" s="52"/>
-    </row>
-    <row r="31" spans="1:36">
-      <c r="A31" t="s">
-        <v>65</v>
+      <c r="AF30"/>
+      <c r="AM30" s="39"/>
+    </row>
+    <row r="31" spans="1:39" s="28" customFormat="1">
+      <c r="A31" s="24" t="s">
+        <v>70</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>41</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
       <c r="G31" s="49"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
       <c r="M31" s="49"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
+      <c r="AB31"/>
+      <c r="AC31"/>
+      <c r="AD31"/>
       <c r="AE31" s="49"/>
-      <c r="AG31" s="28"/>
-      <c r="AJ31" s="52"/>
-    </row>
-    <row r="32" spans="1:36">
-      <c r="A32" t="s">
-        <v>75</v>
+      <c r="AF31"/>
+    </row>
+    <row r="32" spans="1:39" s="28" customFormat="1">
+      <c r="A32" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>76</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
       <c r="G32" s="49"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
       <c r="M32" s="49"/>
-      <c r="AE32" s="49"/>
-      <c r="AG32" s="28"/>
-      <c r="AJ32" s="52"/>
-    </row>
-    <row r="33" spans="1:39">
-      <c r="A33" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="66"/>
-      <c r="G33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="AE33" s="49"/>
-      <c r="AG33" s="28"/>
-    </row>
-    <row r="34" spans="1:39">
-      <c r="A34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="12"/>
-      <c r="G34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="AE34" s="49"/>
-      <c r="AG34" s="28"/>
-    </row>
-    <row r="35" spans="1:39">
-      <c r="A35" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="12"/>
-      <c r="G35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="AE35" s="49"/>
-      <c r="AG35" s="28"/>
-    </row>
-    <row r="36" spans="1:39">
-      <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="AC36" s="24"/>
-      <c r="AD36" s="24"/>
-      <c r="AE36" s="49"/>
-      <c r="AG36" s="28"/>
-      <c r="AJ36" s="12"/>
-    </row>
-    <row r="37" spans="1:39">
-      <c r="A37" s="67" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="68"/>
-      <c r="G37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="AE37" s="49"/>
-      <c r="AG37" s="28"/>
-    </row>
-    <row r="38" spans="1:39">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="G38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="AE38" s="49"/>
-      <c r="AG38" s="28"/>
-    </row>
-    <row r="39" spans="1:39" s="28" customFormat="1">
-      <c r="A39" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39" s="49"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39" s="49"/>
-      <c r="N39"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-      <c r="AB39"/>
-      <c r="AC39"/>
-      <c r="AD39"/>
-      <c r="AE39" s="49"/>
-      <c r="AF39"/>
-      <c r="AM39" s="39"/>
-    </row>
-    <row r="40" spans="1:39" s="28" customFormat="1">
-      <c r="A40" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40" s="49"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40" s="49"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-      <c r="X40"/>
-      <c r="Y40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AB40"/>
-      <c r="AC40"/>
-      <c r="AD40"/>
-      <c r="AE40" s="49"/>
-      <c r="AF40"/>
-    </row>
-    <row r="41" spans="1:39" s="28" customFormat="1">
-      <c r="A41" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41" s="49"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41" s="49"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
-      <c r="Y41"/>
-      <c r="Z41"/>
-      <c r="AA41"/>
-      <c r="AB41"/>
-      <c r="AC41" s="9"/>
-      <c r="AD41" s="9"/>
-      <c r="AE41" s="51"/>
-      <c r="AF41" s="8"/>
-      <c r="AG41" s="55"/>
-      <c r="AH41" s="55"/>
-      <c r="AI41" s="55"/>
-    </row>
-    <row r="42" spans="1:39" s="28" customFormat="1"/>
-    <row r="43" spans="1:39" s="28" customFormat="1"/>
-    <row r="44" spans="1:39" s="28" customFormat="1"/>
-    <row r="45" spans="1:39" s="28" customFormat="1"/>
-    <row r="46" spans="1:39" s="28" customFormat="1"/>
-    <row r="47" spans="1:39" s="28" customFormat="1"/>
-    <row r="48" spans="1:39" s="28" customFormat="1"/>
-    <row r="49" s="28" customFormat="1"/>
-    <row r="50" s="28" customFormat="1"/>
-    <row r="51" s="28" customFormat="1"/>
-    <row r="52" s="28" customFormat="1"/>
-    <row r="53" s="28" customFormat="1"/>
-    <row r="54" s="28" customFormat="1"/>
-    <row r="55" s="28" customFormat="1"/>
-    <row r="56" s="28" customFormat="1"/>
-    <row r="57" s="28" customFormat="1"/>
-    <row r="58" s="28" customFormat="1"/>
-    <row r="59" s="28" customFormat="1"/>
-    <row r="60" s="28" customFormat="1"/>
-    <row r="61" s="28" customFormat="1"/>
-    <row r="62" s="28" customFormat="1"/>
-    <row r="63" s="28" customFormat="1"/>
-    <row r="64" s="28" customFormat="1"/>
-    <row r="65" spans="2:2" s="28" customFormat="1"/>
-    <row r="66" spans="2:2" s="28" customFormat="1"/>
-    <row r="67" spans="2:2" s="28" customFormat="1"/>
-    <row r="68" spans="2:2" s="28" customFormat="1"/>
-    <row r="69" spans="2:2" s="28" customFormat="1"/>
-    <row r="70" spans="2:2" s="28" customFormat="1"/>
-    <row r="71" spans="2:2" s="28" customFormat="1"/>
-    <row r="72" spans="2:2">
-      <c r="B72" s="28"/>
-    </row>
-    <row r="73" spans="2:2">
-      <c r="B73" s="28"/>
-    </row>
-    <row r="74" spans="2:2">
-      <c r="B74" s="28"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+      <c r="AB32"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="51"/>
+      <c r="AF32" s="8"/>
+      <c r="AG32" s="54"/>
+      <c r="AH32" s="54"/>
+      <c r="AI32" s="54"/>
+    </row>
+    <row r="33" s="28" customFormat="1"/>
+    <row r="34" s="28" customFormat="1"/>
+    <row r="35" s="28" customFormat="1"/>
+    <row r="36" s="28" customFormat="1"/>
+    <row r="37" s="28" customFormat="1"/>
+    <row r="38" s="28" customFormat="1"/>
+    <row r="39" s="28" customFormat="1"/>
+    <row r="40" s="28" customFormat="1"/>
+    <row r="41" s="28" customFormat="1"/>
+    <row r="42" s="28" customFormat="1"/>
+    <row r="43" s="28" customFormat="1"/>
+    <row r="44" s="28" customFormat="1"/>
+    <row r="45" s="28" customFormat="1"/>
+    <row r="46" s="28" customFormat="1"/>
+    <row r="47" s="28" customFormat="1"/>
+    <row r="48" s="28" customFormat="1"/>
+    <row r="49" spans="2:2" s="28" customFormat="1"/>
+    <row r="50" spans="2:2" s="28" customFormat="1"/>
+    <row r="51" spans="2:2" s="28" customFormat="1"/>
+    <row r="52" spans="2:2" s="28" customFormat="1"/>
+    <row r="53" spans="2:2" s="28" customFormat="1"/>
+    <row r="54" spans="2:2" s="28" customFormat="1"/>
+    <row r="55" spans="2:2" s="28" customFormat="1"/>
+    <row r="56" spans="2:2" s="28" customFormat="1"/>
+    <row r="57" spans="2:2" s="28" customFormat="1"/>
+    <row r="58" spans="2:2" s="28" customFormat="1"/>
+    <row r="59" spans="2:2" s="28" customFormat="1"/>
+    <row r="60" spans="2:2" s="28" customFormat="1"/>
+    <row r="61" spans="2:2" s="28" customFormat="1"/>
+    <row r="62" spans="2:2" s="28" customFormat="1"/>
+    <row r="63" spans="2:2">
+      <c r="B63" s="28"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="28"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1860,6 +1760,746 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9D7B89-5ABB-3F4A-8359-7BEAEA14AC00}">
+  <dimension ref="A1:AM65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="9.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="28" customWidth="1"/>
+    <col min="14" max="36" width="9.1640625" customWidth="1"/>
+    <col min="37" max="37" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="131">
+      <c r="B1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="40"/>
+      <c r="G1" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="17" thickBot="1">
+      <c r="A2" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="46">
+        <v>43367</v>
+      </c>
+      <c r="D2" s="46">
+        <v>43374</v>
+      </c>
+      <c r="E2" s="46">
+        <v>43381</v>
+      </c>
+      <c r="F2" s="46">
+        <v>43388</v>
+      </c>
+      <c r="G2" s="48">
+        <v>43395</v>
+      </c>
+      <c r="H2" s="46">
+        <v>43402</v>
+      </c>
+      <c r="I2" s="46">
+        <v>43409</v>
+      </c>
+      <c r="J2" s="46">
+        <v>43416</v>
+      </c>
+      <c r="K2" s="46">
+        <v>43423</v>
+      </c>
+      <c r="L2" s="46">
+        <v>43430</v>
+      </c>
+      <c r="M2" s="48">
+        <v>43437</v>
+      </c>
+      <c r="N2" s="46">
+        <v>43444</v>
+      </c>
+      <c r="O2" s="46">
+        <v>43451</v>
+      </c>
+      <c r="P2" s="46">
+        <v>43458</v>
+      </c>
+      <c r="Q2" s="46">
+        <v>43465</v>
+      </c>
+      <c r="R2" s="46">
+        <v>43472</v>
+      </c>
+      <c r="S2" s="46">
+        <v>43479</v>
+      </c>
+      <c r="T2" s="46">
+        <v>43486</v>
+      </c>
+      <c r="U2" s="46">
+        <v>43493</v>
+      </c>
+      <c r="V2" s="46">
+        <v>43500</v>
+      </c>
+      <c r="W2" s="46">
+        <v>43507</v>
+      </c>
+      <c r="X2" s="46">
+        <v>43514</v>
+      </c>
+      <c r="Y2" s="46">
+        <v>43521</v>
+      </c>
+      <c r="Z2" s="46">
+        <v>43528</v>
+      </c>
+      <c r="AA2" s="46">
+        <v>43535</v>
+      </c>
+      <c r="AB2" s="46">
+        <v>43542</v>
+      </c>
+      <c r="AC2" s="46">
+        <v>43549</v>
+      </c>
+      <c r="AD2" s="46">
+        <v>43556</v>
+      </c>
+      <c r="AE2" s="48">
+        <v>43563</v>
+      </c>
+      <c r="AF2" s="46">
+        <v>43570</v>
+      </c>
+      <c r="AG2" s="46">
+        <v>43577</v>
+      </c>
+      <c r="AH2" s="46">
+        <v>43584</v>
+      </c>
+      <c r="AI2" s="46">
+        <v>43591</v>
+      </c>
+      <c r="AJ2" s="46">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="17" thickTop="1">
+      <c r="A3" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="G3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AG3" s="28"/>
+    </row>
+    <row r="4" spans="1:36">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="7"/>
+      <c r="G4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="AE4" s="49"/>
+      <c r="AG4" s="28"/>
+    </row>
+    <row r="5" spans="1:36">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="50"/>
+      <c r="M5" s="49"/>
+      <c r="AE5" s="49"/>
+      <c r="AG5" s="28"/>
+    </row>
+    <row r="6" spans="1:36">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="50"/>
+      <c r="M6" s="49"/>
+      <c r="AE6" s="49"/>
+      <c r="AG6" s="28"/>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="51"/>
+      <c r="I7" s="7"/>
+      <c r="M7" s="49"/>
+      <c r="AE7" s="49"/>
+      <c r="AG7" s="28"/>
+    </row>
+    <row r="8" spans="1:36">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="51"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="M8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AG8" s="28"/>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="51"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AG9" s="28"/>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="51"/>
+      <c r="M10" s="50"/>
+      <c r="AE10" s="49"/>
+      <c r="AG10" s="28"/>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="50"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="28"/>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="A12" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="59"/>
+      <c r="G12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AG12" s="28"/>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="AE13" s="49"/>
+      <c r="AG13" s="28"/>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="M14" s="49"/>
+      <c r="AE14" s="49"/>
+      <c r="AG14" s="28"/>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="49"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="M15" s="49"/>
+      <c r="AE15" s="49"/>
+      <c r="AG15" s="28"/>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="M16" s="49"/>
+      <c r="AE16" s="49"/>
+      <c r="AG16" s="28"/>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="61"/>
+      <c r="G17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="AE17" s="49"/>
+      <c r="AG17" s="28"/>
+    </row>
+    <row r="18" spans="1:39">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AE18" s="49"/>
+      <c r="AG18" s="28"/>
+    </row>
+    <row r="19" spans="1:39">
+      <c r="A19" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="G19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="AE19" s="49"/>
+      <c r="AG19" s="28"/>
+    </row>
+    <row r="20" spans="1:39">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="AE20" s="49"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="52"/>
+      <c r="AI20" s="52"/>
+    </row>
+    <row r="21" spans="1:39">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="AE21" s="49"/>
+      <c r="AG21" s="28"/>
+      <c r="AH21" s="52"/>
+      <c r="AI21" s="52"/>
+    </row>
+    <row r="22" spans="1:39">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="AE22" s="49"/>
+      <c r="AG22" s="28"/>
+      <c r="AJ22" s="52"/>
+    </row>
+    <row r="23" spans="1:39">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="AE23" s="49"/>
+      <c r="AG23" s="28"/>
+      <c r="AJ23" s="52"/>
+    </row>
+    <row r="24" spans="1:39">
+      <c r="A24" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="65"/>
+      <c r="G24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="AE24" s="49"/>
+      <c r="AG24" s="28"/>
+    </row>
+    <row r="25" spans="1:39">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="G25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="AE25" s="49"/>
+      <c r="AG25" s="28"/>
+    </row>
+    <row r="26" spans="1:39">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="G26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="AE26" s="49"/>
+      <c r="AG26" s="28"/>
+    </row>
+    <row r="27" spans="1:39">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="AC27" s="24"/>
+      <c r="AD27" s="24"/>
+      <c r="AE27" s="49"/>
+      <c r="AG27" s="28"/>
+      <c r="AJ27" s="12"/>
+    </row>
+    <row r="28" spans="1:39">
+      <c r="A28" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="67"/>
+      <c r="G28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="AE28" s="49"/>
+      <c r="AG28" s="28"/>
+    </row>
+    <row r="29" spans="1:39">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="G29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="AE29" s="49"/>
+      <c r="AG29" s="28"/>
+    </row>
+    <row r="30" spans="1:39" s="28" customFormat="1">
+      <c r="A30" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30" s="49"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30" s="49"/>
+      <c r="N30"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+      <c r="AB30"/>
+      <c r="AC30"/>
+      <c r="AD30"/>
+      <c r="AE30" s="49"/>
+      <c r="AF30"/>
+      <c r="AM30" s="39"/>
+    </row>
+    <row r="31" spans="1:39" s="28" customFormat="1">
+      <c r="A31" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31" s="49"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31" s="49"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
+      <c r="AB31"/>
+      <c r="AC31"/>
+      <c r="AD31"/>
+      <c r="AE31" s="49"/>
+      <c r="AF31"/>
+    </row>
+    <row r="32" spans="1:39" s="28" customFormat="1">
+      <c r="A32" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32" s="49"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32" s="49"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+      <c r="AB32"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="51"/>
+      <c r="AF32" s="8"/>
+      <c r="AG32" s="54"/>
+      <c r="AH32" s="54"/>
+      <c r="AI32" s="54"/>
+    </row>
+    <row r="33" s="28" customFormat="1"/>
+    <row r="34" s="28" customFormat="1"/>
+    <row r="35" s="28" customFormat="1"/>
+    <row r="36" s="28" customFormat="1"/>
+    <row r="37" s="28" customFormat="1"/>
+    <row r="38" s="28" customFormat="1"/>
+    <row r="39" s="28" customFormat="1"/>
+    <row r="40" s="28" customFormat="1"/>
+    <row r="41" s="28" customFormat="1"/>
+    <row r="42" s="28" customFormat="1"/>
+    <row r="43" s="28" customFormat="1"/>
+    <row r="44" s="28" customFormat="1"/>
+    <row r="45" s="28" customFormat="1"/>
+    <row r="46" s="28" customFormat="1"/>
+    <row r="47" s="28" customFormat="1"/>
+    <row r="48" s="28" customFormat="1"/>
+    <row r="49" spans="2:2" s="28" customFormat="1"/>
+    <row r="50" spans="2:2" s="28" customFormat="1"/>
+    <row r="51" spans="2:2" s="28" customFormat="1"/>
+    <row r="52" spans="2:2" s="28" customFormat="1"/>
+    <row r="53" spans="2:2" s="28" customFormat="1"/>
+    <row r="54" spans="2:2" s="28" customFormat="1"/>
+    <row r="55" spans="2:2" s="28" customFormat="1"/>
+    <row r="56" spans="2:2" s="28" customFormat="1"/>
+    <row r="57" spans="2:2" s="28" customFormat="1"/>
+    <row r="58" spans="2:2" s="28" customFormat="1"/>
+    <row r="59" spans="2:2" s="28" customFormat="1"/>
+    <row r="60" spans="2:2" s="28" customFormat="1"/>
+    <row r="61" spans="2:2" s="28" customFormat="1"/>
+    <row r="62" spans="2:2" s="28" customFormat="1"/>
+    <row r="63" spans="2:2">
+      <c r="B63" s="28"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="28"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A28:B28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL70"/>
   <sheetViews>
@@ -2555,7 +3195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH43"/>
   <sheetViews>
@@ -2982,7 +3622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
@@ -3577,7 +4217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AL220"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Installing framework and random agent to dev
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C71AFA-89E7-3442-8334-B1A9A5C2F024}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB897A45-85BD-1043-9297-ADF09200AFF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="460" windowWidth="18680" windowHeight="35540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
-    <sheet name="Project Proposal - to print" sheetId="8" r:id="rId2"/>
+    <sheet name="PreProject Proposal - to print" sheetId="8" r:id="rId2"/>
     <sheet name="Dissertation - Old" sheetId="4" r:id="rId3"/>
     <sheet name="Original - Old" sheetId="1" r:id="rId4"/>
     <sheet name="Interim Report - Old" sheetId="3" r:id="rId5"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="101">
   <si>
     <t>Week</t>
   </si>
@@ -339,6 +339,15 @@
   </si>
   <si>
     <t>R4</t>
+  </si>
+  <si>
+    <t>Install GVGAI Framework</t>
+  </si>
+  <si>
+    <t>Implement Random Agent</t>
+  </si>
+  <si>
+    <t>Can Start working this week as the deadline is on Monday</t>
   </si>
 </sst>
 </file>
@@ -618,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -697,6 +706,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -727,14 +744,14 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,13 +1038,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM65"/>
+  <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1203,10 +1220,10 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="17" thickTop="1">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="61"/>
       <c r="G3" s="49"/>
       <c r="M3" s="49"/>
       <c r="AE3" s="49"/>
@@ -1250,7 +1267,7 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="24"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="50"/>
       <c r="M6" s="49"/>
       <c r="AE6" s="49"/>
@@ -1301,7 +1318,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51"/>
-      <c r="K9" s="69"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="7"/>
       <c r="M9" s="49"/>
       <c r="AE9" s="49"/>
@@ -1340,10 +1357,10 @@
       <c r="AG11" s="28"/>
     </row>
     <row r="12" spans="1:36">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="63"/>
       <c r="G12" s="49"/>
       <c r="M12" s="49"/>
       <c r="AE12" s="49"/>
@@ -1388,8 +1405,8 @@
         <v>89</v>
       </c>
       <c r="G15" s="49"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
       <c r="M15" s="49"/>
       <c r="AE15" s="49"/>
       <c r="AG15" s="28"/>
@@ -1409,137 +1426,136 @@
       <c r="AG16" s="28"/>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="61"/>
+      <c r="B17" s="65"/>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
       <c r="AE17" s="49"/>
       <c r="AG17" s="28"/>
     </row>
     <row r="18" spans="1:39">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="49"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="10"/>
       <c r="M18" s="49"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
       <c r="AE18" s="49"/>
       <c r="AG18" s="28"/>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="63"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="71" t="s">
+        <v>99</v>
+      </c>
       <c r="G19" s="49"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
       <c r="M19" s="49"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
       <c r="AE19" s="49"/>
       <c r="AG19" s="28"/>
     </row>
     <row r="20" spans="1:39">
       <c r="A20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>91</v>
+        <v>61</v>
+      </c>
+      <c r="B20" s="53" t="s">
+        <v>86</v>
       </c>
       <c r="G20" s="49"/>
       <c r="M20" s="49"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
       <c r="AE20" s="49"/>
       <c r="AG20" s="28"/>
-      <c r="AH20" s="52"/>
-      <c r="AI20" s="52"/>
     </row>
     <row r="21" spans="1:39">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>52</v>
-      </c>
+      <c r="A21" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="67"/>
       <c r="G21" s="49"/>
       <c r="M21" s="49"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
       <c r="AE21" s="49"/>
       <c r="AG21" s="28"/>
-      <c r="AH21" s="52"/>
-      <c r="AI21" s="52"/>
     </row>
     <row r="22" spans="1:39">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" s="44" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="G22" s="49"/>
       <c r="M22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AG22" s="28"/>
-      <c r="AJ22" s="52"/>
+      <c r="AH22" s="52"/>
+      <c r="AI22" s="52"/>
     </row>
     <row r="23" spans="1:39">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B23" s="44" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="G23" s="49"/>
       <c r="M23" s="49"/>
       <c r="AE23" s="49"/>
       <c r="AG23" s="28"/>
-      <c r="AJ23" s="52"/>
+      <c r="AH23" s="52"/>
+      <c r="AI23" s="52"/>
     </row>
     <row r="24" spans="1:39">
-      <c r="A24" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="65"/>
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>41</v>
+      </c>
       <c r="G24" s="49"/>
       <c r="M24" s="49"/>
       <c r="AE24" s="49"/>
       <c r="AG24" s="28"/>
+      <c r="AJ24" s="52"/>
     </row>
     <row r="25" spans="1:39">
       <c r="A25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>75</v>
+      </c>
       <c r="G25" s="49"/>
       <c r="M25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AG25" s="28"/>
+      <c r="AJ25" s="52"/>
     </row>
     <row r="26" spans="1:39">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="12"/>
+      <c r="A26" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="69"/>
       <c r="G26" s="49"/>
       <c r="M26" s="49"/>
       <c r="AE26" s="49"/>
@@ -1547,28 +1563,25 @@
     </row>
     <row r="27" spans="1:39">
       <c r="A27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>72</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="12"/>
       <c r="G27" s="49"/>
       <c r="M27" s="49"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="AC27" s="24"/>
-      <c r="AD27" s="24"/>
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
-      <c r="AJ27" s="12"/>
     </row>
     <row r="28" spans="1:39">
-      <c r="A28" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="67"/>
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="12"/>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
       <c r="AE28" s="49"/>
@@ -1576,103 +1589,55 @@
     </row>
     <row r="29" spans="1:39">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+        <v>72</v>
+      </c>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="AC29" s="24"/>
+      <c r="AD29" s="24"/>
       <c r="AE29" s="49"/>
       <c r="AG29" s="28"/>
-    </row>
-    <row r="30" spans="1:39" s="28" customFormat="1">
-      <c r="A30" s="28" t="s">
+      <c r="AJ29" s="12"/>
+    </row>
+    <row r="30" spans="1:39">
+      <c r="A30" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="59"/>
+      <c r="G30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="AE30" s="49"/>
+      <c r="AG30" s="28"/>
+    </row>
+    <row r="31" spans="1:39">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="G31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="AE31" s="49"/>
+      <c r="AG31" s="28"/>
+    </row>
+    <row r="32" spans="1:39" s="28" customFormat="1">
+      <c r="A32" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B32" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30" s="49"/>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30" s="49"/>
-      <c r="N30"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30"/>
-      <c r="T30"/>
-      <c r="U30"/>
-      <c r="V30"/>
-      <c r="W30"/>
-      <c r="X30"/>
-      <c r="Y30"/>
-      <c r="Z30"/>
-      <c r="AA30"/>
-      <c r="AB30"/>
-      <c r="AC30"/>
-      <c r="AD30"/>
-      <c r="AE30" s="49"/>
-      <c r="AF30"/>
-      <c r="AM30" s="39"/>
-    </row>
-    <row r="31" spans="1:39" s="28" customFormat="1">
-      <c r="A31" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31" s="49"/>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31" s="49"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31"/>
-      <c r="V31"/>
-      <c r="W31"/>
-      <c r="X31"/>
-      <c r="Y31"/>
-      <c r="Z31"/>
-      <c r="AA31"/>
-      <c r="AB31"/>
-      <c r="AC31"/>
-      <c r="AD31"/>
-      <c r="AE31" s="49"/>
-      <c r="AF31"/>
-    </row>
-    <row r="32" spans="1:39" s="28" customFormat="1">
-      <c r="A32" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32"/>
+      <c r="C32" s="9"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
@@ -1684,10 +1649,10 @@
       <c r="L32"/>
       <c r="M32" s="49"/>
       <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
       <c r="S32"/>
       <c r="T32"/>
       <c r="U32"/>
@@ -1698,61 +1663,138 @@
       <c r="Z32"/>
       <c r="AA32"/>
       <c r="AB32"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="51"/>
-      <c r="AF32" s="8"/>
-      <c r="AG32" s="54"/>
-      <c r="AH32" s="54"/>
-      <c r="AI32" s="54"/>
-    </row>
-    <row r="33" s="28" customFormat="1"/>
-    <row r="34" s="28" customFormat="1"/>
-    <row r="35" s="28" customFormat="1"/>
-    <row r="36" s="28" customFormat="1"/>
-    <row r="37" s="28" customFormat="1"/>
-    <row r="38" s="28" customFormat="1"/>
-    <row r="39" s="28" customFormat="1"/>
-    <row r="40" s="28" customFormat="1"/>
-    <row r="41" s="28" customFormat="1"/>
-    <row r="42" s="28" customFormat="1"/>
-    <row r="43" s="28" customFormat="1"/>
-    <row r="44" s="28" customFormat="1"/>
-    <row r="45" s="28" customFormat="1"/>
-    <row r="46" s="28" customFormat="1"/>
-    <row r="47" s="28" customFormat="1"/>
-    <row r="48" s="28" customFormat="1"/>
-    <row r="49" spans="2:2" s="28" customFormat="1"/>
-    <row r="50" spans="2:2" s="28" customFormat="1"/>
-    <row r="51" spans="2:2" s="28" customFormat="1"/>
-    <row r="52" spans="2:2" s="28" customFormat="1"/>
-    <row r="53" spans="2:2" s="28" customFormat="1"/>
-    <row r="54" spans="2:2" s="28" customFormat="1"/>
-    <row r="55" spans="2:2" s="28" customFormat="1"/>
-    <row r="56" spans="2:2" s="28" customFormat="1"/>
-    <row r="57" spans="2:2" s="28" customFormat="1"/>
-    <row r="58" spans="2:2" s="28" customFormat="1"/>
-    <row r="59" spans="2:2" s="28" customFormat="1"/>
-    <row r="60" spans="2:2" s="28" customFormat="1"/>
-    <row r="61" spans="2:2" s="28" customFormat="1"/>
-    <row r="62" spans="2:2" s="28" customFormat="1"/>
-    <row r="63" spans="2:2">
-      <c r="B63" s="28"/>
-    </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="28"/>
-    </row>
+      <c r="AC32"/>
+      <c r="AD32"/>
+      <c r="AE32" s="49"/>
+      <c r="AF32"/>
+      <c r="AM32" s="39"/>
+    </row>
+    <row r="33" spans="1:35" s="28" customFormat="1">
+      <c r="A33" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33" s="49"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33" s="49"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33"/>
+      <c r="AA33"/>
+      <c r="AB33"/>
+      <c r="AC33"/>
+      <c r="AD33"/>
+      <c r="AE33" s="49"/>
+      <c r="AF33"/>
+    </row>
+    <row r="34" spans="1:35" s="28" customFormat="1">
+      <c r="A34" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34" s="49"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34" s="49"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+      <c r="AC34" s="9"/>
+      <c r="AD34" s="9"/>
+      <c r="AE34" s="51"/>
+      <c r="AF34" s="8"/>
+      <c r="AG34" s="54"/>
+      <c r="AH34" s="54"/>
+      <c r="AI34" s="54"/>
+    </row>
+    <row r="35" spans="1:35" s="28" customFormat="1"/>
+    <row r="36" spans="1:35" s="28" customFormat="1"/>
+    <row r="37" spans="1:35" s="28" customFormat="1"/>
+    <row r="38" spans="1:35" s="28" customFormat="1"/>
+    <row r="39" spans="1:35" s="28" customFormat="1"/>
+    <row r="40" spans="1:35" s="28" customFormat="1"/>
+    <row r="41" spans="1:35" s="28" customFormat="1"/>
+    <row r="42" spans="1:35" s="28" customFormat="1"/>
+    <row r="43" spans="1:35" s="28" customFormat="1"/>
+    <row r="44" spans="1:35" s="28" customFormat="1"/>
+    <row r="45" spans="1:35" s="28" customFormat="1"/>
+    <row r="46" spans="1:35" s="28" customFormat="1"/>
+    <row r="47" spans="1:35" s="28" customFormat="1"/>
+    <row r="48" spans="1:35" s="28" customFormat="1"/>
+    <row r="49" s="28" customFormat="1"/>
+    <row r="50" s="28" customFormat="1"/>
+    <row r="51" s="28" customFormat="1"/>
+    <row r="52" s="28" customFormat="1"/>
+    <row r="53" s="28" customFormat="1"/>
+    <row r="54" s="28" customFormat="1"/>
+    <row r="55" s="28" customFormat="1"/>
+    <row r="56" s="28" customFormat="1"/>
+    <row r="57" s="28" customFormat="1"/>
+    <row r="58" s="28" customFormat="1"/>
+    <row r="59" s="28" customFormat="1"/>
+    <row r="60" s="28" customFormat="1"/>
+    <row r="61" s="28" customFormat="1"/>
+    <row r="62" s="28" customFormat="1"/>
+    <row r="63" s="28" customFormat="1"/>
+    <row r="64" s="28" customFormat="1"/>
     <row r="65" spans="2:2">
       <c r="B65" s="28"/>
     </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="28"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="28"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1761,13 +1803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9D7B89-5ABB-3F4A-8359-7BEAEA14AC00}">
-  <dimension ref="A1:AM65"/>
+  <dimension ref="A1:AM99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1780,7 +1819,7 @@
     <col min="37" max="37" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="131">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="131">
       <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
@@ -1803,36 +1842,8 @@
       <c r="M1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" ht="17" thickBot="1">
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1">
       <c r="A2" s="55" t="s">
         <v>54</v>
       </c>
@@ -1872,87 +1883,16 @@
       <c r="M2" s="48">
         <v>43437</v>
       </c>
-      <c r="N2" s="46">
-        <v>43444</v>
-      </c>
-      <c r="O2" s="46">
-        <v>43451</v>
-      </c>
-      <c r="P2" s="46">
-        <v>43458</v>
-      </c>
-      <c r="Q2" s="46">
-        <v>43465</v>
-      </c>
-      <c r="R2" s="46">
-        <v>43472</v>
-      </c>
-      <c r="S2" s="46">
-        <v>43479</v>
-      </c>
-      <c r="T2" s="46">
-        <v>43486</v>
-      </c>
-      <c r="U2" s="46">
-        <v>43493</v>
-      </c>
-      <c r="V2" s="46">
-        <v>43500</v>
-      </c>
-      <c r="W2" s="46">
-        <v>43507</v>
-      </c>
-      <c r="X2" s="46">
-        <v>43514</v>
-      </c>
-      <c r="Y2" s="46">
-        <v>43521</v>
-      </c>
-      <c r="Z2" s="46">
-        <v>43528</v>
-      </c>
-      <c r="AA2" s="46">
-        <v>43535</v>
-      </c>
-      <c r="AB2" s="46">
-        <v>43542</v>
-      </c>
-      <c r="AC2" s="46">
-        <v>43549</v>
-      </c>
-      <c r="AD2" s="46">
-        <v>43556</v>
-      </c>
-      <c r="AE2" s="48">
-        <v>43563</v>
-      </c>
-      <c r="AF2" s="46">
-        <v>43570</v>
-      </c>
-      <c r="AG2" s="46">
-        <v>43577</v>
-      </c>
-      <c r="AH2" s="46">
-        <v>43584</v>
-      </c>
-      <c r="AI2" s="46">
-        <v>43591</v>
-      </c>
-      <c r="AJ2" s="46">
-        <v>43598</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" ht="17" thickTop="1">
-      <c r="A3" s="56" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="17" thickTop="1">
+      <c r="A3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="61"/>
       <c r="G3" s="49"/>
       <c r="M3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AG3" s="28"/>
-    </row>
-    <row r="4" spans="1:36">
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1963,10 +1903,8 @@
       <c r="E4" s="7"/>
       <c r="G4" s="49"/>
       <c r="M4" s="49"/>
-      <c r="AE4" s="49"/>
-      <c r="AG4" s="28"/>
-    </row>
-    <row r="5" spans="1:36">
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1978,10 +1916,8 @@
       <c r="F5" s="7"/>
       <c r="G5" s="50"/>
       <c r="M5" s="49"/>
-      <c r="AE5" s="49"/>
-      <c r="AG5" s="28"/>
-    </row>
-    <row r="6" spans="1:36">
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1993,10 +1929,8 @@
       <c r="F6" s="24"/>
       <c r="G6" s="50"/>
       <c r="M6" s="49"/>
-      <c r="AE6" s="49"/>
-      <c r="AG6" s="28"/>
-    </row>
-    <row r="7" spans="1:36">
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -2009,10 +1943,8 @@
       <c r="G7" s="51"/>
       <c r="I7" s="7"/>
       <c r="M7" s="49"/>
-      <c r="AE7" s="49"/>
-      <c r="AG7" s="28"/>
-    </row>
-    <row r="8" spans="1:36">
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2027,10 +1959,8 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="M8" s="49"/>
-      <c r="AE8" s="49"/>
-      <c r="AG8" s="28"/>
-    </row>
-    <row r="9" spans="1:36">
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -2041,13 +1971,11 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51"/>
-      <c r="K9" s="69"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="7"/>
       <c r="M9" s="49"/>
-      <c r="AE9" s="49"/>
-      <c r="AG9" s="28"/>
-    </row>
-    <row r="10" spans="1:36">
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -2059,10 +1987,8 @@
       <c r="F10" s="9"/>
       <c r="G10" s="51"/>
       <c r="M10" s="50"/>
-      <c r="AE10" s="49"/>
-      <c r="AG10" s="28"/>
-    </row>
-    <row r="11" spans="1:36">
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -2071,25 +1997,16 @@
       </c>
       <c r="G11" s="49"/>
       <c r="M11" s="49"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
-      <c r="AE11" s="50"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="28"/>
-    </row>
-    <row r="12" spans="1:36">
-      <c r="A12" s="58" t="s">
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="63"/>
       <c r="G12" s="49"/>
       <c r="M12" s="49"/>
-      <c r="AE12" s="49"/>
-      <c r="AG12" s="28"/>
-    </row>
-    <row r="13" spans="1:36">
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2101,10 +2018,8 @@
       <c r="F13" s="11"/>
       <c r="G13" s="49"/>
       <c r="M13" s="49"/>
-      <c r="AE13" s="49"/>
-      <c r="AG13" s="28"/>
-    </row>
-    <row r="14" spans="1:36">
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -2117,10 +2032,8 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="M14" s="49"/>
-      <c r="AE14" s="49"/>
-      <c r="AG14" s="28"/>
-    </row>
-    <row r="15" spans="1:36">
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -2128,13 +2041,11 @@
         <v>89</v>
       </c>
       <c r="G15" s="49"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
       <c r="M15" s="49"/>
-      <c r="AE15" s="49"/>
-      <c r="AG15" s="28"/>
-    </row>
-    <row r="16" spans="1:36">
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -2145,18 +2056,14 @@
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="M16" s="49"/>
-      <c r="AE16" s="49"/>
-      <c r="AG16" s="28"/>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="61"/>
+      <c r="B17" s="65"/>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
-      <c r="AE17" s="49"/>
-      <c r="AG17" s="28"/>
     </row>
     <row r="18" spans="1:39">
       <c r="A18" t="s">
@@ -2167,33 +2074,14 @@
       </c>
       <c r="G18" s="49"/>
       <c r="M18" s="49"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AE18" s="49"/>
-      <c r="AG18" s="28"/>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="67"/>
       <c r="G19" s="49"/>
       <c r="M19" s="49"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="AE19" s="49"/>
-      <c r="AG19" s="28"/>
     </row>
     <row r="20" spans="1:39">
       <c r="A20" t="s">
@@ -2204,10 +2092,6 @@
       </c>
       <c r="G20" s="49"/>
       <c r="M20" s="49"/>
-      <c r="AE20" s="49"/>
-      <c r="AG20" s="28"/>
-      <c r="AH20" s="52"/>
-      <c r="AI20" s="52"/>
     </row>
     <row r="21" spans="1:39">
       <c r="A21" t="s">
@@ -2218,10 +2102,6 @@
       </c>
       <c r="G21" s="49"/>
       <c r="M21" s="49"/>
-      <c r="AE21" s="49"/>
-      <c r="AG21" s="28"/>
-      <c r="AH21" s="52"/>
-      <c r="AI21" s="52"/>
     </row>
     <row r="22" spans="1:39">
       <c r="A22" t="s">
@@ -2232,9 +2112,6 @@
       </c>
       <c r="G22" s="49"/>
       <c r="M22" s="49"/>
-      <c r="AE22" s="49"/>
-      <c r="AG22" s="28"/>
-      <c r="AJ22" s="52"/>
     </row>
     <row r="23" spans="1:39">
       <c r="A23" t="s">
@@ -2245,19 +2122,14 @@
       </c>
       <c r="G23" s="49"/>
       <c r="M23" s="49"/>
-      <c r="AE23" s="49"/>
-      <c r="AG23" s="28"/>
-      <c r="AJ23" s="52"/>
     </row>
     <row r="24" spans="1:39">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="65"/>
+      <c r="B24" s="69"/>
       <c r="G24" s="49"/>
       <c r="M24" s="49"/>
-      <c r="AE24" s="49"/>
-      <c r="AG24" s="28"/>
     </row>
     <row r="25" spans="1:39">
       <c r="A25" t="s">
@@ -2269,8 +2141,6 @@
       <c r="D25" s="12"/>
       <c r="G25" s="49"/>
       <c r="M25" s="49"/>
-      <c r="AE25" s="49"/>
-      <c r="AG25" s="28"/>
     </row>
     <row r="26" spans="1:39">
       <c r="A26" t="s">
@@ -2282,8 +2152,6 @@
       <c r="D26" s="12"/>
       <c r="G26" s="49"/>
       <c r="M26" s="49"/>
-      <c r="AE26" s="49"/>
-      <c r="AG26" s="28"/>
     </row>
     <row r="27" spans="1:39">
       <c r="A27" t="s">
@@ -2294,25 +2162,14 @@
       </c>
       <c r="G27" s="49"/>
       <c r="M27" s="49"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="AC27" s="24"/>
-      <c r="AD27" s="24"/>
-      <c r="AE27" s="49"/>
-      <c r="AG27" s="28"/>
-      <c r="AJ27" s="12"/>
     </row>
     <row r="28" spans="1:39">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="67"/>
+      <c r="B28" s="59"/>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
-      <c r="AE28" s="49"/>
-      <c r="AG28" s="28"/>
     </row>
     <row r="29" spans="1:39">
       <c r="A29" t="s">
@@ -2325,8 +2182,6 @@
       <c r="D29" s="8"/>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
-      <c r="AE29" s="49"/>
-      <c r="AG29" s="28"/>
     </row>
     <row r="30" spans="1:39" s="28" customFormat="1">
       <c r="A30" s="28" t="s">
@@ -2346,25 +2201,6 @@
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30" s="49"/>
-      <c r="N30"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30"/>
-      <c r="T30"/>
-      <c r="U30"/>
-      <c r="V30"/>
-      <c r="W30"/>
-      <c r="X30"/>
-      <c r="Y30"/>
-      <c r="Z30"/>
-      <c r="AA30"/>
-      <c r="AB30"/>
-      <c r="AC30"/>
-      <c r="AD30"/>
-      <c r="AE30" s="49"/>
-      <c r="AF30"/>
       <c r="AM30" s="39"/>
     </row>
     <row r="31" spans="1:39" s="28" customFormat="1">
@@ -2385,25 +2221,6 @@
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31" s="49"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31"/>
-      <c r="V31"/>
-      <c r="W31"/>
-      <c r="X31"/>
-      <c r="Y31"/>
-      <c r="Z31"/>
-      <c r="AA31"/>
-      <c r="AB31"/>
-      <c r="AC31"/>
-      <c r="AD31"/>
-      <c r="AE31" s="49"/>
-      <c r="AF31"/>
     </row>
     <row r="32" spans="1:39" s="28" customFormat="1">
       <c r="A32" s="24" t="s">
@@ -2423,79 +2240,1043 @@
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32" s="49"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="51"/>
-      <c r="AF32" s="8"/>
-      <c r="AG32" s="54"/>
-      <c r="AH32" s="54"/>
-      <c r="AI32" s="54"/>
-    </row>
-    <row r="33" s="28" customFormat="1"/>
-    <row r="34" s="28" customFormat="1"/>
-    <row r="35" s="28" customFormat="1"/>
-    <row r="36" s="28" customFormat="1"/>
-    <row r="37" s="28" customFormat="1"/>
-    <row r="38" s="28" customFormat="1"/>
-    <row r="39" s="28" customFormat="1"/>
-    <row r="40" s="28" customFormat="1"/>
-    <row r="41" s="28" customFormat="1"/>
-    <row r="42" s="28" customFormat="1"/>
-    <row r="43" s="28" customFormat="1"/>
-    <row r="44" s="28" customFormat="1"/>
-    <row r="45" s="28" customFormat="1"/>
-    <row r="46" s="28" customFormat="1"/>
-    <row r="47" s="28" customFormat="1"/>
-    <row r="48" s="28" customFormat="1"/>
-    <row r="49" spans="2:2" s="28" customFormat="1"/>
-    <row r="50" spans="2:2" s="28" customFormat="1"/>
-    <row r="51" spans="2:2" s="28" customFormat="1"/>
-    <row r="52" spans="2:2" s="28" customFormat="1"/>
-    <row r="53" spans="2:2" s="28" customFormat="1"/>
-    <row r="54" spans="2:2" s="28" customFormat="1"/>
-    <row r="55" spans="2:2" s="28" customFormat="1"/>
-    <row r="56" spans="2:2" s="28" customFormat="1"/>
-    <row r="57" spans="2:2" s="28" customFormat="1"/>
-    <row r="58" spans="2:2" s="28" customFormat="1"/>
-    <row r="59" spans="2:2" s="28" customFormat="1"/>
-    <row r="60" spans="2:2" s="28" customFormat="1"/>
-    <row r="61" spans="2:2" s="28" customFormat="1"/>
-    <row r="62" spans="2:2" s="28" customFormat="1"/>
-    <row r="63" spans="2:2">
-      <c r="B63" s="28"/>
-    </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="28"/>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="28"/>
+    </row>
+    <row r="33" spans="1:13" s="28" customFormat="1"/>
+    <row r="34" spans="1:13" s="28" customFormat="1" ht="92" customHeight="1">
+      <c r="A34" s="1"/>
+      <c r="B34" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+    </row>
+    <row r="35" spans="1:13" s="28" customFormat="1" ht="17" thickBot="1">
+      <c r="A35" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="46">
+        <v>43444</v>
+      </c>
+      <c r="D35" s="46">
+        <v>43451</v>
+      </c>
+      <c r="E35" s="46">
+        <v>43458</v>
+      </c>
+      <c r="F35" s="46">
+        <v>43465</v>
+      </c>
+      <c r="G35" s="46">
+        <v>43472</v>
+      </c>
+      <c r="H35" s="46">
+        <v>43479</v>
+      </c>
+      <c r="I35" s="46">
+        <v>43486</v>
+      </c>
+      <c r="J35" s="46">
+        <v>43493</v>
+      </c>
+      <c r="K35" s="46">
+        <v>43500</v>
+      </c>
+      <c r="L35" s="46">
+        <v>43507</v>
+      </c>
+      <c r="M35" s="46">
+        <v>43514</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="28" customFormat="1" ht="17" thickTop="1">
+      <c r="A36" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="61"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="1:13" s="28" customFormat="1">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:13" s="28" customFormat="1">
+      <c r="A38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="1:13" s="28" customFormat="1">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="1:13" s="28" customFormat="1">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="1:13" s="28" customFormat="1">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+    </row>
+    <row r="42" spans="1:13" s="28" customFormat="1">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+    </row>
+    <row r="43" spans="1:13" s="28" customFormat="1">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+    </row>
+    <row r="44" spans="1:13" s="28" customFormat="1">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+    </row>
+    <row r="45" spans="1:13" s="28" customFormat="1">
+      <c r="A45" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="63"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+    </row>
+    <row r="46" spans="1:13" s="28" customFormat="1">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+    </row>
+    <row r="47" spans="1:13" s="28" customFormat="1">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+    </row>
+    <row r="48" spans="1:13" s="28" customFormat="1">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+    </row>
+    <row r="49" spans="1:13" s="28" customFormat="1">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+    </row>
+    <row r="50" spans="1:13" s="28" customFormat="1">
+      <c r="A50" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="65"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+    </row>
+    <row r="51" spans="1:13" s="28" customFormat="1">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+    </row>
+    <row r="52" spans="1:13" s="28" customFormat="1">
+      <c r="A52" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="67"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52"/>
+      <c r="M52"/>
+    </row>
+    <row r="53" spans="1:13" s="28" customFormat="1">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+    </row>
+    <row r="54" spans="1:13" s="28" customFormat="1">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+    </row>
+    <row r="55" spans="1:13" s="28" customFormat="1">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+    </row>
+    <row r="56" spans="1:13" s="28" customFormat="1">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+    </row>
+    <row r="57" spans="1:13" s="28" customFormat="1">
+      <c r="A57" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="69"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+    </row>
+    <row r="58" spans="1:13" s="28" customFormat="1">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+    </row>
+    <row r="59" spans="1:13" s="28" customFormat="1">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+    </row>
+    <row r="60" spans="1:13" s="28" customFormat="1">
+      <c r="A60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+    </row>
+    <row r="61" spans="1:13" s="28" customFormat="1">
+      <c r="A61" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="59"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+    </row>
+    <row r="62" spans="1:13" s="28" customFormat="1">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="M63"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="M64"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="M65"/>
+    </row>
+    <row r="67" spans="1:14" ht="75">
+      <c r="A67" s="1"/>
+      <c r="B67" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="40"/>
+      <c r="I67" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="J67" s="40"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="40"/>
+      <c r="M67" s="40"/>
+      <c r="N67" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="17" thickBot="1">
+      <c r="A68" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="46">
+        <v>43521</v>
+      </c>
+      <c r="D68" s="46">
+        <v>43528</v>
+      </c>
+      <c r="E68" s="46">
+        <v>43535</v>
+      </c>
+      <c r="F68" s="46">
+        <v>43542</v>
+      </c>
+      <c r="G68" s="46">
+        <v>43549</v>
+      </c>
+      <c r="H68" s="46">
+        <v>43556</v>
+      </c>
+      <c r="I68" s="48">
+        <v>43563</v>
+      </c>
+      <c r="J68" s="46">
+        <v>43570</v>
+      </c>
+      <c r="K68" s="46">
+        <v>43577</v>
+      </c>
+      <c r="L68" s="46">
+        <v>43584</v>
+      </c>
+      <c r="M68" s="46">
+        <v>43591</v>
+      </c>
+      <c r="N68" s="46">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="17" thickTop="1">
+      <c r="A69" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="61"/>
+      <c r="I69" s="49"/>
+      <c r="K69" s="28"/>
+      <c r="M69"/>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="I70" s="49"/>
+      <c r="K70" s="28"/>
+      <c r="M70"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I71" s="49"/>
+      <c r="K71" s="28"/>
+      <c r="M71"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B72" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="I72" s="49"/>
+      <c r="K72" s="28"/>
+      <c r="M72"/>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B73" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="I73" s="49"/>
+      <c r="K73" s="28"/>
+      <c r="M73"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="I74" s="49"/>
+      <c r="K74" s="28"/>
+      <c r="M74"/>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="I75" s="49"/>
+      <c r="K75" s="28"/>
+      <c r="M75"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" t="s">
+        <v>85</v>
+      </c>
+      <c r="B76" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="I76" s="49"/>
+      <c r="K76" s="28"/>
+      <c r="M76"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="50"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="28"/>
+      <c r="M77"/>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="A78" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" s="63"/>
+      <c r="I78" s="49"/>
+      <c r="K78" s="28"/>
+      <c r="M78"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B79" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="I79" s="49"/>
+      <c r="K79" s="28"/>
+      <c r="M79"/>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="I80" s="49"/>
+      <c r="K80" s="28"/>
+      <c r="M80"/>
+    </row>
+    <row r="81" spans="1:14">
+      <c r="A81" t="s">
+        <v>96</v>
+      </c>
+      <c r="B81" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="I81" s="49"/>
+      <c r="K81" s="28"/>
+      <c r="M81"/>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="A82" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="I82" s="49"/>
+      <c r="K82" s="28"/>
+      <c r="M82"/>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="65"/>
+      <c r="I83" s="49"/>
+      <c r="K83" s="28"/>
+      <c r="M83"/>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="I84" s="49"/>
+      <c r="K84" s="28"/>
+      <c r="M84"/>
+    </row>
+    <row r="85" spans="1:14">
+      <c r="A85" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B85" s="67"/>
+      <c r="I85" s="49"/>
+      <c r="K85" s="28"/>
+      <c r="M85"/>
+    </row>
+    <row r="86" spans="1:14">
+      <c r="A86" t="s">
+        <v>62</v>
+      </c>
+      <c r="B86" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="I86" s="49"/>
+      <c r="K86" s="28"/>
+      <c r="L86" s="52"/>
+      <c r="M86" s="52"/>
+    </row>
+    <row r="87" spans="1:14">
+      <c r="A87" t="s">
+        <v>63</v>
+      </c>
+      <c r="B87" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="I87" s="49"/>
+      <c r="K87" s="28"/>
+      <c r="L87" s="52"/>
+      <c r="M87" s="52"/>
+    </row>
+    <row r="88" spans="1:14">
+      <c r="A88" t="s">
+        <v>64</v>
+      </c>
+      <c r="B88" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="I88" s="49"/>
+      <c r="K88" s="28"/>
+      <c r="M88"/>
+      <c r="N88" s="52"/>
+    </row>
+    <row r="89" spans="1:14">
+      <c r="A89" t="s">
+        <v>74</v>
+      </c>
+      <c r="B89" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="I89" s="49"/>
+      <c r="K89" s="28"/>
+      <c r="M89"/>
+      <c r="N89" s="52"/>
+    </row>
+    <row r="90" spans="1:14">
+      <c r="A90" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" s="69"/>
+      <c r="I90" s="49"/>
+      <c r="K90" s="28"/>
+      <c r="M90"/>
+    </row>
+    <row r="91" spans="1:14">
+      <c r="A91" t="s">
+        <v>65</v>
+      </c>
+      <c r="B91" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="I91" s="49"/>
+      <c r="K91" s="28"/>
+      <c r="M91"/>
+    </row>
+    <row r="92" spans="1:14">
+      <c r="A92" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="I92" s="49"/>
+      <c r="K92" s="28"/>
+      <c r="M92"/>
+    </row>
+    <row r="93" spans="1:14">
+      <c r="A93" t="s">
+        <v>67</v>
+      </c>
+      <c r="B93" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="49"/>
+      <c r="K93" s="28"/>
+      <c r="M93"/>
+      <c r="N93" s="12"/>
+    </row>
+    <row r="94" spans="1:14">
+      <c r="A94" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B94" s="59"/>
+      <c r="I94" s="49"/>
+      <c r="K94" s="28"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:14">
+      <c r="A95" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I95" s="49"/>
+      <c r="K95" s="28"/>
+      <c r="M95"/>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="A96" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I96" s="49"/>
+      <c r="K96" s="28"/>
+      <c r="L96" s="28"/>
+      <c r="N96" s="28"/>
+    </row>
+    <row r="97" spans="1:14">
+      <c r="A97" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" s="49"/>
+      <c r="K97" s="28"/>
+      <c r="L97" s="28"/>
+      <c r="N97" s="28"/>
+    </row>
+    <row r="98" spans="1:14">
+      <c r="A98" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B98" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="51"/>
+      <c r="J98" s="8"/>
+      <c r="K98" s="54"/>
+      <c r="L98" s="54"/>
+      <c r="M98" s="54"/>
+      <c r="N98" s="28"/>
+    </row>
+    <row r="99" spans="1:14">
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="28"/>
+      <c r="I99" s="28"/>
+      <c r="J99" s="28"/>
+      <c r="K99" s="28"/>
+      <c r="L99" s="28"/>
+      <c r="N99" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="18">
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A90:B90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added reminder for meeting minutes file
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB897A45-85BD-1043-9297-ADF09200AFF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382C2FC8-1D62-8947-AD08-7137D327C989}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="102">
   <si>
     <t>Week</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Can Start working this week as the deadline is on Monday</t>
+  </si>
+  <si>
+    <t>Create meeting minutes email file thing</t>
   </si>
 </sst>
 </file>
@@ -1038,19 +1041,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM67"/>
+  <dimension ref="A1:AM68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="9.1640625" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" style="28" customWidth="1"/>
     <col min="14" max="36" width="9.1640625" customWidth="1"/>
@@ -1425,7 +1428,7 @@
       <c r="AE16" s="49"/>
       <c r="AG16" s="28"/>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:36">
       <c r="A17" s="64" t="s">
         <v>8</v>
       </c>
@@ -1435,7 +1438,7 @@
       <c r="AE17" s="49"/>
       <c r="AG17" s="28"/>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:36">
       <c r="A18" s="70"/>
       <c r="B18" s="71" t="s">
         <v>98</v>
@@ -1448,7 +1451,7 @@
       <c r="AE18" s="49"/>
       <c r="AG18" s="28"/>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:36">
       <c r="A19" s="70"/>
       <c r="B19" s="71" t="s">
         <v>99</v>
@@ -1460,7 +1463,7 @@
       <c r="AE19" s="49"/>
       <c r="AG19" s="28"/>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:36">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1485,7 +1488,7 @@
       <c r="AE20" s="49"/>
       <c r="AG20" s="28"/>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:36">
       <c r="A21" s="66" t="s">
         <v>51</v>
       </c>
@@ -1497,7 +1500,7 @@
       <c r="AE21" s="49"/>
       <c r="AG21" s="28"/>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:36">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1511,7 +1514,7 @@
       <c r="AH22" s="52"/>
       <c r="AI22" s="52"/>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:36">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1525,7 +1528,7 @@
       <c r="AH23" s="52"/>
       <c r="AI23" s="52"/>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:36">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -1538,7 +1541,7 @@
       <c r="AG24" s="28"/>
       <c r="AJ24" s="52"/>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:36">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1551,7 +1554,7 @@
       <c r="AG25" s="28"/>
       <c r="AJ25" s="52"/>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:36">
       <c r="A26" s="68" t="s">
         <v>73</v>
       </c>
@@ -1561,7 +1564,7 @@
       <c r="AE26" s="49"/>
       <c r="AG26" s="28"/>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:36">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1574,7 +1577,7 @@
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:36">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -1587,96 +1590,67 @@
       <c r="AE28" s="49"/>
       <c r="AG28" s="28"/>
     </row>
-    <row r="29" spans="1:39">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>72</v>
-      </c>
+    <row r="29" spans="1:36">
+      <c r="B29" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="9"/>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="AC29" s="24"/>
-      <c r="AD29" s="24"/>
       <c r="AE29" s="49"/>
       <c r="AG29" s="28"/>
-      <c r="AJ29" s="12"/>
-    </row>
-    <row r="30" spans="1:39">
-      <c r="A30" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="59"/>
+    </row>
+    <row r="30" spans="1:36">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="G30" s="49"/>
       <c r="M30" s="49"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="AC30" s="24"/>
+      <c r="AD30" s="24"/>
       <c r="AE30" s="49"/>
       <c r="AG30" s="28"/>
-    </row>
-    <row r="31" spans="1:39">
-      <c r="A31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="AJ30" s="12"/>
+    </row>
+    <row r="31" spans="1:36">
+      <c r="A31" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="59"/>
       <c r="G31" s="49"/>
       <c r="M31" s="49"/>
       <c r="AE31" s="49"/>
       <c r="AG31" s="28"/>
     </row>
-    <row r="32" spans="1:39" s="28" customFormat="1">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:36">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="G32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="AE32" s="49"/>
+      <c r="AG32" s="28"/>
+    </row>
+    <row r="33" spans="1:39" s="28" customFormat="1">
+      <c r="A33" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B33" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32" s="49"/>
-      <c r="H32"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32" s="49"/>
-      <c r="N32"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32" s="49"/>
-      <c r="AF32"/>
-      <c r="AM32" s="39"/>
-    </row>
-    <row r="33" spans="1:35" s="28" customFormat="1">
-      <c r="A33" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33"/>
+      <c r="C33" s="9"/>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33"/>
@@ -1688,12 +1662,12 @@
       <c r="L33"/>
       <c r="M33" s="49"/>
       <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33"/>
+      <c r="T33"/>
       <c r="U33"/>
       <c r="V33"/>
       <c r="W33"/>
@@ -1706,13 +1680,14 @@
       <c r="AD33"/>
       <c r="AE33" s="49"/>
       <c r="AF33"/>
-    </row>
-    <row r="34" spans="1:35" s="28" customFormat="1">
+      <c r="AM33" s="39"/>
+    </row>
+    <row r="34" spans="1:39" s="28" customFormat="1">
       <c r="A34" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
@@ -1730,8 +1705,8 @@
       <c r="P34"/>
       <c r="Q34"/>
       <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
       <c r="U34"/>
       <c r="V34"/>
       <c r="W34"/>
@@ -1740,28 +1715,65 @@
       <c r="Z34"/>
       <c r="AA34"/>
       <c r="AB34"/>
-      <c r="AC34" s="9"/>
-      <c r="AD34" s="9"/>
-      <c r="AE34" s="51"/>
-      <c r="AF34" s="8"/>
-      <c r="AG34" s="54"/>
-      <c r="AH34" s="54"/>
-      <c r="AI34" s="54"/>
-    </row>
-    <row r="35" spans="1:35" s="28" customFormat="1"/>
-    <row r="36" spans="1:35" s="28" customFormat="1"/>
-    <row r="37" spans="1:35" s="28" customFormat="1"/>
-    <row r="38" spans="1:35" s="28" customFormat="1"/>
-    <row r="39" spans="1:35" s="28" customFormat="1"/>
-    <row r="40" spans="1:35" s="28" customFormat="1"/>
-    <row r="41" spans="1:35" s="28" customFormat="1"/>
-    <row r="42" spans="1:35" s="28" customFormat="1"/>
-    <row r="43" spans="1:35" s="28" customFormat="1"/>
-    <row r="44" spans="1:35" s="28" customFormat="1"/>
-    <row r="45" spans="1:35" s="28" customFormat="1"/>
-    <row r="46" spans="1:35" s="28" customFormat="1"/>
-    <row r="47" spans="1:35" s="28" customFormat="1"/>
-    <row r="48" spans="1:35" s="28" customFormat="1"/>
+      <c r="AC34"/>
+      <c r="AD34"/>
+      <c r="AE34" s="49"/>
+      <c r="AF34"/>
+    </row>
+    <row r="35" spans="1:39" s="28" customFormat="1">
+      <c r="A35" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35" s="49"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35" s="49"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35" s="9"/>
+      <c r="AD35" s="9"/>
+      <c r="AE35" s="51"/>
+      <c r="AF35" s="8"/>
+      <c r="AG35" s="54"/>
+      <c r="AH35" s="54"/>
+      <c r="AI35" s="54"/>
+    </row>
+    <row r="36" spans="1:39" s="28" customFormat="1"/>
+    <row r="37" spans="1:39" s="28" customFormat="1"/>
+    <row r="38" spans="1:39" s="28" customFormat="1"/>
+    <row r="39" spans="1:39" s="28" customFormat="1"/>
+    <row r="40" spans="1:39" s="28" customFormat="1"/>
+    <row r="41" spans="1:39" s="28" customFormat="1"/>
+    <row r="42" spans="1:39" s="28" customFormat="1"/>
+    <row r="43" spans="1:39" s="28" customFormat="1"/>
+    <row r="44" spans="1:39" s="28" customFormat="1"/>
+    <row r="45" spans="1:39" s="28" customFormat="1"/>
+    <row r="46" spans="1:39" s="28" customFormat="1"/>
+    <row r="47" spans="1:39" s="28" customFormat="1"/>
+    <row r="48" spans="1:39" s="28" customFormat="1"/>
     <row r="49" s="28" customFormat="1"/>
     <row r="50" s="28" customFormat="1"/>
     <row r="51" s="28" customFormat="1"/>
@@ -1778,18 +1790,19 @@
     <row r="62" s="28" customFormat="1"/>
     <row r="63" s="28" customFormat="1"/>
     <row r="64" s="28" customFormat="1"/>
-    <row r="65" spans="2:2">
-      <c r="B65" s="28"/>
-    </row>
+    <row r="65" spans="2:2" s="28" customFormat="1"/>
     <row r="66" spans="2:2">
       <c r="B66" s="28"/>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="28"/>
     </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="28"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:B17"/>

</xml_diff>

<commit_message>
Finalised Documentation Section of workplan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382C2FC8-1D62-8947-AD08-7137D327C989}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FC52C4-9831-2B4A-A81B-F5C0A848280C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="115">
   <si>
     <t>Week</t>
   </si>
@@ -350,7 +350,46 @@
     <t>Can Start working this week as the deadline is on Monday</t>
   </si>
   <si>
-    <t>Create meeting minutes email file thing</t>
+    <t>Could move this section around maybe have it during/after research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not sure where to put this need to research to find some :) </t>
+  </si>
+  <si>
+    <t>GVGAI Framework Review</t>
+  </si>
+  <si>
+    <t>Run avalible Previous Agents</t>
+  </si>
+  <si>
+    <t>Create Meeting Document</t>
+  </si>
+  <si>
+    <t>Research Paper Structure Sections</t>
+  </si>
+  <si>
+    <t>Research Paper Abstract</t>
+  </si>
+  <si>
+    <t>Research Paper Draft</t>
+  </si>
+  <si>
+    <t>Research Paper Finalise</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>Background Research</t>
   </si>
 </sst>
 </file>
@@ -630,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -711,6 +750,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -747,14 +795,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,26 +1081,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM68"/>
+  <dimension ref="A1:AM73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="9.1640625" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" style="28" customWidth="1"/>
     <col min="14" max="36" width="9.1640625" customWidth="1"/>
     <col min="37" max="37" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="131">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="139">
       <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
@@ -1223,10 +1263,10 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="17" thickTop="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="61"/>
+      <c r="B3" s="66"/>
       <c r="G3" s="49"/>
       <c r="M3" s="49"/>
       <c r="AE3" s="49"/>
@@ -1270,8 +1310,8 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="50"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="51"/>
       <c r="M6" s="49"/>
       <c r="AE6" s="49"/>
       <c r="AG6" s="28"/>
@@ -1347,283 +1387,298 @@
         <v>93</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="G11" s="49"/>
       <c r="M11" s="49"/>
       <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
-      <c r="AE11" s="50"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="51"/>
       <c r="AF11" s="9"/>
       <c r="AG11" s="28"/>
     </row>
     <row r="12" spans="1:36">
-      <c r="A12" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="63"/>
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>107</v>
+      </c>
       <c r="G12" s="49"/>
       <c r="M12" s="49"/>
-      <c r="AE12" s="49"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="51"/>
+      <c r="AF12" s="9"/>
       <c r="AG12" s="28"/>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+        <v>111</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>108</v>
+      </c>
       <c r="G13" s="49"/>
       <c r="M13" s="49"/>
-      <c r="AE13" s="49"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="51"/>
+      <c r="AF13" s="9"/>
       <c r="AG13" s="28"/>
     </row>
     <row r="14" spans="1:36">
       <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
+        <v>112</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>109</v>
+      </c>
       <c r="G14" s="49"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
       <c r="M14" s="49"/>
-      <c r="AE14" s="49"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="50"/>
+      <c r="AF14" s="9"/>
       <c r="AG14" s="28"/>
     </row>
     <row r="15" spans="1:36">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="53" t="s">
-        <v>89</v>
-      </c>
+      <c r="A15" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="68"/>
       <c r="G15" s="49"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
       <c r="M15" s="49"/>
       <c r="AE15" s="49"/>
       <c r="AG15" s="28"/>
     </row>
     <row r="16" spans="1:36">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>90</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="49"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
       <c r="M16" s="49"/>
       <c r="AE16" s="49"/>
       <c r="AG16" s="28"/>
     </row>
     <row r="17" spans="1:36">
-      <c r="A17" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="65"/>
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
       <c r="G17" s="49"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
       <c r="M17" s="49"/>
       <c r="AE17" s="49"/>
       <c r="AG17" s="28"/>
     </row>
     <row r="18" spans="1:36">
-      <c r="A18" s="70"/>
-      <c r="B18" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="10"/>
+      <c r="B18" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
       <c r="M18" s="49"/>
       <c r="AE18" s="49"/>
       <c r="AG18" s="28"/>
     </row>
     <row r="19" spans="1:36">
-      <c r="A19" s="70"/>
-      <c r="B19" s="71" t="s">
-        <v>99</v>
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>89</v>
       </c>
       <c r="G19" s="49"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
       <c r="M19" s="49"/>
       <c r="AE19" s="49"/>
       <c r="AG19" s="28"/>
     </row>
     <row r="20" spans="1:36">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G20" s="49"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
       <c r="M20" s="49"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
       <c r="AE20" s="49"/>
       <c r="AG20" s="28"/>
     </row>
     <row r="21" spans="1:36">
-      <c r="A21" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="67"/>
+      <c r="A21" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="70"/>
       <c r="G21" s="49"/>
       <c r="M21" s="49"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
       <c r="AE21" s="49"/>
       <c r="AG21" s="28"/>
     </row>
     <row r="22" spans="1:36">
-      <c r="A22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="49"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="10"/>
       <c r="M22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AG22" s="28"/>
-      <c r="AH22" s="52"/>
-      <c r="AI22" s="52"/>
     </row>
     <row r="23" spans="1:36">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="49"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
       <c r="M23" s="49"/>
       <c r="AE23" s="49"/>
       <c r="AG23" s="28"/>
-      <c r="AH23" s="52"/>
-      <c r="AI23" s="52"/>
     </row>
     <row r="24" spans="1:36">
-      <c r="A24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="44" t="s">
-        <v>41</v>
+      <c r="A24" s="58"/>
+      <c r="B24" s="59" t="s">
+        <v>104</v>
       </c>
       <c r="G24" s="49"/>
+      <c r="H24" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" s="10"/>
       <c r="M24" s="49"/>
       <c r="AE24" s="49"/>
       <c r="AG24" s="28"/>
-      <c r="AJ24" s="52"/>
     </row>
     <row r="25" spans="1:36">
       <c r="A25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>86</v>
       </c>
       <c r="G25" s="49"/>
       <c r="M25" s="49"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
       <c r="AE25" s="49"/>
       <c r="AG25" s="28"/>
-      <c r="AJ25" s="52"/>
     </row>
     <row r="26" spans="1:36">
-      <c r="A26" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="69"/>
+      <c r="A26" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="72"/>
       <c r="G26" s="49"/>
       <c r="M26" s="49"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
       <c r="AE26" s="49"/>
       <c r="AG26" s="28"/>
     </row>
     <row r="27" spans="1:36">
       <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>91</v>
+      </c>
       <c r="G27" s="49"/>
       <c r="M27" s="49"/>
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
+      <c r="AH27" s="52"/>
+      <c r="AI27" s="52"/>
     </row>
     <row r="28" spans="1:36">
       <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>52</v>
+      </c>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
       <c r="AE28" s="49"/>
       <c r="AG28" s="28"/>
+      <c r="AH28" s="52"/>
+      <c r="AI28" s="52"/>
     </row>
     <row r="29" spans="1:36">
-      <c r="B29" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="9"/>
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>41</v>
+      </c>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
       <c r="AE29" s="49"/>
       <c r="AG29" s="28"/>
+      <c r="AJ29" s="52"/>
     </row>
     <row r="30" spans="1:36">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G30" s="49"/>
       <c r="M30" s="49"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="AC30" s="24"/>
-      <c r="AD30" s="24"/>
       <c r="AE30" s="49"/>
       <c r="AG30" s="28"/>
-      <c r="AJ30" s="12"/>
+      <c r="AJ30" s="52"/>
     </row>
     <row r="31" spans="1:36">
-      <c r="A31" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="59"/>
+      <c r="A31" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="74"/>
       <c r="G31" s="49"/>
       <c r="M31" s="49"/>
       <c r="AE31" s="49"/>
@@ -1631,141 +1686,204 @@
     </row>
     <row r="32" spans="1:36">
       <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+        <v>65</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="12"/>
       <c r="G32" s="49"/>
       <c r="M32" s="49"/>
       <c r="AE32" s="49"/>
       <c r="AG32" s="28"/>
     </row>
-    <row r="33" spans="1:39" s="28" customFormat="1">
-      <c r="A33" s="28" t="s">
+    <row r="33" spans="1:39">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="G33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="AE33" s="49"/>
+      <c r="AG33" s="28"/>
+    </row>
+    <row r="34" spans="1:39">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="G34" s="62"/>
+      <c r="M34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AG34" s="28"/>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="AC35" s="24"/>
+      <c r="AD35" s="24"/>
+      <c r="AE35" s="49"/>
+      <c r="AG35" s="28"/>
+      <c r="AJ35" s="12"/>
+    </row>
+    <row r="36" spans="1:39">
+      <c r="A36" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="64"/>
+      <c r="G36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="AE36" s="49"/>
+      <c r="AG36" s="28"/>
+    </row>
+    <row r="37" spans="1:39">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="G37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="AE37" s="49"/>
+      <c r="AG37" s="28"/>
+    </row>
+    <row r="38" spans="1:39" s="28" customFormat="1">
+      <c r="A38" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B38" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33" s="49"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33" s="49"/>
-      <c r="N33"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33" s="49"/>
-      <c r="AF33"/>
-      <c r="AM33" s="39"/>
-    </row>
-    <row r="34" spans="1:39" s="28" customFormat="1">
-      <c r="A34" s="24" t="s">
+      <c r="C38" s="9"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38" s="49"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38" s="49"/>
+      <c r="N38"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38"/>
+      <c r="AA38"/>
+      <c r="AB38"/>
+      <c r="AC38"/>
+      <c r="AD38"/>
+      <c r="AE38" s="49"/>
+      <c r="AF38"/>
+      <c r="AM38" s="39"/>
+    </row>
+    <row r="39" spans="1:39" s="28" customFormat="1">
+      <c r="A39" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B39" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34" s="49"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34" s="49"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34" s="49"/>
-      <c r="AF34"/>
-    </row>
-    <row r="35" spans="1:39" s="28" customFormat="1">
-      <c r="A35" s="24" t="s">
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39" s="49"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39" s="49"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39"/>
+      <c r="AA39"/>
+      <c r="AB39"/>
+      <c r="AC39"/>
+      <c r="AD39"/>
+      <c r="AE39" s="49"/>
+      <c r="AF39"/>
+    </row>
+    <row r="40" spans="1:39" s="28" customFormat="1">
+      <c r="A40" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B40" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35" s="49"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35" s="49"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35" s="9"/>
-      <c r="AD35" s="9"/>
-      <c r="AE35" s="51"/>
-      <c r="AF35" s="8"/>
-      <c r="AG35" s="54"/>
-      <c r="AH35" s="54"/>
-      <c r="AI35" s="54"/>
-    </row>
-    <row r="36" spans="1:39" s="28" customFormat="1"/>
-    <row r="37" spans="1:39" s="28" customFormat="1"/>
-    <row r="38" spans="1:39" s="28" customFormat="1"/>
-    <row r="39" spans="1:39" s="28" customFormat="1"/>
-    <row r="40" spans="1:39" s="28" customFormat="1"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40" s="49"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40" s="49"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+      <c r="AA40"/>
+      <c r="AB40"/>
+      <c r="AC40" s="9"/>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="51"/>
+      <c r="AF40" s="8"/>
+      <c r="AG40" s="54"/>
+      <c r="AH40" s="54"/>
+      <c r="AI40" s="54"/>
+    </row>
     <row r="41" spans="1:39" s="28" customFormat="1"/>
     <row r="42" spans="1:39" s="28" customFormat="1"/>
     <row r="43" spans="1:39" s="28" customFormat="1"/>
@@ -1791,23 +1909,28 @@
     <row r="63" s="28" customFormat="1"/>
     <row r="64" s="28" customFormat="1"/>
     <row r="65" spans="2:2" s="28" customFormat="1"/>
-    <row r="66" spans="2:2">
-      <c r="B66" s="28"/>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" s="28"/>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="28"/>
+    <row r="66" spans="2:2" s="28" customFormat="1"/>
+    <row r="67" spans="2:2" s="28" customFormat="1"/>
+    <row r="68" spans="2:2" s="28" customFormat="1"/>
+    <row r="69" spans="2:2" s="28" customFormat="1"/>
+    <row r="70" spans="2:2" s="28" customFormat="1"/>
+    <row r="71" spans="2:2">
+      <c r="B71" s="28"/>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="28"/>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1819,7 +1942,7 @@
   <dimension ref="A1:AM99"/>
   <sheetViews>
     <sheetView zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B32" sqref="A1:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1898,10 +2021,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" thickTop="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="61"/>
+      <c r="B3" s="66"/>
       <c r="G3" s="49"/>
       <c r="M3" s="49"/>
     </row>
@@ -2012,10 +2135,10 @@
       <c r="M11" s="49"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="63"/>
+      <c r="B12" s="68"/>
       <c r="G12" s="49"/>
       <c r="M12" s="49"/>
     </row>
@@ -2071,10 +2194,10 @@
       <c r="M16" s="49"/>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="65"/>
+      <c r="B17" s="70"/>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
     </row>
@@ -2089,10 +2212,10 @@
       <c r="M18" s="49"/>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="72"/>
       <c r="G19" s="49"/>
       <c r="M19" s="49"/>
     </row>
@@ -2137,10 +2260,10 @@
       <c r="M23" s="49"/>
     </row>
     <row r="24" spans="1:39">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="69"/>
+      <c r="B24" s="74"/>
       <c r="G24" s="49"/>
       <c r="M24" s="49"/>
     </row>
@@ -2177,10 +2300,10 @@
       <c r="M27" s="49"/>
     </row>
     <row r="28" spans="1:39">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="59"/>
+      <c r="B28" s="64"/>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
     </row>
@@ -2316,10 +2439,10 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="28" customFormat="1" ht="17" thickTop="1">
-      <c r="A36" s="60" t="s">
+      <c r="A36" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="61"/>
+      <c r="B36" s="66"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
@@ -2485,10 +2608,10 @@
       <c r="M44"/>
     </row>
     <row r="45" spans="1:13" s="28" customFormat="1">
-      <c r="A45" s="62" t="s">
+      <c r="A45" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="63"/>
+      <c r="B45" s="68"/>
       <c r="C45"/>
       <c r="D45"/>
       <c r="E45"/>
@@ -2578,10 +2701,10 @@
       <c r="M49"/>
     </row>
     <row r="50" spans="1:13" s="28" customFormat="1">
-      <c r="A50" s="64" t="s">
+      <c r="A50" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="65"/>
+      <c r="B50" s="70"/>
       <c r="C50"/>
       <c r="D50"/>
       <c r="E50"/>
@@ -2614,10 +2737,10 @@
       <c r="M51" s="10"/>
     </row>
     <row r="52" spans="1:13" s="28" customFormat="1">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="67"/>
+      <c r="B52" s="72"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
@@ -2707,10 +2830,10 @@
       <c r="M56"/>
     </row>
     <row r="57" spans="1:13" s="28" customFormat="1">
-      <c r="A57" s="68" t="s">
+      <c r="A57" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="69"/>
+      <c r="B57" s="74"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
@@ -2781,10 +2904,10 @@
       <c r="M60"/>
     </row>
     <row r="61" spans="1:13" s="28" customFormat="1">
-      <c r="A61" s="58" t="s">
+      <c r="A61" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="59"/>
+      <c r="B61" s="64"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
@@ -2916,10 +3039,10 @@
       </c>
     </row>
     <row r="69" spans="1:14" ht="17" thickTop="1">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="61"/>
+      <c r="B69" s="66"/>
       <c r="I69" s="49"/>
       <c r="K69" s="28"/>
       <c r="M69"/>
@@ -3018,10 +3141,10 @@
       <c r="M77"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="62" t="s">
+      <c r="A78" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="63"/>
+      <c r="B78" s="68"/>
       <c r="I78" s="49"/>
       <c r="K78" s="28"/>
       <c r="M78"/>
@@ -3071,10 +3194,10 @@
       <c r="M82"/>
     </row>
     <row r="83" spans="1:14">
-      <c r="A83" s="64" t="s">
+      <c r="A83" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="65"/>
+      <c r="B83" s="70"/>
       <c r="I83" s="49"/>
       <c r="K83" s="28"/>
       <c r="M83"/>
@@ -3093,10 +3216,10 @@
       <c r="M84"/>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="66" t="s">
+      <c r="A85" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B85" s="67"/>
+      <c r="B85" s="72"/>
       <c r="I85" s="49"/>
       <c r="K85" s="28"/>
       <c r="M85"/>
@@ -3150,10 +3273,10 @@
       <c r="N89" s="52"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="68" t="s">
+      <c r="A90" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="B90" s="69"/>
+      <c r="B90" s="74"/>
       <c r="I90" s="49"/>
       <c r="K90" s="28"/>
       <c r="M90"/>
@@ -3195,10 +3318,10 @@
       <c r="N93" s="12"/>
     </row>
     <row r="94" spans="1:14">
-      <c r="A94" s="58" t="s">
+      <c r="A94" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B94" s="59"/>
+      <c r="B94" s="64"/>
       <c r="I94" s="49"/>
       <c r="K94" s="28"/>
       <c r="M94"/>
@@ -3269,12 +3392,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A94:B94"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A45:B45"/>
@@ -3287,6 +3404,12 @@
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3997,7 +4120,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4424,7 +4547,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Added Percentage completion to work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FC52C4-9831-2B4A-A81B-F5C0A848280C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014E98BA-112D-8B49-8AD1-6A9120FA7AE7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Interim Report - Old" sheetId="3" r:id="rId5"/>
     <sheet name="Dissertation to print - Old" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="116">
   <si>
     <t>Week</t>
   </si>
@@ -347,9 +347,6 @@
     <t>Implement Random Agent</t>
   </si>
   <si>
-    <t>Can Start working this week as the deadline is on Monday</t>
-  </si>
-  <si>
     <t>Could move this section around maybe have it during/after research</t>
   </si>
   <si>
@@ -390,6 +387,12 @@
   </si>
   <si>
     <t>Background Research</t>
+  </si>
+  <si>
+    <t>Precentage Completiton</t>
+  </si>
+  <si>
+    <t>Week Number</t>
   </si>
 </sst>
 </file>
@@ -669,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -795,6 +798,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,13 +1086,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM73"/>
+  <dimension ref="A1:AM75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="180" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1100,471 +1105,694 @@
     <col min="37" max="37" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="139">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:36">
+      <c r="B1" s="76" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+      <c r="AI1">
+        <v>33</v>
+      </c>
+      <c r="AJ1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
+      <c r="B2" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="75">
+        <f>SUM(100/$AJ$1*C1)/100</f>
+        <v>2.9411764705882356E-2</v>
+      </c>
+      <c r="D2" s="75">
+        <f t="shared" ref="D2:K2" si="0">SUM(100/$AJ$1*D1)/100</f>
+        <v>5.8823529411764712E-2</v>
+      </c>
+      <c r="E2" s="75">
+        <f t="shared" si="0"/>
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="F2" s="75">
+        <f t="shared" si="0"/>
+        <v>0.11764705882352942</v>
+      </c>
+      <c r="G2" s="75">
+        <f t="shared" si="0"/>
+        <v>0.14705882352941177</v>
+      </c>
+      <c r="H2" s="75">
+        <f t="shared" si="0"/>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="I2" s="75">
+        <f t="shared" si="0"/>
+        <v>0.20588235294117649</v>
+      </c>
+      <c r="J2" s="75">
+        <f t="shared" si="0"/>
+        <v>0.23529411764705885</v>
+      </c>
+      <c r="K2" s="75">
+        <f t="shared" si="0"/>
+        <v>0.26470588235294118</v>
+      </c>
+      <c r="L2" s="75">
+        <f t="shared" ref="L2" si="1">SUM(100/$AJ$1*L1)/100</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="M2" s="75">
+        <f t="shared" ref="M2" si="2">SUM(100/$AJ$1*M1)/100</f>
+        <v>0.32352941176470595</v>
+      </c>
+      <c r="N2" s="75">
+        <f t="shared" ref="N2" si="3">SUM(100/$AJ$1*N1)/100</f>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="O2" s="75">
+        <f t="shared" ref="O2" si="4">SUM(100/$AJ$1*O1)/100</f>
+        <v>0.38235294117647056</v>
+      </c>
+      <c r="P2" s="75">
+        <f t="shared" ref="P2" si="5">SUM(100/$AJ$1*P1)/100</f>
+        <v>0.41176470588235298</v>
+      </c>
+      <c r="Q2" s="75">
+        <f t="shared" ref="Q2" si="6">SUM(100/$AJ$1*Q1)/100</f>
+        <v>0.44117647058823534</v>
+      </c>
+      <c r="R2" s="75">
+        <f t="shared" ref="R2:S2" si="7">SUM(100/$AJ$1*R1)/100</f>
+        <v>0.4705882352941177</v>
+      </c>
+      <c r="S2" s="75">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="T2" s="75">
+        <f t="shared" ref="T2" si="8">SUM(100/$AJ$1*T1)/100</f>
+        <v>0.52941176470588236</v>
+      </c>
+      <c r="U2" s="75">
+        <f t="shared" ref="U2" si="9">SUM(100/$AJ$1*U1)/100</f>
+        <v>0.55882352941176483</v>
+      </c>
+      <c r="V2" s="75">
+        <f t="shared" ref="V2" si="10">SUM(100/$AJ$1*V1)/100</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="W2" s="75">
+        <f t="shared" ref="W2" si="11">SUM(100/$AJ$1*W1)/100</f>
+        <v>0.61764705882352944</v>
+      </c>
+      <c r="X2" s="75">
+        <f t="shared" ref="X2" si="12">SUM(100/$AJ$1*X1)/100</f>
+        <v>0.64705882352941191</v>
+      </c>
+      <c r="Y2" s="75">
+        <f t="shared" ref="Y2" si="13">SUM(100/$AJ$1*Y1)/100</f>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="Z2" s="75">
+        <f t="shared" ref="Z2:AA2" si="14">SUM(100/$AJ$1*Z1)/100</f>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="AA2" s="75">
+        <f t="shared" si="14"/>
+        <v>0.73529411764705888</v>
+      </c>
+      <c r="AB2" s="75">
+        <f t="shared" ref="AB2" si="15">SUM(100/$AJ$1*AB1)/100</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="AC2" s="75">
+        <f t="shared" ref="AC2" si="16">SUM(100/$AJ$1*AC1)/100</f>
+        <v>0.79411764705882359</v>
+      </c>
+      <c r="AD2" s="75">
+        <f t="shared" ref="AD2" si="17">SUM(100/$AJ$1*AD1)/100</f>
+        <v>0.82352941176470595</v>
+      </c>
+      <c r="AE2" s="75">
+        <f t="shared" ref="AE2" si="18">SUM(100/$AJ$1*AE1)/100</f>
+        <v>0.85294117647058831</v>
+      </c>
+      <c r="AF2" s="75">
+        <f t="shared" ref="AF2" si="19">SUM(100/$AJ$1*AF1)/100</f>
+        <v>0.88235294117647067</v>
+      </c>
+      <c r="AG2" s="75">
+        <f t="shared" ref="AG2" si="20">SUM(100/$AJ$1*AG1)/100</f>
+        <v>0.91176470588235303</v>
+      </c>
+      <c r="AH2" s="75">
+        <f t="shared" ref="AH2:AI2" si="21">SUM(100/$AJ$1*AH1)/100</f>
+        <v>0.94117647058823539</v>
+      </c>
+      <c r="AI2" s="75">
+        <f t="shared" si="21"/>
+        <v>0.97058823529411764</v>
+      </c>
+      <c r="AJ2" s="75">
+        <f t="shared" ref="AJ2" si="22">SUM(100/$AJ$1*AJ1)/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" s="1" customFormat="1" ht="139">
+      <c r="B3" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="47" t="s">
+      <c r="F3" s="40"/>
+      <c r="G3" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="47" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40" t="s">
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="47" t="s">
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40" t="s">
+      <c r="AF3" s="40"/>
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="17" thickBot="1">
-      <c r="A2" s="55" t="s">
+    <row r="4" spans="1:36" ht="17" thickBot="1">
+      <c r="A4" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C4" s="46">
         <v>43367</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D4" s="46">
         <v>43374</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E4" s="46">
         <v>43381</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F4" s="46">
         <v>43388</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G4" s="48">
         <v>43395</v>
       </c>
-      <c r="H2" s="46">
+      <c r="H4" s="46">
         <v>43402</v>
       </c>
-      <c r="I2" s="46">
+      <c r="I4" s="46">
         <v>43409</v>
       </c>
-      <c r="J2" s="46">
+      <c r="J4" s="46">
         <v>43416</v>
       </c>
-      <c r="K2" s="46">
+      <c r="K4" s="46">
         <v>43423</v>
       </c>
-      <c r="L2" s="46">
+      <c r="L4" s="46">
         <v>43430</v>
       </c>
-      <c r="M2" s="48">
+      <c r="M4" s="48">
         <v>43437</v>
       </c>
-      <c r="N2" s="46">
+      <c r="N4" s="46">
         <v>43444</v>
       </c>
-      <c r="O2" s="46">
+      <c r="O4" s="46">
         <v>43451</v>
       </c>
-      <c r="P2" s="46">
+      <c r="P4" s="46">
         <v>43458</v>
       </c>
-      <c r="Q2" s="46">
+      <c r="Q4" s="46">
         <v>43465</v>
       </c>
-      <c r="R2" s="46">
+      <c r="R4" s="46">
         <v>43472</v>
       </c>
-      <c r="S2" s="46">
+      <c r="S4" s="46">
         <v>43479</v>
       </c>
-      <c r="T2" s="46">
+      <c r="T4" s="46">
         <v>43486</v>
       </c>
-      <c r="U2" s="46">
+      <c r="U4" s="46">
         <v>43493</v>
       </c>
-      <c r="V2" s="46">
+      <c r="V4" s="46">
         <v>43500</v>
       </c>
-      <c r="W2" s="46">
+      <c r="W4" s="46">
         <v>43507</v>
       </c>
-      <c r="X2" s="46">
+      <c r="X4" s="46">
         <v>43514</v>
       </c>
-      <c r="Y2" s="46">
+      <c r="Y4" s="46">
         <v>43521</v>
       </c>
-      <c r="Z2" s="46">
+      <c r="Z4" s="46">
         <v>43528</v>
       </c>
-      <c r="AA2" s="46">
+      <c r="AA4" s="46">
         <v>43535</v>
       </c>
-      <c r="AB2" s="46">
+      <c r="AB4" s="46">
         <v>43542</v>
       </c>
-      <c r="AC2" s="46">
+      <c r="AC4" s="46">
         <v>43549</v>
       </c>
-      <c r="AD2" s="46">
+      <c r="AD4" s="46">
         <v>43556</v>
       </c>
-      <c r="AE2" s="48">
+      <c r="AE4" s="48">
         <v>43563</v>
       </c>
-      <c r="AF2" s="46">
+      <c r="AF4" s="46">
         <v>43570</v>
       </c>
-      <c r="AG2" s="46">
+      <c r="AG4" s="46">
         <v>43577</v>
       </c>
-      <c r="AH2" s="46">
+      <c r="AH4" s="46">
         <v>43584</v>
       </c>
-      <c r="AI2" s="46">
+      <c r="AI4" s="46">
         <v>43591</v>
       </c>
-      <c r="AJ2" s="46">
+      <c r="AJ4" s="46">
         <v>43598</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="17" thickTop="1">
-      <c r="A3" s="65" t="s">
+    <row r="5" spans="1:36" ht="17" thickTop="1">
+      <c r="A5" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="G3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AG3" s="28"/>
-    </row>
-    <row r="4" spans="1:36">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="7"/>
-      <c r="G4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="AE4" s="49"/>
-      <c r="AG4" s="28"/>
-    </row>
-    <row r="5" spans="1:36">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="50"/>
+      <c r="B5" s="66"/>
+      <c r="G5" s="49"/>
       <c r="M5" s="49"/>
       <c r="AE5" s="49"/>
       <c r="AG5" s="28"/>
     </row>
     <row r="6" spans="1:36">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="51"/>
+      <c r="E6" s="7"/>
+      <c r="G6" s="49"/>
       <c r="M6" s="49"/>
       <c r="AE6" s="49"/>
       <c r="AG6" s="28"/>
     </row>
     <row r="7" spans="1:36">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="51"/>
-      <c r="I7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="50"/>
       <c r="M7" s="49"/>
       <c r="AE7" s="49"/>
       <c r="AG7" s="28"/>
     </row>
     <row r="8" spans="1:36">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="51"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
       <c r="M8" s="49"/>
       <c r="AE8" s="49"/>
       <c r="AG8" s="28"/>
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="51"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="7"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="7"/>
       <c r="M9" s="49"/>
       <c r="AE9" s="49"/>
       <c r="AG9" s="28"/>
     </row>
     <row r="10" spans="1:36">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="51"/>
-      <c r="M10" s="50"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="M10" s="49"/>
       <c r="AE10" s="49"/>
       <c r="AG10" s="28"/>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="49"/>
+        <v>83</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="51"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="49"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="51"/>
-      <c r="AF11" s="9"/>
+      <c r="AE11" s="49"/>
       <c r="AG11" s="28"/>
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="51"/>
-      <c r="AF12" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="51"/>
+      <c r="M12" s="50"/>
+      <c r="AE12" s="49"/>
       <c r="AG12" s="28"/>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G13" s="49"/>
       <c r="M13" s="49"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
       <c r="AE13" s="51"/>
       <c r="AF13" s="9"/>
       <c r="AG13" s="28"/>
     </row>
     <row r="14" spans="1:36">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G14" s="49"/>
       <c r="M14" s="49"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
       <c r="AC14" s="9"/>
       <c r="AD14" s="9"/>
-      <c r="AE14" s="50"/>
+      <c r="AE14" s="51"/>
       <c r="AF14" s="9"/>
       <c r="AG14" s="28"/>
     </row>
     <row r="15" spans="1:36">
-      <c r="A15" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="68"/>
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>107</v>
+      </c>
       <c r="G15" s="49"/>
       <c r="M15" s="49"/>
-      <c r="AE15" s="49"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="51"/>
+      <c r="AF15" s="9"/>
       <c r="AG15" s="28"/>
     </row>
     <row r="16" spans="1:36">
       <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+        <v>111</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>108</v>
+      </c>
       <c r="G16" s="49"/>
       <c r="M16" s="49"/>
-      <c r="AE16" s="49"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="50"/>
+      <c r="AF16" s="9"/>
       <c r="AG16" s="28"/>
     </row>
     <row r="17" spans="1:36">
-      <c r="A17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
+      <c r="A17" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="68"/>
       <c r="G17" s="49"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
       <c r="M17" s="49"/>
       <c r="AE17" s="49"/>
       <c r="AG17" s="28"/>
     </row>
     <row r="18" spans="1:36">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
       <c r="B18" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+        <v>113</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="49"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
       <c r="M18" s="49"/>
       <c r="AE18" s="49"/>
       <c r="AG18" s="28"/>
     </row>
     <row r="19" spans="1:36">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="49"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+        <v>88</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
       <c r="M19" s="49"/>
       <c r="AE19" s="49"/>
       <c r="AG19" s="28"/>
     </row>
     <row r="20" spans="1:36">
-      <c r="A20" t="s">
-        <v>97</v>
-      </c>
       <c r="B20" s="53" t="s">
-        <v>90</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
       <c r="G20" s="49"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
       <c r="M20" s="49"/>
       <c r="AE20" s="49"/>
       <c r="AG20" s="28"/>
     </row>
     <row r="21" spans="1:36">
-      <c r="A21" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="70"/>
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>89</v>
+      </c>
       <c r="G21" s="49"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
       <c r="M21" s="49"/>
       <c r="AE21" s="49"/>
       <c r="AG21" s="28"/>
     </row>
     <row r="22" spans="1:36">
-      <c r="A22" s="58"/>
-      <c r="B22" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="H22" s="10"/>
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="49"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
       <c r="M22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AG22" s="28"/>
     </row>
     <row r="23" spans="1:36">
-      <c r="A23" s="58"/>
-      <c r="B23" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
+      <c r="A23" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="70"/>
+      <c r="G23" s="49"/>
       <c r="M23" s="49"/>
       <c r="AE23" s="49"/>
       <c r="AG23" s="28"/>
@@ -1572,139 +1800,139 @@
     <row r="24" spans="1:36">
       <c r="A24" s="58"/>
       <c r="B24" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="I24" s="10"/>
+        <v>98</v>
+      </c>
+      <c r="G24" s="60"/>
+      <c r="H24" s="10"/>
       <c r="M24" s="49"/>
       <c r="AE24" s="49"/>
       <c r="AG24" s="28"/>
     </row>
     <row r="25" spans="1:36">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="53" t="s">
-        <v>86</v>
+      <c r="A25" s="58"/>
+      <c r="B25" s="59" t="s">
+        <v>99</v>
       </c>
       <c r="G25" s="49"/>
+      <c r="H25" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="I25" s="10"/>
       <c r="M25" s="49"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="10"/>
-      <c r="Y25" s="10"/>
-      <c r="Z25" s="10"/>
       <c r="AE25" s="49"/>
       <c r="AG25" s="28"/>
     </row>
     <row r="26" spans="1:36">
-      <c r="A26" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="72"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="59" t="s">
+        <v>103</v>
+      </c>
       <c r="G26" s="49"/>
+      <c r="H26" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
       <c r="M26" s="49"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
       <c r="AE26" s="49"/>
       <c r="AG26" s="28"/>
     </row>
     <row r="27" spans="1:36">
       <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>91</v>
+        <v>61</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>86</v>
       </c>
       <c r="G27" s="49"/>
       <c r="M27" s="49"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
-      <c r="AH27" s="52"/>
-      <c r="AI27" s="52"/>
     </row>
     <row r="28" spans="1:36">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>52</v>
-      </c>
+      <c r="A28" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="72"/>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
       <c r="AE28" s="49"/>
       <c r="AG28" s="28"/>
-      <c r="AH28" s="52"/>
-      <c r="AI28" s="52"/>
     </row>
     <row r="29" spans="1:36">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
       <c r="AE29" s="49"/>
       <c r="AG29" s="28"/>
-      <c r="AJ29" s="52"/>
+      <c r="AH29" s="52"/>
+      <c r="AI29" s="52"/>
     </row>
     <row r="30" spans="1:36">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="G30" s="49"/>
       <c r="M30" s="49"/>
       <c r="AE30" s="49"/>
       <c r="AG30" s="28"/>
-      <c r="AJ30" s="52"/>
+      <c r="AH30" s="52"/>
+      <c r="AI30" s="52"/>
     </row>
     <row r="31" spans="1:36">
-      <c r="A31" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="74"/>
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>41</v>
+      </c>
       <c r="G31" s="49"/>
       <c r="M31" s="49"/>
       <c r="AE31" s="49"/>
       <c r="AG31" s="28"/>
+      <c r="AJ31" s="52"/>
     </row>
     <row r="32" spans="1:36">
       <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>75</v>
+      </c>
       <c r="G32" s="49"/>
       <c r="M32" s="49"/>
       <c r="AE32" s="49"/>
       <c r="AG32" s="28"/>
+      <c r="AJ32" s="52"/>
     </row>
     <row r="33" spans="1:39">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="12"/>
+      <c r="A33" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="74"/>
       <c r="G33" s="49"/>
       <c r="M33" s="49"/>
       <c r="AE33" s="49"/>
@@ -1712,145 +1940,94 @@
     </row>
     <row r="34" spans="1:39">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="9"/>
-      <c r="G34" s="62"/>
+        <v>46</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="G34" s="49"/>
       <c r="M34" s="49"/>
       <c r="AE34" s="49"/>
       <c r="AG34" s="28"/>
     </row>
     <row r="35" spans="1:39">
       <c r="A35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" s="44" t="s">
-        <v>72</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="12"/>
       <c r="G35" s="49"/>
       <c r="M35" s="49"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="AC35" s="24"/>
-      <c r="AD35" s="24"/>
       <c r="AE35" s="49"/>
       <c r="AG35" s="28"/>
-      <c r="AJ35" s="12"/>
     </row>
     <row r="36" spans="1:39">
-      <c r="A36" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="64"/>
-      <c r="G36" s="49"/>
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="G36" s="62"/>
       <c r="M36" s="49"/>
       <c r="AE36" s="49"/>
       <c r="AG36" s="28"/>
     </row>
     <row r="37" spans="1:39">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+        <v>72</v>
+      </c>
       <c r="G37" s="49"/>
       <c r="M37" s="49"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="AC37" s="24"/>
+      <c r="AD37" s="24"/>
       <c r="AE37" s="49"/>
       <c r="AG37" s="28"/>
-    </row>
-    <row r="38" spans="1:39" s="28" customFormat="1">
-      <c r="A38" s="28" t="s">
+      <c r="AJ37" s="12"/>
+    </row>
+    <row r="38" spans="1:39">
+      <c r="A38" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="64"/>
+      <c r="G38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="AE38" s="49"/>
+      <c r="AG38" s="28"/>
+    </row>
+    <row r="39" spans="1:39">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="G39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="AE39" s="49"/>
+      <c r="AG39" s="28"/>
+    </row>
+    <row r="40" spans="1:39" s="28" customFormat="1">
+      <c r="A40" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B40" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38" s="49"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38" s="49"/>
-      <c r="N38"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-      <c r="W38"/>
-      <c r="X38"/>
-      <c r="Y38"/>
-      <c r="Z38"/>
-      <c r="AA38"/>
-      <c r="AB38"/>
-      <c r="AC38"/>
-      <c r="AD38"/>
-      <c r="AE38" s="49"/>
-      <c r="AF38"/>
-      <c r="AM38" s="39"/>
-    </row>
-    <row r="39" spans="1:39" s="28" customFormat="1">
-      <c r="A39" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39" s="49"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39" s="49"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-      <c r="AB39"/>
-      <c r="AC39"/>
-      <c r="AD39"/>
-      <c r="AE39" s="49"/>
-      <c r="AF39"/>
-    </row>
-    <row r="40" spans="1:39" s="28" customFormat="1">
-      <c r="A40" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40"/>
+      <c r="C40" s="9"/>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
@@ -1862,10 +2039,10 @@
       <c r="L40"/>
       <c r="M40" s="49"/>
       <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
       <c r="S40"/>
       <c r="T40"/>
       <c r="U40"/>
@@ -1876,16 +2053,91 @@
       <c r="Z40"/>
       <c r="AA40"/>
       <c r="AB40"/>
-      <c r="AC40" s="9"/>
-      <c r="AD40" s="9"/>
-      <c r="AE40" s="51"/>
-      <c r="AF40" s="8"/>
-      <c r="AG40" s="54"/>
-      <c r="AH40" s="54"/>
-      <c r="AI40" s="54"/>
-    </row>
-    <row r="41" spans="1:39" s="28" customFormat="1"/>
-    <row r="42" spans="1:39" s="28" customFormat="1"/>
+      <c r="AC40"/>
+      <c r="AD40"/>
+      <c r="AE40" s="49"/>
+      <c r="AF40"/>
+      <c r="AM40" s="39"/>
+    </row>
+    <row r="41" spans="1:39" s="28" customFormat="1">
+      <c r="A41" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41" s="49"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41" s="49"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+      <c r="Z41"/>
+      <c r="AA41"/>
+      <c r="AB41"/>
+      <c r="AC41"/>
+      <c r="AD41"/>
+      <c r="AE41" s="49"/>
+      <c r="AF41"/>
+    </row>
+    <row r="42" spans="1:39" s="28" customFormat="1">
+      <c r="A42" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42" s="49"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42" s="49"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+      <c r="Z42"/>
+      <c r="AA42"/>
+      <c r="AB42"/>
+      <c r="AC42" s="9"/>
+      <c r="AD42" s="9"/>
+      <c r="AE42" s="51"/>
+      <c r="AF42" s="8"/>
+      <c r="AG42" s="54"/>
+      <c r="AH42" s="54"/>
+      <c r="AI42" s="54"/>
+    </row>
     <row r="43" spans="1:39" s="28" customFormat="1"/>
     <row r="44" spans="1:39" s="28" customFormat="1"/>
     <row r="45" spans="1:39" s="28" customFormat="1"/>
@@ -1914,24 +2166,46 @@
     <row r="68" spans="2:2" s="28" customFormat="1"/>
     <row r="69" spans="2:2" s="28" customFormat="1"/>
     <row r="70" spans="2:2" s="28" customFormat="1"/>
-    <row r="71" spans="2:2">
-      <c r="B71" s="28"/>
-    </row>
-    <row r="72" spans="2:2">
-      <c r="B72" s="28"/>
-    </row>
+    <row r="71" spans="2:2" s="28" customFormat="1"/>
+    <row r="72" spans="2:2" s="28" customFormat="1"/>
     <row r="73" spans="2:2">
       <c r="B73" s="28"/>
     </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="28"/>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="28"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A33:B33"/>
   </mergeCells>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:AJ2">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
WorkPlan final draft of tasks
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014E98BA-112D-8B49-8AD1-6A9120FA7AE7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124DF421-B46F-AF42-8D17-AC022AC26E05}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="120">
   <si>
     <t>Week</t>
   </si>
@@ -347,12 +347,6 @@
     <t>Implement Random Agent</t>
   </si>
   <si>
-    <t>Could move this section around maybe have it during/after research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not sure where to put this need to research to find some :) </t>
-  </si>
-  <si>
     <t>GVGAI Framework Review</t>
   </si>
   <si>
@@ -393,6 +387,24 @@
   </si>
   <si>
     <t>Week Number</t>
+  </si>
+  <si>
+    <t>Research for Solution</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
   </si>
 </sst>
 </file>
@@ -672,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -753,9 +765,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -800,6 +809,13 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,13 +1102,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM75"/>
+  <dimension ref="A1:AM76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1106,8 +1122,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
-      <c r="B1" s="76" t="s">
-        <v>115</v>
+      <c r="B1" s="75" t="s">
+        <v>113</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1213,142 +1229,142 @@
       </c>
     </row>
     <row r="2" spans="1:36">
-      <c r="B2" s="76" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="75">
+      <c r="B2" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="74">
         <f>SUM(100/$AJ$1*C1)/100</f>
         <v>2.9411764705882356E-2</v>
       </c>
-      <c r="D2" s="75">
+      <c r="D2" s="74">
         <f t="shared" ref="D2:K2" si="0">SUM(100/$AJ$1*D1)/100</f>
         <v>5.8823529411764712E-2</v>
       </c>
-      <c r="E2" s="75">
+      <c r="E2" s="74">
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="F2" s="75">
+      <c r="F2" s="74">
         <f t="shared" si="0"/>
         <v>0.11764705882352942</v>
       </c>
-      <c r="G2" s="75">
+      <c r="G2" s="74">
         <f t="shared" si="0"/>
         <v>0.14705882352941177</v>
       </c>
-      <c r="H2" s="75">
+      <c r="H2" s="74">
         <f t="shared" si="0"/>
         <v>0.17647058823529413</v>
       </c>
-      <c r="I2" s="75">
+      <c r="I2" s="74">
         <f t="shared" si="0"/>
         <v>0.20588235294117649</v>
       </c>
-      <c r="J2" s="75">
+      <c r="J2" s="74">
         <f t="shared" si="0"/>
         <v>0.23529411764705885</v>
       </c>
-      <c r="K2" s="75">
+      <c r="K2" s="74">
         <f t="shared" si="0"/>
         <v>0.26470588235294118</v>
       </c>
-      <c r="L2" s="75">
+      <c r="L2" s="74">
         <f t="shared" ref="L2" si="1">SUM(100/$AJ$1*L1)/100</f>
         <v>0.29411764705882354</v>
       </c>
-      <c r="M2" s="75">
+      <c r="M2" s="74">
         <f t="shared" ref="M2" si="2">SUM(100/$AJ$1*M1)/100</f>
         <v>0.32352941176470595</v>
       </c>
-      <c r="N2" s="75">
+      <c r="N2" s="74">
         <f t="shared" ref="N2" si="3">SUM(100/$AJ$1*N1)/100</f>
         <v>0.35294117647058826</v>
       </c>
-      <c r="O2" s="75">
+      <c r="O2" s="74">
         <f t="shared" ref="O2" si="4">SUM(100/$AJ$1*O1)/100</f>
         <v>0.38235294117647056</v>
       </c>
-      <c r="P2" s="75">
+      <c r="P2" s="74">
         <f t="shared" ref="P2" si="5">SUM(100/$AJ$1*P1)/100</f>
         <v>0.41176470588235298</v>
       </c>
-      <c r="Q2" s="75">
+      <c r="Q2" s="74">
         <f t="shared" ref="Q2" si="6">SUM(100/$AJ$1*Q1)/100</f>
         <v>0.44117647058823534</v>
       </c>
-      <c r="R2" s="75">
+      <c r="R2" s="74">
         <f t="shared" ref="R2:S2" si="7">SUM(100/$AJ$1*R1)/100</f>
         <v>0.4705882352941177</v>
       </c>
-      <c r="S2" s="75">
+      <c r="S2" s="74">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="T2" s="75">
+      <c r="T2" s="74">
         <f t="shared" ref="T2" si="8">SUM(100/$AJ$1*T1)/100</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="U2" s="75">
+      <c r="U2" s="74">
         <f t="shared" ref="U2" si="9">SUM(100/$AJ$1*U1)/100</f>
         <v>0.55882352941176483</v>
       </c>
-      <c r="V2" s="75">
+      <c r="V2" s="74">
         <f t="shared" ref="V2" si="10">SUM(100/$AJ$1*V1)/100</f>
         <v>0.58823529411764708</v>
       </c>
-      <c r="W2" s="75">
+      <c r="W2" s="74">
         <f t="shared" ref="W2" si="11">SUM(100/$AJ$1*W1)/100</f>
         <v>0.61764705882352944</v>
       </c>
-      <c r="X2" s="75">
+      <c r="X2" s="74">
         <f t="shared" ref="X2" si="12">SUM(100/$AJ$1*X1)/100</f>
         <v>0.64705882352941191</v>
       </c>
-      <c r="Y2" s="75">
+      <c r="Y2" s="74">
         <f t="shared" ref="Y2" si="13">SUM(100/$AJ$1*Y1)/100</f>
         <v>0.67647058823529416</v>
       </c>
-      <c r="Z2" s="75">
+      <c r="Z2" s="74">
         <f t="shared" ref="Z2:AA2" si="14">SUM(100/$AJ$1*Z1)/100</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="AA2" s="75">
+      <c r="AA2" s="74">
         <f t="shared" si="14"/>
         <v>0.73529411764705888</v>
       </c>
-      <c r="AB2" s="75">
+      <c r="AB2" s="74">
         <f t="shared" ref="AB2" si="15">SUM(100/$AJ$1*AB1)/100</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="AC2" s="75">
+      <c r="AC2" s="74">
         <f t="shared" ref="AC2" si="16">SUM(100/$AJ$1*AC1)/100</f>
         <v>0.79411764705882359</v>
       </c>
-      <c r="AD2" s="75">
+      <c r="AD2" s="74">
         <f t="shared" ref="AD2" si="17">SUM(100/$AJ$1*AD1)/100</f>
         <v>0.82352941176470595</v>
       </c>
-      <c r="AE2" s="75">
+      <c r="AE2" s="74">
         <f t="shared" ref="AE2" si="18">SUM(100/$AJ$1*AE1)/100</f>
         <v>0.85294117647058831</v>
       </c>
-      <c r="AF2" s="75">
+      <c r="AF2" s="74">
         <f t="shared" ref="AF2" si="19">SUM(100/$AJ$1*AF1)/100</f>
         <v>0.88235294117647067</v>
       </c>
-      <c r="AG2" s="75">
+      <c r="AG2" s="74">
         <f t="shared" ref="AG2" si="20">SUM(100/$AJ$1*AG1)/100</f>
         <v>0.91176470588235303</v>
       </c>
-      <c r="AH2" s="75">
+      <c r="AH2" s="74">
         <f t="shared" ref="AH2:AI2" si="21">SUM(100/$AJ$1*AH1)/100</f>
         <v>0.94117647058823539</v>
       </c>
-      <c r="AI2" s="75">
+      <c r="AI2" s="74">
         <f t="shared" si="21"/>
         <v>0.97058823529411764</v>
       </c>
-      <c r="AJ2" s="75">
+      <c r="AJ2" s="74">
         <f t="shared" ref="AJ2" si="22">SUM(100/$AJ$1*AJ1)/100</f>
         <v>1</v>
       </c>
@@ -1516,10 +1532,10 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="17" thickTop="1">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="66"/>
+      <c r="B5" s="65"/>
       <c r="G5" s="49"/>
       <c r="M5" s="49"/>
       <c r="AE5" s="49"/>
@@ -1563,7 +1579,7 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="61"/>
+      <c r="F8" s="60"/>
       <c r="G8" s="51"/>
       <c r="M8" s="49"/>
       <c r="AE8" s="49"/>
@@ -1642,7 +1658,7 @@
         <v>93</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G13" s="49"/>
       <c r="M13" s="49"/>
@@ -1656,10 +1672,10 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G14" s="49"/>
       <c r="M14" s="49"/>
@@ -1673,10 +1689,10 @@
     </row>
     <row r="15" spans="1:36">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G15" s="49"/>
       <c r="M15" s="49"/>
@@ -1690,10 +1706,10 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G16" s="49"/>
       <c r="M16" s="49"/>
@@ -1706,10 +1722,10 @@
       <c r="AG16" s="28"/>
     </row>
     <row r="17" spans="1:36">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="68"/>
+      <c r="B17" s="67"/>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
       <c r="AE17" s="49"/>
@@ -1720,7 +1736,7 @@
         <v>60</v>
       </c>
       <c r="B18" s="53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -1739,15 +1755,18 @@
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
-      <c r="G19" s="11"/>
+      <c r="G19" s="76"/>
       <c r="H19" s="11"/>
       <c r="M19" s="49"/>
       <c r="AE19" s="49"/>
       <c r="AG19" s="28"/>
     </row>
     <row r="20" spans="1:36">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
       <c r="B20" s="53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -1760,7 +1779,7 @@
     </row>
     <row r="21" spans="1:36">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B21" s="53" t="s">
         <v>89</v>
@@ -1775,7 +1794,7 @@
     </row>
     <row r="22" spans="1:36">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>90</v>
@@ -1788,112 +1807,127 @@
       <c r="AG22" s="28"/>
     </row>
     <row r="23" spans="1:36">
-      <c r="A23" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="70"/>
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>114</v>
+      </c>
       <c r="G23" s="49"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
       <c r="M23" s="49"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
       <c r="AE23" s="49"/>
       <c r="AG23" s="28"/>
     </row>
     <row r="24" spans="1:36">
-      <c r="A24" s="58"/>
-      <c r="B24" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="60"/>
-      <c r="H24" s="10"/>
+      <c r="A24" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="69"/>
+      <c r="G24" s="49"/>
       <c r="M24" s="49"/>
       <c r="AE24" s="49"/>
       <c r="AG24" s="28"/>
     </row>
     <row r="25" spans="1:36">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="49"/>
-      <c r="H25" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="I25" s="10"/>
+      <c r="A25" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="59"/>
+      <c r="H25" s="10"/>
       <c r="M25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AG25" s="28"/>
     </row>
     <row r="26" spans="1:36">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59" t="s">
-        <v>103</v>
+      <c r="A26" s="78" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>99</v>
       </c>
       <c r="G26" s="49"/>
-      <c r="H26" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
       <c r="M26" s="49"/>
       <c r="AE26" s="49"/>
       <c r="AG26" s="28"/>
     </row>
     <row r="27" spans="1:36">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="53" t="s">
-        <v>86</v>
+      <c r="A27" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>101</v>
       </c>
       <c r="G27" s="49"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
       <c r="M27" s="49"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10"/>
-      <c r="Z27" s="10"/>
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
     </row>
     <row r="28" spans="1:36">
-      <c r="A28" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="72"/>
+      <c r="A28" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>86</v>
+      </c>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
       <c r="AE28" s="49"/>
       <c r="AG28" s="28"/>
     </row>
     <row r="29" spans="1:36">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>91</v>
-      </c>
+      <c r="A29" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="71"/>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
       <c r="AE29" s="49"/>
       <c r="AG29" s="28"/>
-      <c r="AH29" s="52"/>
-      <c r="AI29" s="52"/>
     </row>
     <row r="30" spans="1:36">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="G30" s="49"/>
       <c r="M30" s="49"/>
@@ -1904,23 +1938,24 @@
     </row>
     <row r="31" spans="1:36">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G31" s="49"/>
       <c r="M31" s="49"/>
       <c r="AE31" s="49"/>
       <c r="AG31" s="28"/>
-      <c r="AJ31" s="52"/>
+      <c r="AH31" s="52"/>
+      <c r="AI31" s="52"/>
     </row>
     <row r="32" spans="1:36">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="G32" s="49"/>
       <c r="M32" s="49"/>
@@ -1929,23 +1964,23 @@
       <c r="AJ32" s="52"/>
     </row>
     <row r="33" spans="1:39">
-      <c r="A33" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="74"/>
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>75</v>
+      </c>
       <c r="G33" s="49"/>
       <c r="M33" s="49"/>
       <c r="AE33" s="49"/>
       <c r="AG33" s="28"/>
+      <c r="AJ33" s="52"/>
     </row>
     <row r="34" spans="1:39">
-      <c r="A34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="12"/>
+      <c r="A34" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="73"/>
       <c r="G34" s="49"/>
       <c r="M34" s="49"/>
       <c r="AE34" s="49"/>
@@ -1953,10 +1988,10 @@
     </row>
     <row r="35" spans="1:39">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="53" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="D35" s="12"/>
       <c r="G35" s="49"/>
@@ -1966,107 +2001,81 @@
     </row>
     <row r="36" spans="1:39">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="G36" s="62"/>
+        <v>87</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="G36" s="49"/>
       <c r="M36" s="49"/>
       <c r="AE36" s="49"/>
       <c r="AG36" s="28"/>
     </row>
     <row r="37" spans="1:39">
       <c r="A37" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="G37" s="49"/>
+        <v>67</v>
+      </c>
+      <c r="B37" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="G37" s="61"/>
       <c r="M37" s="49"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="AC37" s="24"/>
-      <c r="AD37" s="24"/>
       <c r="AE37" s="49"/>
       <c r="AG37" s="28"/>
-      <c r="AJ37" s="12"/>
     </row>
     <row r="38" spans="1:39">
-      <c r="A38" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="64"/>
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="G38" s="49"/>
       <c r="M38" s="49"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="AC38" s="24"/>
+      <c r="AD38" s="24"/>
       <c r="AE38" s="49"/>
       <c r="AG38" s="28"/>
+      <c r="AJ38" s="12"/>
     </row>
     <row r="39" spans="1:39">
-      <c r="A39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="A39" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="63"/>
       <c r="G39" s="49"/>
       <c r="M39" s="49"/>
       <c r="AE39" s="49"/>
       <c r="AG39" s="28"/>
     </row>
-    <row r="40" spans="1:39" s="28" customFormat="1">
-      <c r="A40" s="28" t="s">
+    <row r="40" spans="1:39">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="G40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="AE40" s="49"/>
+      <c r="AG40" s="28"/>
+    </row>
+    <row r="41" spans="1:39" s="28" customFormat="1">
+      <c r="A41" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B41" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40" s="49"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40" s="49"/>
-      <c r="N40"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-      <c r="X40"/>
-      <c r="Y40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AB40"/>
-      <c r="AC40"/>
-      <c r="AD40"/>
-      <c r="AE40" s="49"/>
-      <c r="AF40"/>
-      <c r="AM40" s="39"/>
-    </row>
-    <row r="41" spans="1:39" s="28" customFormat="1">
-      <c r="A41" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41"/>
+      <c r="C41" s="9"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
@@ -2078,12 +2087,12 @@
       <c r="L41"/>
       <c r="M41" s="49"/>
       <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41"/>
+      <c r="T41"/>
       <c r="U41"/>
       <c r="V41"/>
       <c r="W41"/>
@@ -2096,13 +2105,14 @@
       <c r="AD41"/>
       <c r="AE41" s="49"/>
       <c r="AF41"/>
+      <c r="AM41" s="39"/>
     </row>
     <row r="42" spans="1:39" s="28" customFormat="1">
       <c r="A42" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C42"/>
       <c r="D42"/>
@@ -2120,8 +2130,8 @@
       <c r="P42"/>
       <c r="Q42"/>
       <c r="R42"/>
-      <c r="S42"/>
-      <c r="T42"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
       <c r="U42"/>
       <c r="V42"/>
       <c r="W42"/>
@@ -2130,15 +2140,52 @@
       <c r="Z42"/>
       <c r="AA42"/>
       <c r="AB42"/>
-      <c r="AC42" s="9"/>
-      <c r="AD42" s="9"/>
-      <c r="AE42" s="51"/>
-      <c r="AF42" s="8"/>
-      <c r="AG42" s="54"/>
-      <c r="AH42" s="54"/>
-      <c r="AI42" s="54"/>
-    </row>
-    <row r="43" spans="1:39" s="28" customFormat="1"/>
+      <c r="AC42"/>
+      <c r="AD42"/>
+      <c r="AE42" s="49"/>
+      <c r="AF42"/>
+    </row>
+    <row r="43" spans="1:39" s="28" customFormat="1">
+      <c r="A43" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43" s="49"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43" s="49"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43"/>
+      <c r="Y43"/>
+      <c r="Z43"/>
+      <c r="AA43"/>
+      <c r="AB43"/>
+      <c r="AC43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="51"/>
+      <c r="AF43" s="8"/>
+      <c r="AG43" s="54"/>
+      <c r="AH43" s="54"/>
+      <c r="AI43" s="54"/>
+    </row>
     <row r="44" spans="1:39" s="28" customFormat="1"/>
     <row r="45" spans="1:39" s="28" customFormat="1"/>
     <row r="46" spans="1:39" s="28" customFormat="1"/>
@@ -2168,23 +2215,24 @@
     <row r="70" spans="2:2" s="28" customFormat="1"/>
     <row r="71" spans="2:2" s="28" customFormat="1"/>
     <row r="72" spans="2:2" s="28" customFormat="1"/>
-    <row r="73" spans="2:2">
-      <c r="B73" s="28"/>
-    </row>
+    <row r="73" spans="2:2" s="28" customFormat="1"/>
     <row r="74" spans="2:2">
       <c r="B74" s="28"/>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" s="28"/>
     </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="28"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="colorScale" priority="2">
@@ -2295,10 +2343,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" thickTop="1">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="66"/>
+      <c r="B3" s="65"/>
       <c r="G3" s="49"/>
       <c r="M3" s="49"/>
     </row>
@@ -2409,10 +2457,10 @@
       <c r="M11" s="49"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="68"/>
+      <c r="B12" s="67"/>
       <c r="G12" s="49"/>
       <c r="M12" s="49"/>
     </row>
@@ -2468,10 +2516,10 @@
       <c r="M16" s="49"/>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="70"/>
+      <c r="B17" s="69"/>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
     </row>
@@ -2486,10 +2534,10 @@
       <c r="M18" s="49"/>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="72"/>
+      <c r="B19" s="71"/>
       <c r="G19" s="49"/>
       <c r="M19" s="49"/>
     </row>
@@ -2534,10 +2582,10 @@
       <c r="M23" s="49"/>
     </row>
     <row r="24" spans="1:39">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="74"/>
+      <c r="B24" s="73"/>
       <c r="G24" s="49"/>
       <c r="M24" s="49"/>
     </row>
@@ -2574,10 +2622,10 @@
       <c r="M27" s="49"/>
     </row>
     <row r="28" spans="1:39">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="64"/>
+      <c r="B28" s="63"/>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
     </row>
@@ -2713,10 +2761,10 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="28" customFormat="1" ht="17" thickTop="1">
-      <c r="A36" s="65" t="s">
+      <c r="A36" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="66"/>
+      <c r="B36" s="65"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
@@ -2882,10 +2930,10 @@
       <c r="M44"/>
     </row>
     <row r="45" spans="1:13" s="28" customFormat="1">
-      <c r="A45" s="67" t="s">
+      <c r="A45" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="68"/>
+      <c r="B45" s="67"/>
       <c r="C45"/>
       <c r="D45"/>
       <c r="E45"/>
@@ -2975,10 +3023,10 @@
       <c r="M49"/>
     </row>
     <row r="50" spans="1:13" s="28" customFormat="1">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="70"/>
+      <c r="B50" s="69"/>
       <c r="C50"/>
       <c r="D50"/>
       <c r="E50"/>
@@ -3011,10 +3059,10 @@
       <c r="M51" s="10"/>
     </row>
     <row r="52" spans="1:13" s="28" customFormat="1">
-      <c r="A52" s="71" t="s">
+      <c r="A52" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="72"/>
+      <c r="B52" s="71"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
@@ -3104,10 +3152,10 @@
       <c r="M56"/>
     </row>
     <row r="57" spans="1:13" s="28" customFormat="1">
-      <c r="A57" s="73" t="s">
+      <c r="A57" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="74"/>
+      <c r="B57" s="73"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
@@ -3178,10 +3226,10 @@
       <c r="M60"/>
     </row>
     <row r="61" spans="1:13" s="28" customFormat="1">
-      <c r="A61" s="63" t="s">
+      <c r="A61" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="64"/>
+      <c r="B61" s="63"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
@@ -3313,10 +3361,10 @@
       </c>
     </row>
     <row r="69" spans="1:14" ht="17" thickTop="1">
-      <c r="A69" s="65" t="s">
+      <c r="A69" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="66"/>
+      <c r="B69" s="65"/>
       <c r="I69" s="49"/>
       <c r="K69" s="28"/>
       <c r="M69"/>
@@ -3415,10 +3463,10 @@
       <c r="M77"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="67" t="s">
+      <c r="A78" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="68"/>
+      <c r="B78" s="67"/>
       <c r="I78" s="49"/>
       <c r="K78" s="28"/>
       <c r="M78"/>
@@ -3468,10 +3516,10 @@
       <c r="M82"/>
     </row>
     <row r="83" spans="1:14">
-      <c r="A83" s="69" t="s">
+      <c r="A83" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="70"/>
+      <c r="B83" s="69"/>
       <c r="I83" s="49"/>
       <c r="K83" s="28"/>
       <c r="M83"/>
@@ -3490,10 +3538,10 @@
       <c r="M84"/>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="71" t="s">
+      <c r="A85" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B85" s="72"/>
+      <c r="B85" s="71"/>
       <c r="I85" s="49"/>
       <c r="K85" s="28"/>
       <c r="M85"/>
@@ -3547,10 +3595,10 @@
       <c r="N89" s="52"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="73" t="s">
+      <c r="A90" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="B90" s="74"/>
+      <c r="B90" s="73"/>
       <c r="I90" s="49"/>
       <c r="K90" s="28"/>
       <c r="M90"/>
@@ -3592,10 +3640,10 @@
       <c r="N93" s="12"/>
     </row>
     <row r="94" spans="1:14">
-      <c r="A94" s="63" t="s">
+      <c r="A94" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B94" s="64"/>
+      <c r="B94" s="63"/>
       <c r="I94" s="49"/>
       <c r="K94" s="28"/>
       <c r="M94"/>

</xml_diff>

<commit_message>
Work Plan description titles & codes match the work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124DF421-B46F-AF42-8D17-AC022AC26E05}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4F8F0F-A9E1-854E-94DE-91738ED92598}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="124">
   <si>
     <t>Week</t>
   </si>
@@ -353,9 +353,6 @@
     <t>Run avalible Previous Agents</t>
   </si>
   <si>
-    <t>Create Meeting Document</t>
-  </si>
-  <si>
     <t>Research Paper Structure Sections</t>
   </si>
   <si>
@@ -405,6 +402,21 @@
   </si>
   <si>
     <t>S4</t>
+  </si>
+  <si>
+    <t>Create Meeting Minutes Document</t>
+  </si>
+  <si>
+    <t>Print and Collate Final Hand In</t>
+  </si>
+  <si>
+    <t>Research Paper Video Demo</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>M5</t>
   </si>
 </sst>
 </file>
@@ -771,6 +783,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,15 +827,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1102,19 +1114,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
-  <dimension ref="A1:AM76"/>
+  <dimension ref="A1:AM78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="9.1640625" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" style="28" customWidth="1"/>
     <col min="14" max="36" width="9.1640625" customWidth="1"/>
@@ -1122,8 +1134,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
-      <c r="B1" s="75" t="s">
-        <v>113</v>
+      <c r="B1" s="63" t="s">
+        <v>112</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1229,142 +1241,142 @@
       </c>
     </row>
     <row r="2" spans="1:36">
-      <c r="B2" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="74">
+      <c r="B2" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="62">
         <f>SUM(100/$AJ$1*C1)/100</f>
         <v>2.9411764705882356E-2</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="62">
         <f t="shared" ref="D2:K2" si="0">SUM(100/$AJ$1*D1)/100</f>
         <v>5.8823529411764712E-2</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E2" s="62">
         <f t="shared" si="0"/>
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="F2" s="74">
+      <c r="F2" s="62">
         <f t="shared" si="0"/>
         <v>0.11764705882352942</v>
       </c>
-      <c r="G2" s="74">
+      <c r="G2" s="62">
         <f t="shared" si="0"/>
         <v>0.14705882352941177</v>
       </c>
-      <c r="H2" s="74">
+      <c r="H2" s="62">
         <f t="shared" si="0"/>
         <v>0.17647058823529413</v>
       </c>
-      <c r="I2" s="74">
+      <c r="I2" s="62">
         <f t="shared" si="0"/>
         <v>0.20588235294117649</v>
       </c>
-      <c r="J2" s="74">
+      <c r="J2" s="62">
         <f t="shared" si="0"/>
         <v>0.23529411764705885</v>
       </c>
-      <c r="K2" s="74">
+      <c r="K2" s="62">
         <f t="shared" si="0"/>
         <v>0.26470588235294118</v>
       </c>
-      <c r="L2" s="74">
+      <c r="L2" s="62">
         <f t="shared" ref="L2" si="1">SUM(100/$AJ$1*L1)/100</f>
         <v>0.29411764705882354</v>
       </c>
-      <c r="M2" s="74">
+      <c r="M2" s="62">
         <f t="shared" ref="M2" si="2">SUM(100/$AJ$1*M1)/100</f>
         <v>0.32352941176470595</v>
       </c>
-      <c r="N2" s="74">
+      <c r="N2" s="62">
         <f t="shared" ref="N2" si="3">SUM(100/$AJ$1*N1)/100</f>
         <v>0.35294117647058826</v>
       </c>
-      <c r="O2" s="74">
+      <c r="O2" s="62">
         <f t="shared" ref="O2" si="4">SUM(100/$AJ$1*O1)/100</f>
         <v>0.38235294117647056</v>
       </c>
-      <c r="P2" s="74">
+      <c r="P2" s="62">
         <f t="shared" ref="P2" si="5">SUM(100/$AJ$1*P1)/100</f>
         <v>0.41176470588235298</v>
       </c>
-      <c r="Q2" s="74">
+      <c r="Q2" s="62">
         <f t="shared" ref="Q2" si="6">SUM(100/$AJ$1*Q1)/100</f>
         <v>0.44117647058823534</v>
       </c>
-      <c r="R2" s="74">
+      <c r="R2" s="62">
         <f t="shared" ref="R2:S2" si="7">SUM(100/$AJ$1*R1)/100</f>
         <v>0.4705882352941177</v>
       </c>
-      <c r="S2" s="74">
+      <c r="S2" s="62">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="T2" s="74">
+      <c r="T2" s="62">
         <f t="shared" ref="T2" si="8">SUM(100/$AJ$1*T1)/100</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="U2" s="74">
+      <c r="U2" s="62">
         <f t="shared" ref="U2" si="9">SUM(100/$AJ$1*U1)/100</f>
         <v>0.55882352941176483</v>
       </c>
-      <c r="V2" s="74">
+      <c r="V2" s="62">
         <f t="shared" ref="V2" si="10">SUM(100/$AJ$1*V1)/100</f>
         <v>0.58823529411764708</v>
       </c>
-      <c r="W2" s="74">
+      <c r="W2" s="62">
         <f t="shared" ref="W2" si="11">SUM(100/$AJ$1*W1)/100</f>
         <v>0.61764705882352944</v>
       </c>
-      <c r="X2" s="74">
+      <c r="X2" s="62">
         <f t="shared" ref="X2" si="12">SUM(100/$AJ$1*X1)/100</f>
         <v>0.64705882352941191</v>
       </c>
-      <c r="Y2" s="74">
+      <c r="Y2" s="62">
         <f t="shared" ref="Y2" si="13">SUM(100/$AJ$1*Y1)/100</f>
         <v>0.67647058823529416</v>
       </c>
-      <c r="Z2" s="74">
+      <c r="Z2" s="62">
         <f t="shared" ref="Z2:AA2" si="14">SUM(100/$AJ$1*Z1)/100</f>
         <v>0.70588235294117652</v>
       </c>
-      <c r="AA2" s="74">
+      <c r="AA2" s="62">
         <f t="shared" si="14"/>
         <v>0.73529411764705888</v>
       </c>
-      <c r="AB2" s="74">
+      <c r="AB2" s="62">
         <f t="shared" ref="AB2" si="15">SUM(100/$AJ$1*AB1)/100</f>
         <v>0.76470588235294112</v>
       </c>
-      <c r="AC2" s="74">
+      <c r="AC2" s="62">
         <f t="shared" ref="AC2" si="16">SUM(100/$AJ$1*AC1)/100</f>
         <v>0.79411764705882359</v>
       </c>
-      <c r="AD2" s="74">
+      <c r="AD2" s="62">
         <f t="shared" ref="AD2" si="17">SUM(100/$AJ$1*AD1)/100</f>
         <v>0.82352941176470595</v>
       </c>
-      <c r="AE2" s="74">
+      <c r="AE2" s="62">
         <f t="shared" ref="AE2" si="18">SUM(100/$AJ$1*AE1)/100</f>
         <v>0.85294117647058831</v>
       </c>
-      <c r="AF2" s="74">
+      <c r="AF2" s="62">
         <f t="shared" ref="AF2" si="19">SUM(100/$AJ$1*AF1)/100</f>
         <v>0.88235294117647067</v>
       </c>
-      <c r="AG2" s="74">
+      <c r="AG2" s="62">
         <f t="shared" ref="AG2" si="20">SUM(100/$AJ$1*AG1)/100</f>
         <v>0.91176470588235303</v>
       </c>
-      <c r="AH2" s="74">
+      <c r="AH2" s="62">
         <f t="shared" ref="AH2:AI2" si="21">SUM(100/$AJ$1*AH1)/100</f>
         <v>0.94117647058823539</v>
       </c>
-      <c r="AI2" s="74">
+      <c r="AI2" s="62">
         <f t="shared" si="21"/>
         <v>0.97058823529411764</v>
       </c>
-      <c r="AJ2" s="74">
+      <c r="AJ2" s="62">
         <f t="shared" ref="AJ2" si="22">SUM(100/$AJ$1*AJ1)/100</f>
         <v>1</v>
       </c>
@@ -1532,10 +1544,10 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="17" thickTop="1">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="65"/>
+      <c r="B5" s="70"/>
       <c r="G5" s="49"/>
       <c r="M5" s="49"/>
       <c r="AE5" s="49"/>
@@ -1658,7 +1670,7 @@
         <v>93</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" s="49"/>
       <c r="M13" s="49"/>
@@ -1672,10 +1684,10 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14" s="49"/>
       <c r="M14" s="49"/>
@@ -1689,10 +1701,10 @@
     </row>
     <row r="15" spans="1:36">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G15" s="49"/>
       <c r="M15" s="49"/>
@@ -1706,10 +1718,10 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="G16" s="49"/>
       <c r="M16" s="49"/>
@@ -1721,227 +1733,230 @@
       <c r="AF16" s="9"/>
       <c r="AG16" s="28"/>
     </row>
-    <row r="17" spans="1:36">
-      <c r="A17" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="67"/>
+    <row r="17" spans="1:35">
+      <c r="A17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>105</v>
+      </c>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
-      <c r="AE17" s="49"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="9"/>
       <c r="AG17" s="28"/>
     </row>
-    <row r="18" spans="1:36">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+    <row r="18" spans="1:35">
+      <c r="A18" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="72"/>
       <c r="G18" s="49"/>
       <c r="M18" s="49"/>
       <c r="AE18" s="49"/>
       <c r="AG18" s="28"/>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:35">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="11"/>
+        <v>110</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="49"/>
       <c r="M19" s="49"/>
       <c r="AE19" s="49"/>
       <c r="AG19" s="28"/>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:35">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
-      <c r="G20" s="49"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
       <c r="M20" s="49"/>
       <c r="AE20" s="49"/>
       <c r="AG20" s="28"/>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:35">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="53" t="s">
-        <v>89</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
       <c r="G21" s="49"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
+      <c r="I21" s="11"/>
       <c r="M21" s="49"/>
       <c r="AE21" s="49"/>
       <c r="AG21" s="28"/>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="49"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
       <c r="M22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AG22" s="28"/>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:35">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="G23" s="49"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
       <c r="M23" s="49"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
       <c r="AE23" s="49"/>
       <c r="AG23" s="28"/>
     </row>
-    <row r="24" spans="1:36">
-      <c r="A24" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="69"/>
+    <row r="24" spans="1:35">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>113</v>
+      </c>
       <c r="G24" s="49"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
       <c r="M24" s="49"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
       <c r="AE24" s="49"/>
       <c r="AG24" s="28"/>
     </row>
-    <row r="25" spans="1:36">
-      <c r="A25" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="G25" s="59"/>
-      <c r="H25" s="10"/>
+    <row r="25" spans="1:35">
+      <c r="A25" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="74"/>
+      <c r="G25" s="49"/>
       <c r="M25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AG25" s="28"/>
     </row>
-    <row r="26" spans="1:36">
-      <c r="A26" s="78" t="s">
-        <v>117</v>
+    <row r="26" spans="1:35">
+      <c r="A26" s="65" t="s">
+        <v>61</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="49"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
+        <v>98</v>
+      </c>
+      <c r="G26" s="59"/>
+      <c r="H26" s="10"/>
       <c r="M26" s="49"/>
       <c r="AE26" s="49"/>
       <c r="AG26" s="28"/>
     </row>
-    <row r="27" spans="1:36">
-      <c r="A27" s="77" t="s">
-        <v>118</v>
+    <row r="27" spans="1:35">
+      <c r="A27" s="66" t="s">
+        <v>116</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G27" s="49"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
       <c r="M27" s="49"/>
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
     </row>
-    <row r="28" spans="1:36">
-      <c r="A28" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="B28" s="53" t="s">
-        <v>86</v>
+    <row r="28" spans="1:35">
+      <c r="A28" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>101</v>
       </c>
       <c r="G28" s="49"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
       <c r="M28" s="49"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
-      <c r="W28" s="10"/>
-      <c r="X28" s="10"/>
-      <c r="Y28" s="10"/>
-      <c r="Z28" s="10"/>
       <c r="AE28" s="49"/>
       <c r="AG28" s="28"/>
     </row>
-    <row r="29" spans="1:36">
-      <c r="A29" s="70" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="71"/>
+    <row r="29" spans="1:35">
+      <c r="A29" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>86</v>
+      </c>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="10"/>
       <c r="AE29" s="49"/>
       <c r="AG29" s="28"/>
     </row>
-    <row r="30" spans="1:36">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>91</v>
-      </c>
+    <row r="30" spans="1:35">
+      <c r="A30" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="76"/>
       <c r="G30" s="49"/>
       <c r="M30" s="49"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
       <c r="AE30" s="49"/>
       <c r="AG30" s="28"/>
-      <c r="AH30" s="52"/>
-      <c r="AI30" s="52"/>
-    </row>
-    <row r="31" spans="1:36">
+    </row>
+    <row r="31" spans="1:35">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="G31" s="49"/>
       <c r="M31" s="49"/>
@@ -1950,25 +1965,26 @@
       <c r="AH31" s="52"/>
       <c r="AI31" s="52"/>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:35">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G32" s="49"/>
       <c r="M32" s="49"/>
       <c r="AE32" s="49"/>
       <c r="AG32" s="28"/>
-      <c r="AJ32" s="52"/>
+      <c r="AH32" s="52"/>
+      <c r="AI32" s="52"/>
     </row>
     <row r="33" spans="1:39">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="G33" s="49"/>
       <c r="M33" s="49"/>
@@ -1977,23 +1993,23 @@
       <c r="AJ33" s="52"/>
     </row>
     <row r="34" spans="1:39">
-      <c r="A34" s="72" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" s="73"/>
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>75</v>
+      </c>
       <c r="G34" s="49"/>
       <c r="M34" s="49"/>
       <c r="AE34" s="49"/>
       <c r="AG34" s="28"/>
+      <c r="AJ34" s="52"/>
     </row>
     <row r="35" spans="1:39">
-      <c r="A35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="12"/>
+      <c r="A35" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="78"/>
       <c r="G35" s="49"/>
       <c r="M35" s="49"/>
       <c r="AE35" s="49"/>
@@ -2001,10 +2017,10 @@
     </row>
     <row r="36" spans="1:39">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="D36" s="12"/>
       <c r="G36" s="49"/>
@@ -2014,145 +2030,94 @@
     </row>
     <row r="37" spans="1:39">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="G37" s="61"/>
+        <v>87</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="G37" s="49"/>
       <c r="M37" s="49"/>
       <c r="AE37" s="49"/>
       <c r="AG37" s="28"/>
     </row>
     <row r="38" spans="1:39">
       <c r="A38" t="s">
-        <v>110</v>
-      </c>
-      <c r="B38" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" s="49"/>
+        <v>67</v>
+      </c>
+      <c r="B38" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="G38" s="61"/>
       <c r="M38" s="49"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
-      <c r="AC38" s="24"/>
-      <c r="AD38" s="24"/>
       <c r="AE38" s="49"/>
       <c r="AG38" s="28"/>
-      <c r="AJ38" s="12"/>
     </row>
     <row r="39" spans="1:39">
-      <c r="A39" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="63"/>
-      <c r="G39" s="49"/>
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="G39" s="51"/>
       <c r="M39" s="49"/>
-      <c r="AE39" s="49"/>
+      <c r="AE39" s="61"/>
       <c r="AG39" s="28"/>
     </row>
     <row r="40" spans="1:39">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+        <v>72</v>
+      </c>
       <c r="G40" s="49"/>
       <c r="M40" s="49"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="AC40" s="24"/>
+      <c r="AD40" s="24"/>
       <c r="AE40" s="49"/>
       <c r="AG40" s="28"/>
-    </row>
-    <row r="41" spans="1:39" s="28" customFormat="1">
-      <c r="A41" s="28" t="s">
+      <c r="AJ40" s="12"/>
+    </row>
+    <row r="41" spans="1:39">
+      <c r="A41" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="68"/>
+      <c r="G41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="AE41" s="49"/>
+      <c r="AG41" s="28"/>
+    </row>
+    <row r="42" spans="1:39">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="G42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="AE42" s="49"/>
+      <c r="AG42" s="28"/>
+    </row>
+    <row r="43" spans="1:39" s="28" customFormat="1">
+      <c r="A43" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B43" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41" s="49"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41" s="49"/>
-      <c r="N41"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
-      <c r="Y41"/>
-      <c r="Z41"/>
-      <c r="AA41"/>
-      <c r="AB41"/>
-      <c r="AC41"/>
-      <c r="AD41"/>
-      <c r="AE41" s="49"/>
-      <c r="AF41"/>
-      <c r="AM41" s="39"/>
-    </row>
-    <row r="42" spans="1:39" s="28" customFormat="1">
-      <c r="A42" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42" s="49"/>
-      <c r="H42"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42" s="49"/>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42"/>
-      <c r="Q42"/>
-      <c r="R42"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42"/>
-      <c r="V42"/>
-      <c r="W42"/>
-      <c r="X42"/>
-      <c r="Y42"/>
-      <c r="Z42"/>
-      <c r="AA42"/>
-      <c r="AB42"/>
-      <c r="AC42"/>
-      <c r="AD42"/>
-      <c r="AE42" s="49"/>
-      <c r="AF42"/>
-    </row>
-    <row r="43" spans="1:39" s="28" customFormat="1">
-      <c r="A43" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43"/>
+      <c r="C43" s="9"/>
       <c r="D43"/>
       <c r="E43"/>
       <c r="F43"/>
@@ -2164,10 +2129,10 @@
       <c r="L43"/>
       <c r="M43" s="49"/>
       <c r="N43"/>
-      <c r="O43"/>
-      <c r="P43"/>
-      <c r="Q43"/>
-      <c r="R43"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
       <c r="S43"/>
       <c r="T43"/>
       <c r="U43"/>
@@ -2178,16 +2143,91 @@
       <c r="Z43"/>
       <c r="AA43"/>
       <c r="AB43"/>
-      <c r="AC43" s="9"/>
-      <c r="AD43" s="9"/>
-      <c r="AE43" s="51"/>
-      <c r="AF43" s="8"/>
-      <c r="AG43" s="54"/>
-      <c r="AH43" s="54"/>
-      <c r="AI43" s="54"/>
-    </row>
-    <row r="44" spans="1:39" s="28" customFormat="1"/>
-    <row r="45" spans="1:39" s="28" customFormat="1"/>
+      <c r="AC43"/>
+      <c r="AD43"/>
+      <c r="AE43" s="49"/>
+      <c r="AF43"/>
+      <c r="AM43" s="39"/>
+    </row>
+    <row r="44" spans="1:39" s="28" customFormat="1">
+      <c r="A44" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44" s="49"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44" s="49"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44"/>
+      <c r="X44"/>
+      <c r="Y44"/>
+      <c r="Z44"/>
+      <c r="AA44"/>
+      <c r="AB44"/>
+      <c r="AC44"/>
+      <c r="AD44"/>
+      <c r="AE44" s="49"/>
+      <c r="AF44"/>
+    </row>
+    <row r="45" spans="1:39" s="28" customFormat="1">
+      <c r="A45" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45" s="49"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45" s="49"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+      <c r="Y45"/>
+      <c r="Z45"/>
+      <c r="AA45"/>
+      <c r="AB45"/>
+      <c r="AC45" s="9"/>
+      <c r="AD45" s="9"/>
+      <c r="AE45" s="51"/>
+      <c r="AF45" s="8"/>
+      <c r="AG45" s="54"/>
+      <c r="AH45" s="54"/>
+      <c r="AI45" s="54"/>
+    </row>
     <row r="46" spans="1:39" s="28" customFormat="1"/>
     <row r="47" spans="1:39" s="28" customFormat="1"/>
     <row r="48" spans="1:39" s="28" customFormat="1"/>
@@ -2216,23 +2256,25 @@
     <row r="71" spans="2:2" s="28" customFormat="1"/>
     <row r="72" spans="2:2" s="28" customFormat="1"/>
     <row r="73" spans="2:2" s="28" customFormat="1"/>
-    <row r="74" spans="2:2">
-      <c r="B74" s="28"/>
-    </row>
-    <row r="75" spans="2:2">
-      <c r="B75" s="28"/>
-    </row>
+    <row r="74" spans="2:2" s="28" customFormat="1"/>
+    <row r="75" spans="2:2" s="28" customFormat="1"/>
     <row r="76" spans="2:2">
       <c r="B76" s="28"/>
     </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="28"/>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="28"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="colorScale" priority="2">
@@ -2343,10 +2385,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" thickTop="1">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="65"/>
+      <c r="B3" s="70"/>
       <c r="G3" s="49"/>
       <c r="M3" s="49"/>
     </row>
@@ -2457,10 +2499,10 @@
       <c r="M11" s="49"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="72"/>
       <c r="G12" s="49"/>
       <c r="M12" s="49"/>
     </row>
@@ -2516,10 +2558,10 @@
       <c r="M16" s="49"/>
     </row>
     <row r="17" spans="1:39">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="69"/>
+      <c r="B17" s="74"/>
       <c r="G17" s="49"/>
       <c r="M17" s="49"/>
     </row>
@@ -2534,10 +2576,10 @@
       <c r="M18" s="49"/>
     </row>
     <row r="19" spans="1:39">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="71"/>
+      <c r="B19" s="76"/>
       <c r="G19" s="49"/>
       <c r="M19" s="49"/>
     </row>
@@ -2582,10 +2624,10 @@
       <c r="M23" s="49"/>
     </row>
     <row r="24" spans="1:39">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="73"/>
+      <c r="B24" s="78"/>
       <c r="G24" s="49"/>
       <c r="M24" s="49"/>
     </row>
@@ -2622,10 +2664,10 @@
       <c r="M27" s="49"/>
     </row>
     <row r="28" spans="1:39">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="63"/>
+      <c r="B28" s="68"/>
       <c r="G28" s="49"/>
       <c r="M28" s="49"/>
     </row>
@@ -2761,10 +2803,10 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="28" customFormat="1" ht="17" thickTop="1">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="65"/>
+      <c r="B36" s="70"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
@@ -2930,10 +2972,10 @@
       <c r="M44"/>
     </row>
     <row r="45" spans="1:13" s="28" customFormat="1">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="67"/>
+      <c r="B45" s="72"/>
       <c r="C45"/>
       <c r="D45"/>
       <c r="E45"/>
@@ -3023,10 +3065,10 @@
       <c r="M49"/>
     </row>
     <row r="50" spans="1:13" s="28" customFormat="1">
-      <c r="A50" s="68" t="s">
+      <c r="A50" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="69"/>
+      <c r="B50" s="74"/>
       <c r="C50"/>
       <c r="D50"/>
       <c r="E50"/>
@@ -3059,10 +3101,10 @@
       <c r="M51" s="10"/>
     </row>
     <row r="52" spans="1:13" s="28" customFormat="1">
-      <c r="A52" s="70" t="s">
+      <c r="A52" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="71"/>
+      <c r="B52" s="76"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
@@ -3152,10 +3194,10 @@
       <c r="M56"/>
     </row>
     <row r="57" spans="1:13" s="28" customFormat="1">
-      <c r="A57" s="72" t="s">
+      <c r="A57" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="73"/>
+      <c r="B57" s="78"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
@@ -3226,10 +3268,10 @@
       <c r="M60"/>
     </row>
     <row r="61" spans="1:13" s="28" customFormat="1">
-      <c r="A61" s="62" t="s">
+      <c r="A61" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="63"/>
+      <c r="B61" s="68"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
@@ -3361,10 +3403,10 @@
       </c>
     </row>
     <row r="69" spans="1:14" ht="17" thickTop="1">
-      <c r="A69" s="64" t="s">
+      <c r="A69" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="65"/>
+      <c r="B69" s="70"/>
       <c r="I69" s="49"/>
       <c r="K69" s="28"/>
       <c r="M69"/>
@@ -3463,10 +3505,10 @@
       <c r="M77"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="66" t="s">
+      <c r="A78" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="67"/>
+      <c r="B78" s="72"/>
       <c r="I78" s="49"/>
       <c r="K78" s="28"/>
       <c r="M78"/>
@@ -3516,10 +3558,10 @@
       <c r="M82"/>
     </row>
     <row r="83" spans="1:14">
-      <c r="A83" s="68" t="s">
+      <c r="A83" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="69"/>
+      <c r="B83" s="74"/>
       <c r="I83" s="49"/>
       <c r="K83" s="28"/>
       <c r="M83"/>
@@ -3538,10 +3580,10 @@
       <c r="M84"/>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="70" t="s">
+      <c r="A85" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="B85" s="71"/>
+      <c r="B85" s="76"/>
       <c r="I85" s="49"/>
       <c r="K85" s="28"/>
       <c r="M85"/>
@@ -3595,10 +3637,10 @@
       <c r="N89" s="52"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="72" t="s">
+      <c r="A90" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="B90" s="73"/>
+      <c r="B90" s="78"/>
       <c r="I90" s="49"/>
       <c r="K90" s="28"/>
       <c r="M90"/>
@@ -3640,10 +3682,10 @@
       <c r="N93" s="12"/>
     </row>
     <row r="94" spans="1:14">
-      <c r="A94" s="62" t="s">
+      <c r="A94" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B94" s="63"/>
+      <c r="B94" s="68"/>
       <c r="I94" s="49"/>
       <c r="K94" s="28"/>
       <c r="M94"/>
@@ -3714,6 +3756,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A94:B94"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A45:B45"/>
@@ -3726,12 +3774,6 @@
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added task to plan 2nd phase of project
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0C5DF9-5F51-0940-A0AA-5AE24FFACFF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAA851E-E381-7349-8342-6C58F809A48B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="127">
   <si>
     <t>Week</t>
   </si>
@@ -422,7 +422,10 @@
     <t>Project Proposal Finalise</t>
   </si>
   <si>
-    <t>Plan the 2nd stage of Project</t>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>Plan 2nd stage of Project</t>
   </si>
 </sst>
 </file>
@@ -702,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -834,8 +837,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1128,7 +1129,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1854,7 +1855,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="M24" s="49"/>
-      <c r="N24" s="11"/>
+      <c r="N24" s="9"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
@@ -1877,6 +1878,7 @@
       <c r="B25" s="74"/>
       <c r="G25" s="49"/>
       <c r="M25" s="49"/>
+      <c r="N25" s="9"/>
       <c r="AE25" s="49"/>
       <c r="AG25" s="28"/>
     </row>
@@ -1890,6 +1892,7 @@
       <c r="G26" s="59"/>
       <c r="H26" s="10"/>
       <c r="M26" s="49"/>
+      <c r="N26" s="9"/>
       <c r="AE26" s="49"/>
       <c r="AG26" s="28"/>
     </row>
@@ -1904,6 +1907,7 @@
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
       <c r="M27" s="49"/>
+      <c r="N27" s="9"/>
       <c r="AE27" s="49"/>
       <c r="AG27" s="28"/>
     </row>
@@ -1919,6 +1923,7 @@
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="M28" s="49"/>
+      <c r="N28" s="9"/>
       <c r="AE28" s="49"/>
       <c r="AG28" s="28"/>
     </row>
@@ -1931,7 +1936,7 @@
       </c>
       <c r="G29" s="49"/>
       <c r="M29" s="49"/>
-      <c r="N29" s="10"/>
+      <c r="N29" s="9"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
@@ -2062,18 +2067,22 @@
       <c r="AE38" s="49"/>
       <c r="AG38" s="28"/>
     </row>
-    <row r="39" spans="1:39" s="12" customFormat="1">
-      <c r="B39" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="G39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="AE39" s="61"/>
-      <c r="AG39" s="80"/>
+    <row r="39" spans="1:39" s="9" customFormat="1">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="G39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="12"/>
+      <c r="AE39" s="51"/>
+      <c r="AG39" s="24"/>
     </row>
     <row r="40" spans="1:39">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B40" s="53" t="s">
         <v>120</v>
@@ -2086,7 +2095,7 @@
     </row>
     <row r="41" spans="1:39">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B41" s="44" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Updated the work plan to current version
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51A81C0-49B4-FA4C-8699-1DA4318E7D5F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CE85AB-A9B2-0749-87B2-907727E3848F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
+    <sheet name="Project Proposal (Print)" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="90">
   <si>
     <t>Week</t>
   </si>
@@ -466,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -558,6 +559,17 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,11 +858,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
   <dimension ref="A1:AM79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2046,4 +2058,2662 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB78A94-45E5-D041-A9F3-CF4F27E90595}">
+  <dimension ref="A1:AJ137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="9.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="9" customWidth="1"/>
+    <col min="14" max="36" width="9.1640625" customWidth="1"/>
+    <col min="37" max="37" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" hidden="1">
+      <c r="B1" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+      <c r="AI1">
+        <v>33</v>
+      </c>
+      <c r="AJ1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" hidden="1">
+      <c r="B2" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="32">
+        <f>SUM(100/$AJ$1*C1)/100</f>
+        <v>2.9411764705882356E-2</v>
+      </c>
+      <c r="D2" s="32">
+        <f t="shared" ref="D2:K2" si="0">SUM(100/$AJ$1*D1)/100</f>
+        <v>5.8823529411764712E-2</v>
+      </c>
+      <c r="E2" s="32">
+        <f t="shared" si="0"/>
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="F2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.11764705882352942</v>
+      </c>
+      <c r="G2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.14705882352941177</v>
+      </c>
+      <c r="H2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="I2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.20588235294117649</v>
+      </c>
+      <c r="J2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.23529411764705885</v>
+      </c>
+      <c r="K2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.26470588235294118</v>
+      </c>
+      <c r="L2" s="32">
+        <f t="shared" ref="L2:AJ2" si="1">SUM(100/$AJ$1*L1)/100</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="M2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.32352941176470595</v>
+      </c>
+      <c r="N2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="O2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.38235294117647056</v>
+      </c>
+      <c r="P2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.41176470588235298</v>
+      </c>
+      <c r="Q2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.44117647058823534</v>
+      </c>
+      <c r="R2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.4705882352941177</v>
+      </c>
+      <c r="S2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="T2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.52941176470588236</v>
+      </c>
+      <c r="U2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.55882352941176483</v>
+      </c>
+      <c r="V2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="W2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.61764705882352944</v>
+      </c>
+      <c r="X2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.64705882352941191</v>
+      </c>
+      <c r="Y2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="Z2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="AA2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.73529411764705888</v>
+      </c>
+      <c r="AB2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="AC2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.79411764705882359</v>
+      </c>
+      <c r="AD2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.82352941176470595</v>
+      </c>
+      <c r="AE2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.85294117647058831</v>
+      </c>
+      <c r="AF2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.88235294117647067</v>
+      </c>
+      <c r="AG2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.91176470588235303</v>
+      </c>
+      <c r="AH2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.94117647058823539</v>
+      </c>
+      <c r="AI2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.97058823529411764</v>
+      </c>
+      <c r="AJ2" s="32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" s="1" customFormat="1" ht="139">
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+    </row>
+    <row r="4" spans="1:36" ht="17" thickBot="1">
+      <c r="A4" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>43367</v>
+      </c>
+      <c r="D4" s="16">
+        <v>43374</v>
+      </c>
+      <c r="E4" s="16">
+        <v>43381</v>
+      </c>
+      <c r="F4" s="16">
+        <v>43388</v>
+      </c>
+      <c r="G4" s="18">
+        <v>43395</v>
+      </c>
+      <c r="H4" s="16">
+        <v>43402</v>
+      </c>
+      <c r="I4" s="16">
+        <v>43409</v>
+      </c>
+      <c r="J4" s="16">
+        <v>43416</v>
+      </c>
+      <c r="K4" s="16">
+        <v>43423</v>
+      </c>
+      <c r="L4" s="16">
+        <v>43430</v>
+      </c>
+      <c r="M4" s="18">
+        <v>43437</v>
+      </c>
+      <c r="N4" s="16">
+        <v>43444</v>
+      </c>
+      <c r="O4" s="16">
+        <v>43451</v>
+      </c>
+      <c r="P4" s="16">
+        <v>43458</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>43465</v>
+      </c>
+      <c r="R4" s="16">
+        <v>43472</v>
+      </c>
+      <c r="S4" s="16">
+        <v>43479</v>
+      </c>
+      <c r="T4" s="16">
+        <v>43486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="17" thickTop="1">
+      <c r="A5" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="G5" s="19"/>
+      <c r="M5" s="19"/>
+    </row>
+    <row r="6" spans="1:36">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="19"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="20"/>
+      <c r="M7" s="19"/>
+    </row>
+    <row r="8" spans="1:36">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="21"/>
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="21"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="2"/>
+      <c r="M9" s="19"/>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="21"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="M10" s="19"/>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="21"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="21"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="M17" s="19"/>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="42"/>
+      <c r="G18" s="19"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="19"/>
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="6"/>
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="M22" s="19"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="M23" s="19"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="44"/>
+      <c r="G25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="5"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="46"/>
+      <c r="G30" s="19"/>
+      <c r="M30" s="19"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="M31" s="19"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="M32" s="19"/>
+    </row>
+    <row r="33" spans="1:30">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="19"/>
+      <c r="M33" s="19"/>
+    </row>
+    <row r="34" spans="1:30">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="19"/>
+      <c r="M34" s="19"/>
+    </row>
+    <row r="35" spans="1:30">
+      <c r="A35" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="48"/>
+      <c r="G35" s="19"/>
+      <c r="M35" s="19"/>
+    </row>
+    <row r="36" spans="1:30">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="G36" s="19"/>
+      <c r="M36" s="19"/>
+    </row>
+    <row r="37" spans="1:30">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="G37" s="19"/>
+      <c r="M37" s="19"/>
+    </row>
+    <row r="38" spans="1:30">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="G38" s="31"/>
+      <c r="M38" s="19"/>
+    </row>
+    <row r="39" spans="1:30" s="4" customFormat="1">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="7"/>
+    </row>
+    <row r="40" spans="1:30">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="G40" s="21"/>
+      <c r="M40" s="19"/>
+    </row>
+    <row r="41" spans="1:30">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+    </row>
+    <row r="42" spans="1:30">
+      <c r="A42" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="38"/>
+      <c r="G42" s="19"/>
+      <c r="M42" s="19"/>
+    </row>
+    <row r="43" spans="1:30">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="G43" s="19"/>
+      <c r="M43" s="19"/>
+    </row>
+    <row r="44" spans="1:30" s="9" customFormat="1">
+      <c r="A44" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44" s="19"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44" s="19"/>
+      <c r="N44"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44"/>
+      <c r="T44"/>
+    </row>
+    <row r="45" spans="1:30" s="9" customFormat="1">
+      <c r="A45" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45" s="19"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45" s="19"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+    </row>
+    <row r="46" spans="1:30" s="9" customFormat="1">
+      <c r="A46" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46" s="19"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46" s="19"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+    </row>
+    <row r="47" spans="1:30" s="9" customFormat="1"/>
+    <row r="48" spans="1:30" s="9" customFormat="1" ht="75">
+      <c r="A48" s="1"/>
+      <c r="B48" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N48" s="12"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1"/>
+      <c r="AD48" s="1"/>
+    </row>
+    <row r="49" spans="1:30" s="9" customFormat="1" ht="17" thickBot="1">
+      <c r="A49" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="16">
+        <v>43493</v>
+      </c>
+      <c r="D49" s="16">
+        <v>43500</v>
+      </c>
+      <c r="E49" s="16">
+        <v>43507</v>
+      </c>
+      <c r="F49" s="16">
+        <v>43514</v>
+      </c>
+      <c r="G49" s="16">
+        <v>43521</v>
+      </c>
+      <c r="H49" s="16">
+        <v>43528</v>
+      </c>
+      <c r="I49" s="16">
+        <v>43535</v>
+      </c>
+      <c r="J49" s="16">
+        <v>43542</v>
+      </c>
+      <c r="K49" s="16">
+        <v>43549</v>
+      </c>
+      <c r="L49" s="16">
+        <v>43556</v>
+      </c>
+      <c r="M49" s="18">
+        <v>43563</v>
+      </c>
+      <c r="N49" s="16">
+        <v>43570</v>
+      </c>
+      <c r="O49" s="16">
+        <v>43577</v>
+      </c>
+      <c r="P49" s="16">
+        <v>43584</v>
+      </c>
+      <c r="Q49" s="16">
+        <v>43591</v>
+      </c>
+      <c r="R49" s="16">
+        <v>43598</v>
+      </c>
+      <c r="Z49"/>
+      <c r="AA49"/>
+      <c r="AB49"/>
+      <c r="AC49"/>
+      <c r="AD49"/>
+    </row>
+    <row r="50" spans="1:30" s="9" customFormat="1" ht="17" thickTop="1">
+      <c r="A50" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="40"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50" s="19"/>
+      <c r="N50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="Z50"/>
+      <c r="AA50"/>
+      <c r="AB50"/>
+      <c r="AC50"/>
+      <c r="AD50"/>
+    </row>
+    <row r="51" spans="1:30" s="9" customFormat="1">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51" s="19"/>
+      <c r="N51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="Z51"/>
+      <c r="AA51"/>
+      <c r="AB51"/>
+      <c r="AC51"/>
+      <c r="AD51"/>
+    </row>
+    <row r="52" spans="1:30" s="9" customFormat="1">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52" s="19"/>
+      <c r="N52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="Z52"/>
+      <c r="AA52"/>
+      <c r="AB52"/>
+      <c r="AC52"/>
+      <c r="AD52"/>
+    </row>
+    <row r="53" spans="1:30" s="9" customFormat="1">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53" s="19"/>
+      <c r="N53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="Z53"/>
+      <c r="AA53"/>
+      <c r="AB53"/>
+      <c r="AC53"/>
+      <c r="AD53"/>
+    </row>
+    <row r="54" spans="1:30" s="9" customFormat="1">
+      <c r="A54" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54" s="19"/>
+      <c r="N54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="Z54"/>
+      <c r="AA54"/>
+      <c r="AB54"/>
+      <c r="AC54"/>
+      <c r="AD54"/>
+    </row>
+    <row r="55" spans="1:30" s="9" customFormat="1">
+      <c r="A55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55" s="19"/>
+      <c r="N55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="Z55"/>
+      <c r="AA55"/>
+      <c r="AB55"/>
+      <c r="AC55"/>
+      <c r="AD55"/>
+    </row>
+    <row r="56" spans="1:30" s="9" customFormat="1">
+      <c r="A56" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56" s="19"/>
+      <c r="N56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="Z56"/>
+      <c r="AA56"/>
+      <c r="AB56"/>
+      <c r="AC56"/>
+      <c r="AD56"/>
+    </row>
+    <row r="57" spans="1:30" s="9" customFormat="1">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57" s="19"/>
+      <c r="N57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="Z57"/>
+      <c r="AA57"/>
+      <c r="AB57"/>
+      <c r="AC57"/>
+      <c r="AD57"/>
+    </row>
+    <row r="58" spans="1:30" s="9" customFormat="1">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="4"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="Z58"/>
+      <c r="AA58"/>
+      <c r="AB58"/>
+      <c r="AC58"/>
+      <c r="AD58"/>
+    </row>
+    <row r="59" spans="1:30" s="9" customFormat="1">
+      <c r="A59" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="21"/>
+      <c r="N59" s="4"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="Z59"/>
+      <c r="AA59"/>
+      <c r="AB59"/>
+      <c r="AC59"/>
+      <c r="AD59"/>
+    </row>
+    <row r="60" spans="1:30" s="9" customFormat="1">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="21"/>
+      <c r="N60" s="4"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="Z60"/>
+      <c r="AA60"/>
+      <c r="AB60"/>
+      <c r="AC60"/>
+      <c r="AD60"/>
+    </row>
+    <row r="61" spans="1:30" s="9" customFormat="1">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="4"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="Z61"/>
+      <c r="AA61"/>
+      <c r="AB61"/>
+      <c r="AC61"/>
+      <c r="AD61"/>
+    </row>
+    <row r="62" spans="1:30" s="9" customFormat="1">
+      <c r="A62" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="4"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="Z62"/>
+      <c r="AA62"/>
+      <c r="AB62"/>
+      <c r="AC62"/>
+      <c r="AD62"/>
+    </row>
+    <row r="63" spans="1:30" s="9" customFormat="1">
+      <c r="A63" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="42"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63" s="19"/>
+      <c r="N63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="Z63"/>
+      <c r="AA63"/>
+      <c r="AB63"/>
+      <c r="AC63"/>
+      <c r="AD63"/>
+    </row>
+    <row r="64" spans="1:30" s="9" customFormat="1">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64" s="19"/>
+      <c r="N64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="Z64"/>
+      <c r="AA64"/>
+      <c r="AB64"/>
+      <c r="AC64"/>
+      <c r="AD64"/>
+    </row>
+    <row r="65" spans="1:30" s="9" customFormat="1">
+      <c r="A65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65" s="19"/>
+      <c r="N65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="Z65"/>
+      <c r="AA65"/>
+      <c r="AB65"/>
+      <c r="AC65"/>
+      <c r="AD65"/>
+    </row>
+    <row r="66" spans="1:30" s="9" customFormat="1">
+      <c r="A66" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66" s="19"/>
+      <c r="N66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="Z66"/>
+      <c r="AA66"/>
+      <c r="AB66"/>
+      <c r="AC66"/>
+      <c r="AD66"/>
+    </row>
+    <row r="67" spans="1:30" s="9" customFormat="1">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67" s="19"/>
+      <c r="N67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="Z67"/>
+      <c r="AA67"/>
+      <c r="AB67"/>
+      <c r="AC67"/>
+      <c r="AD67"/>
+    </row>
+    <row r="68" spans="1:30" s="9" customFormat="1">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+      <c r="H68"/>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68" s="19"/>
+      <c r="N68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+      <c r="R68"/>
+      <c r="Z68"/>
+      <c r="AA68"/>
+      <c r="AB68"/>
+      <c r="AC68"/>
+      <c r="AD68"/>
+    </row>
+    <row r="69" spans="1:30" s="9" customFormat="1">
+      <c r="A69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69" s="19"/>
+      <c r="N69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
+      <c r="R69"/>
+      <c r="Z69"/>
+      <c r="AA69"/>
+      <c r="AB69"/>
+      <c r="AC69"/>
+      <c r="AD69"/>
+    </row>
+    <row r="70" spans="1:30" s="9" customFormat="1">
+      <c r="A70" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="44"/>
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70" s="19"/>
+      <c r="N70"/>
+      <c r="P70"/>
+      <c r="Q70"/>
+      <c r="R70"/>
+      <c r="Z70"/>
+      <c r="AA70"/>
+      <c r="AB70"/>
+      <c r="AC70"/>
+      <c r="AD70"/>
+    </row>
+    <row r="71" spans="1:30" s="9" customFormat="1">
+      <c r="A71" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71" s="19"/>
+      <c r="N71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="Z71"/>
+      <c r="AA71"/>
+      <c r="AB71"/>
+      <c r="AC71"/>
+      <c r="AD71"/>
+    </row>
+    <row r="72" spans="1:30" s="9" customFormat="1">
+      <c r="A72" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72" s="19"/>
+      <c r="N72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="Z72"/>
+      <c r="AA72"/>
+      <c r="AB72"/>
+      <c r="AC72"/>
+      <c r="AD72"/>
+    </row>
+    <row r="73" spans="1:30" s="9" customFormat="1">
+      <c r="A73" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+      <c r="H73"/>
+      <c r="I73"/>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="M73" s="19"/>
+      <c r="N73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
+      <c r="R73"/>
+      <c r="Z73"/>
+      <c r="AA73"/>
+      <c r="AB73"/>
+      <c r="AC73"/>
+      <c r="AD73"/>
+    </row>
+    <row r="74" spans="1:30" s="9" customFormat="1">
+      <c r="A74" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74" s="19"/>
+      <c r="N74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
+      <c r="R74"/>
+      <c r="Z74"/>
+      <c r="AA74"/>
+      <c r="AB74"/>
+      <c r="AC74"/>
+      <c r="AD74"/>
+    </row>
+    <row r="75" spans="1:30" s="9" customFormat="1">
+      <c r="A75" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75" s="46"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
+      <c r="H75"/>
+      <c r="I75"/>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75" s="19"/>
+      <c r="N75"/>
+      <c r="P75"/>
+      <c r="Q75"/>
+      <c r="R75"/>
+      <c r="Z75"/>
+      <c r="AA75"/>
+      <c r="AB75"/>
+      <c r="AC75"/>
+      <c r="AD75"/>
+    </row>
+    <row r="76" spans="1:30" s="9" customFormat="1">
+      <c r="A76" t="s">
+        <v>27</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76"/>
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76" s="19"/>
+      <c r="N76"/>
+      <c r="P76" s="22"/>
+      <c r="Q76" s="22"/>
+      <c r="R76"/>
+      <c r="Z76"/>
+      <c r="AA76"/>
+      <c r="AB76"/>
+      <c r="AC76"/>
+      <c r="AD76"/>
+    </row>
+    <row r="77" spans="1:30">
+      <c r="A77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M77" s="19"/>
+      <c r="O77" s="9"/>
+      <c r="P77" s="22"/>
+      <c r="Q77" s="22"/>
+    </row>
+    <row r="78" spans="1:30">
+      <c r="A78" t="s">
+        <v>29</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M78" s="19"/>
+      <c r="O78" s="9"/>
+      <c r="R78" s="22"/>
+    </row>
+    <row r="79" spans="1:30">
+      <c r="A79" t="s">
+        <v>39</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M79" s="19"/>
+      <c r="O79" s="9"/>
+      <c r="R79" s="22"/>
+    </row>
+    <row r="80" spans="1:30">
+      <c r="A80" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80" s="48"/>
+      <c r="M80" s="19"/>
+      <c r="O80" s="9"/>
+    </row>
+    <row r="81" spans="1:30">
+      <c r="A81" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M81" s="19"/>
+      <c r="O81" s="9"/>
+    </row>
+    <row r="82" spans="1:30">
+      <c r="A82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M82" s="19"/>
+      <c r="O82" s="9"/>
+    </row>
+    <row r="83" spans="1:30">
+      <c r="A83" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="M83" s="19"/>
+      <c r="O83" s="9"/>
+    </row>
+    <row r="84" spans="1:30">
+      <c r="A84" t="s">
+        <v>72</v>
+      </c>
+      <c r="B84" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="21"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="8"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="4"/>
+      <c r="Z84" s="4"/>
+      <c r="AA84" s="4"/>
+      <c r="AB84" s="4"/>
+      <c r="AC84" s="4"/>
+      <c r="AD84" s="4"/>
+    </row>
+    <row r="85" spans="1:30">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="M85" s="31"/>
+      <c r="O85" s="9"/>
+    </row>
+    <row r="86" spans="1:30">
+      <c r="A86" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="19"/>
+      <c r="O86" s="9"/>
+      <c r="R86" s="7"/>
+    </row>
+    <row r="87" spans="1:30">
+      <c r="A87" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="38"/>
+      <c r="M87" s="19"/>
+      <c r="O87" s="9"/>
+    </row>
+    <row r="88" spans="1:30">
+      <c r="A88" t="s">
+        <v>33</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="M88" s="19"/>
+      <c r="O88" s="9"/>
+    </row>
+    <row r="89" spans="1:30">
+      <c r="A89" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M89" s="19"/>
+      <c r="O89" s="9"/>
+      <c r="P89" s="9"/>
+      <c r="Q89" s="9"/>
+      <c r="R89" s="9"/>
+      <c r="Z89" s="9"/>
+      <c r="AA89" s="9"/>
+      <c r="AB89" s="11"/>
+      <c r="AC89" s="9"/>
+      <c r="AD89" s="9"/>
+    </row>
+    <row r="90" spans="1:30">
+      <c r="A90" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M90" s="19"/>
+      <c r="O90" s="9"/>
+      <c r="P90" s="9"/>
+      <c r="Q90" s="9"/>
+      <c r="R90" s="9"/>
+      <c r="Z90" s="9"/>
+      <c r="AA90" s="9"/>
+      <c r="AB90" s="9"/>
+      <c r="AC90" s="9"/>
+      <c r="AD90" s="9"/>
+    </row>
+    <row r="91" spans="1:30">
+      <c r="A91" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="21"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="24"/>
+      <c r="P91" s="24"/>
+      <c r="Q91" s="24"/>
+      <c r="R91" s="9"/>
+      <c r="Z91" s="9"/>
+      <c r="AA91" s="9"/>
+      <c r="AB91" s="9"/>
+      <c r="AC91" s="9"/>
+      <c r="AD91" s="9"/>
+    </row>
+    <row r="93" spans="1:30">
+      <c r="A93" s="50"/>
+      <c r="B93" s="51"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
+      <c r="L93" s="8"/>
+      <c r="M93" s="8"/>
+    </row>
+    <row r="94" spans="1:30">
+      <c r="A94" s="52"/>
+      <c r="B94" s="52"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8"/>
+      <c r="L94" s="8"/>
+      <c r="M94" s="8"/>
+    </row>
+    <row r="95" spans="1:30">
+      <c r="A95" s="49"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="8"/>
+    </row>
+    <row r="96" spans="1:30">
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="8"/>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="8"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="8"/>
+      <c r="J97" s="8"/>
+      <c r="K97" s="8"/>
+      <c r="L97" s="8"/>
+      <c r="M97" s="8"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="8"/>
+      <c r="I98" s="8"/>
+      <c r="J98" s="8"/>
+      <c r="K98" s="8"/>
+      <c r="L98" s="8"/>
+      <c r="M98" s="8"/>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="8"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="8"/>
+      <c r="L99" s="8"/>
+      <c r="M99" s="8"/>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="8"/>
+      <c r="L100" s="8"/>
+      <c r="M100" s="8"/>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" s="8"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="8"/>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" s="8"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="8"/>
+      <c r="J102" s="8"/>
+      <c r="K102" s="8"/>
+      <c r="L102" s="8"/>
+      <c r="M102" s="8"/>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103" s="8"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="8"/>
+      <c r="I103" s="8"/>
+      <c r="J103" s="8"/>
+      <c r="K103" s="8"/>
+      <c r="L103" s="8"/>
+      <c r="M103" s="8"/>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="A104" s="8"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="8"/>
+      <c r="K104" s="8"/>
+      <c r="L104" s="8"/>
+      <c r="M104" s="8"/>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="A105" s="8"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="8"/>
+      <c r="K105" s="8"/>
+      <c r="L105" s="8"/>
+      <c r="M105" s="8"/>
+    </row>
+    <row r="106" spans="1:13">
+      <c r="A106" s="8"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
+      <c r="J106" s="8"/>
+      <c r="K106" s="8"/>
+      <c r="L106" s="8"/>
+      <c r="M106" s="8"/>
+    </row>
+    <row r="107" spans="1:13">
+      <c r="A107" s="8"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="8"/>
+      <c r="I107" s="8"/>
+      <c r="J107" s="8"/>
+      <c r="K107" s="8"/>
+      <c r="L107" s="8"/>
+      <c r="M107" s="8"/>
+    </row>
+    <row r="108" spans="1:13">
+      <c r="A108" s="49"/>
+      <c r="B108" s="49"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
+      <c r="I108" s="8"/>
+      <c r="J108" s="8"/>
+      <c r="K108" s="8"/>
+      <c r="L108" s="8"/>
+      <c r="M108" s="8"/>
+    </row>
+    <row r="109" spans="1:13">
+      <c r="A109" s="8"/>
+      <c r="B109" s="53"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+      <c r="G109" s="8"/>
+      <c r="H109" s="8"/>
+      <c r="I109" s="8"/>
+      <c r="J109" s="8"/>
+      <c r="K109" s="8"/>
+      <c r="L109" s="8"/>
+      <c r="M109" s="8"/>
+    </row>
+    <row r="110" spans="1:13">
+      <c r="A110" s="8"/>
+      <c r="B110" s="53"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="G110" s="8"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8"/>
+      <c r="J110" s="8"/>
+      <c r="K110" s="8"/>
+      <c r="L110" s="8"/>
+      <c r="M110" s="8"/>
+    </row>
+    <row r="111" spans="1:13">
+      <c r="A111" s="8"/>
+      <c r="B111" s="53"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="8"/>
+      <c r="H111" s="8"/>
+      <c r="I111" s="8"/>
+      <c r="J111" s="8"/>
+      <c r="K111" s="8"/>
+      <c r="L111" s="8"/>
+      <c r="M111" s="8"/>
+    </row>
+    <row r="112" spans="1:13">
+      <c r="A112" s="8"/>
+      <c r="B112" s="53"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="8"/>
+      <c r="H112" s="8"/>
+      <c r="I112" s="8"/>
+      <c r="J112" s="8"/>
+      <c r="K112" s="8"/>
+      <c r="L112" s="8"/>
+      <c r="M112" s="8"/>
+    </row>
+    <row r="113" spans="1:13">
+      <c r="A113" s="8"/>
+      <c r="B113" s="53"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="8"/>
+      <c r="I113" s="8"/>
+      <c r="J113" s="8"/>
+      <c r="K113" s="8"/>
+      <c r="L113" s="8"/>
+      <c r="M113" s="8"/>
+    </row>
+    <row r="114" spans="1:13">
+      <c r="A114" s="8"/>
+      <c r="B114" s="53"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="8"/>
+      <c r="H114" s="8"/>
+      <c r="I114" s="8"/>
+      <c r="J114" s="8"/>
+      <c r="K114" s="8"/>
+      <c r="L114" s="8"/>
+      <c r="M114" s="8"/>
+    </row>
+    <row r="115" spans="1:13">
+      <c r="A115" s="49"/>
+      <c r="B115" s="49"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
+      <c r="F115" s="8"/>
+      <c r="G115" s="8"/>
+      <c r="H115" s="8"/>
+      <c r="I115" s="8"/>
+      <c r="J115" s="8"/>
+      <c r="K115" s="8"/>
+      <c r="L115" s="8"/>
+      <c r="M115" s="8"/>
+    </row>
+    <row r="116" spans="1:13">
+      <c r="A116" s="36"/>
+      <c r="B116" s="36"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8"/>
+      <c r="I116" s="8"/>
+      <c r="J116" s="8"/>
+      <c r="K116" s="8"/>
+      <c r="L116" s="8"/>
+      <c r="M116" s="8"/>
+    </row>
+    <row r="117" spans="1:13">
+      <c r="A117" s="36"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="8"/>
+      <c r="I117" s="8"/>
+      <c r="J117" s="8"/>
+      <c r="K117" s="8"/>
+      <c r="L117" s="8"/>
+      <c r="M117" s="8"/>
+    </row>
+    <row r="118" spans="1:13">
+      <c r="A118" s="36"/>
+      <c r="B118" s="36"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
+      <c r="J118" s="8"/>
+      <c r="K118" s="8"/>
+      <c r="L118" s="8"/>
+      <c r="M118" s="8"/>
+    </row>
+    <row r="119" spans="1:13">
+      <c r="A119" s="36"/>
+      <c r="B119" s="53"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="8"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="8"/>
+      <c r="I119" s="8"/>
+      <c r="J119" s="8"/>
+      <c r="K119" s="8"/>
+      <c r="L119" s="8"/>
+      <c r="M119" s="8"/>
+    </row>
+    <row r="120" spans="1:13">
+      <c r="A120" s="49"/>
+      <c r="B120" s="49"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="8"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8"/>
+      <c r="I120" s="8"/>
+      <c r="J120" s="8"/>
+      <c r="K120" s="8"/>
+      <c r="L120" s="8"/>
+      <c r="M120" s="8"/>
+    </row>
+    <row r="121" spans="1:13">
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+      <c r="I121" s="8"/>
+      <c r="J121" s="8"/>
+      <c r="K121" s="8"/>
+      <c r="L121" s="8"/>
+      <c r="M121" s="8"/>
+    </row>
+    <row r="122" spans="1:13">
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
+      <c r="J122" s="8"/>
+      <c r="K122" s="8"/>
+      <c r="L122" s="8"/>
+      <c r="M122" s="8"/>
+    </row>
+    <row r="123" spans="1:13">
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="8"/>
+      <c r="I123" s="8"/>
+      <c r="J123" s="8"/>
+      <c r="K123" s="8"/>
+      <c r="L123" s="8"/>
+      <c r="M123" s="8"/>
+    </row>
+    <row r="124" spans="1:13">
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+      <c r="F124" s="8"/>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
+      <c r="I124" s="8"/>
+      <c r="J124" s="8"/>
+      <c r="K124" s="8"/>
+      <c r="L124" s="8"/>
+      <c r="M124" s="8"/>
+    </row>
+    <row r="125" spans="1:13">
+      <c r="A125" s="49"/>
+      <c r="B125" s="49"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8"/>
+      <c r="F125" s="8"/>
+      <c r="G125" s="8"/>
+      <c r="H125" s="8"/>
+      <c r="I125" s="8"/>
+      <c r="J125" s="8"/>
+      <c r="K125" s="8"/>
+      <c r="L125" s="8"/>
+      <c r="M125" s="8"/>
+    </row>
+    <row r="126" spans="1:13">
+      <c r="A126" s="8"/>
+      <c r="B126" s="53"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
+      <c r="F126" s="8"/>
+      <c r="G126" s="8"/>
+      <c r="H126" s="8"/>
+      <c r="I126" s="8"/>
+      <c r="J126" s="8"/>
+      <c r="K126" s="8"/>
+      <c r="L126" s="8"/>
+      <c r="M126" s="8"/>
+    </row>
+    <row r="127" spans="1:13">
+      <c r="A127" s="8"/>
+      <c r="B127" s="53"/>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
+      <c r="I127" s="8"/>
+      <c r="J127" s="8"/>
+      <c r="K127" s="8"/>
+      <c r="L127" s="8"/>
+      <c r="M127" s="8"/>
+    </row>
+    <row r="128" spans="1:13">
+      <c r="A128" s="8"/>
+      <c r="B128" s="53"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+      <c r="F128" s="8"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
+      <c r="I128" s="8"/>
+      <c r="J128" s="8"/>
+      <c r="K128" s="8"/>
+      <c r="L128" s="8"/>
+      <c r="M128" s="8"/>
+    </row>
+    <row r="129" spans="1:13">
+      <c r="A129" s="8"/>
+      <c r="B129" s="53"/>
+      <c r="C129" s="8"/>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8"/>
+      <c r="F129" s="8"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="8"/>
+      <c r="I129" s="8"/>
+      <c r="J129" s="8"/>
+      <c r="K129" s="8"/>
+      <c r="L129" s="8"/>
+      <c r="M129" s="8"/>
+    </row>
+    <row r="130" spans="1:13">
+      <c r="A130" s="8"/>
+      <c r="B130" s="53"/>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8"/>
+      <c r="J130" s="8"/>
+      <c r="K130" s="8"/>
+      <c r="L130" s="8"/>
+      <c r="M130" s="8"/>
+    </row>
+    <row r="131" spans="1:13">
+      <c r="A131" s="8"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="8"/>
+      <c r="D131" s="8"/>
+      <c r="E131" s="8"/>
+      <c r="F131" s="8"/>
+      <c r="G131" s="8"/>
+      <c r="H131" s="8"/>
+      <c r="I131" s="8"/>
+      <c r="J131" s="8"/>
+      <c r="K131" s="8"/>
+      <c r="L131" s="8"/>
+      <c r="M131" s="8"/>
+    </row>
+    <row r="132" spans="1:13">
+      <c r="A132" s="49"/>
+      <c r="B132" s="49"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
+      <c r="I132" s="8"/>
+      <c r="J132" s="8"/>
+      <c r="K132" s="8"/>
+      <c r="L132" s="8"/>
+      <c r="M132" s="8"/>
+    </row>
+    <row r="133" spans="1:13">
+      <c r="A133" s="8"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="8"/>
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
+      <c r="I133" s="8"/>
+      <c r="J133" s="8"/>
+      <c r="K133" s="8"/>
+      <c r="L133" s="8"/>
+      <c r="M133" s="8"/>
+    </row>
+    <row r="134" spans="1:13">
+      <c r="A134" s="8"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8"/>
+      <c r="J134" s="8"/>
+      <c r="K134" s="8"/>
+      <c r="L134" s="8"/>
+      <c r="M134" s="8"/>
+    </row>
+    <row r="135" spans="1:13">
+      <c r="A135" s="8"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="8"/>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8"/>
+      <c r="F135" s="8"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
+      <c r="I135" s="8"/>
+      <c r="J135" s="8"/>
+      <c r="K135" s="8"/>
+      <c r="L135" s="8"/>
+      <c r="M135" s="8"/>
+    </row>
+    <row r="136" spans="1:13">
+      <c r="A136" s="8"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
+      <c r="F136" s="8"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="8"/>
+      <c r="J136" s="8"/>
+      <c r="K136" s="8"/>
+      <c r="L136" s="8"/>
+      <c r="M136" s="8"/>
+    </row>
+    <row r="137" spans="1:13">
+      <c r="A137" s="8"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="8"/>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
+      <c r="F137" s="8"/>
+      <c r="G137" s="8"/>
+      <c r="H137" s="8"/>
+      <c r="I137" s="8"/>
+      <c r="J137" s="8"/>
+      <c r="K137" s="8"/>
+      <c r="L137" s="8"/>
+      <c r="M137" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A42:B42"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:AJ2">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created active section of the work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EB66A9-D876-DA4E-B804-05108C338C20}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4CF0F-F239-814A-BD06-F1A281F67C84}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="39760" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Project Proposal" sheetId="7" r:id="rId1"/>
-    <sheet name="Project Proposal (Print)" sheetId="9" r:id="rId2"/>
+    <sheet name="Active WorkPlan" sheetId="10" r:id="rId1"/>
+    <sheet name="Project Proposal" sheetId="7" r:id="rId2"/>
+    <sheet name="Project Proposal (Print)" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="93">
   <si>
     <t>Week</t>
   </si>
@@ -864,11 +865,1217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13957A64-6344-8943-90F3-268E017FF0FC}">
+  <dimension ref="A1:AM79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="9.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="9" customWidth="1"/>
+    <col min="14" max="36" width="9.1640625" customWidth="1"/>
+    <col min="37" max="37" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36">
+      <c r="B1" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+      <c r="AI1">
+        <v>33</v>
+      </c>
+      <c r="AJ1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
+      <c r="B2" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="32">
+        <f>SUM(100/$AJ$1*C1)/100</f>
+        <v>2.9411764705882356E-2</v>
+      </c>
+      <c r="D2" s="32">
+        <f t="shared" ref="D2:K2" si="0">SUM(100/$AJ$1*D1)/100</f>
+        <v>5.8823529411764712E-2</v>
+      </c>
+      <c r="E2" s="32">
+        <f t="shared" si="0"/>
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="F2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.11764705882352942</v>
+      </c>
+      <c r="G2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.14705882352941177</v>
+      </c>
+      <c r="H2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="I2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.20588235294117649</v>
+      </c>
+      <c r="J2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.23529411764705885</v>
+      </c>
+      <c r="K2" s="32">
+        <f t="shared" si="0"/>
+        <v>0.26470588235294118</v>
+      </c>
+      <c r="L2" s="32">
+        <f t="shared" ref="L2:AJ2" si="1">SUM(100/$AJ$1*L1)/100</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="M2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.32352941176470595</v>
+      </c>
+      <c r="N2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="O2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.38235294117647056</v>
+      </c>
+      <c r="P2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.41176470588235298</v>
+      </c>
+      <c r="Q2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.44117647058823534</v>
+      </c>
+      <c r="R2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.4705882352941177</v>
+      </c>
+      <c r="S2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="T2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.52941176470588236</v>
+      </c>
+      <c r="U2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.55882352941176483</v>
+      </c>
+      <c r="V2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="W2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.61764705882352944</v>
+      </c>
+      <c r="X2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.64705882352941191</v>
+      </c>
+      <c r="Y2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.67647058823529416</v>
+      </c>
+      <c r="Z2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="AA2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.73529411764705888</v>
+      </c>
+      <c r="AB2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="AC2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.79411764705882359</v>
+      </c>
+      <c r="AD2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.82352941176470595</v>
+      </c>
+      <c r="AE2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.85294117647058831</v>
+      </c>
+      <c r="AF2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.88235294117647067</v>
+      </c>
+      <c r="AG2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.91176470588235303</v>
+      </c>
+      <c r="AH2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.94117647058823539</v>
+      </c>
+      <c r="AI2" s="32">
+        <f t="shared" si="1"/>
+        <v>0.97058823529411764</v>
+      </c>
+      <c r="AJ2" s="32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" s="1" customFormat="1" ht="139">
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="17" thickBot="1">
+      <c r="A4" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>43367</v>
+      </c>
+      <c r="D4" s="16">
+        <v>43374</v>
+      </c>
+      <c r="E4" s="16">
+        <v>43381</v>
+      </c>
+      <c r="F4" s="16">
+        <v>43388</v>
+      </c>
+      <c r="G4" s="18">
+        <v>43395</v>
+      </c>
+      <c r="H4" s="16">
+        <v>43402</v>
+      </c>
+      <c r="I4" s="16">
+        <v>43409</v>
+      </c>
+      <c r="J4" s="16">
+        <v>43416</v>
+      </c>
+      <c r="K4" s="16">
+        <v>43423</v>
+      </c>
+      <c r="L4" s="16">
+        <v>43430</v>
+      </c>
+      <c r="M4" s="18">
+        <v>43437</v>
+      </c>
+      <c r="N4" s="16">
+        <v>43444</v>
+      </c>
+      <c r="O4" s="16">
+        <v>43451</v>
+      </c>
+      <c r="P4" s="16">
+        <v>43458</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>43465</v>
+      </c>
+      <c r="R4" s="16">
+        <v>43472</v>
+      </c>
+      <c r="S4" s="16">
+        <v>43479</v>
+      </c>
+      <c r="T4" s="16">
+        <v>43486</v>
+      </c>
+      <c r="U4" s="16">
+        <v>43493</v>
+      </c>
+      <c r="V4" s="16">
+        <v>43500</v>
+      </c>
+      <c r="W4" s="16">
+        <v>43507</v>
+      </c>
+      <c r="X4" s="16">
+        <v>43514</v>
+      </c>
+      <c r="Y4" s="16">
+        <v>43521</v>
+      </c>
+      <c r="Z4" s="16">
+        <v>43528</v>
+      </c>
+      <c r="AA4" s="16">
+        <v>43535</v>
+      </c>
+      <c r="AB4" s="16">
+        <v>43542</v>
+      </c>
+      <c r="AC4" s="16">
+        <v>43549</v>
+      </c>
+      <c r="AD4" s="16">
+        <v>43556</v>
+      </c>
+      <c r="AE4" s="18">
+        <v>43563</v>
+      </c>
+      <c r="AF4" s="16">
+        <v>43570</v>
+      </c>
+      <c r="AG4" s="16">
+        <v>43577</v>
+      </c>
+      <c r="AH4" s="16">
+        <v>43584</v>
+      </c>
+      <c r="AI4" s="16">
+        <v>43591</v>
+      </c>
+      <c r="AJ4" s="16">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="17" thickTop="1">
+      <c r="A5" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="G5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AG5" s="9"/>
+    </row>
+    <row r="6" spans="1:36">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AG6" s="9"/>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="20"/>
+      <c r="M7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AG7" s="9"/>
+    </row>
+    <row r="8" spans="1:36">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="21"/>
+      <c r="M8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AG8" s="9"/>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="21"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="2"/>
+      <c r="M9" s="19"/>
+      <c r="AE9" s="19"/>
+      <c r="AG9" s="9"/>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="21"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="M10" s="19"/>
+      <c r="AE10" s="19"/>
+      <c r="AG10" s="9"/>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="21"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AG11" s="9"/>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="21"/>
+      <c r="M12" s="20"/>
+      <c r="AE12" s="19"/>
+      <c r="AG12" s="9"/>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="9"/>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="9"/>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="21"/>
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="9"/>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="9"/>
+    </row>
+    <row r="17" spans="1:35">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="9"/>
+    </row>
+    <row r="18" spans="1:35">
+      <c r="A18" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="46"/>
+      <c r="G18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AG18" s="9"/>
+    </row>
+    <row r="19" spans="1:35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="AE19" s="19"/>
+      <c r="AG19" s="9"/>
+    </row>
+    <row r="20" spans="1:35">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="6"/>
+      <c r="M20" s="19"/>
+      <c r="AE20" s="19"/>
+      <c r="AG20" s="9"/>
+    </row>
+    <row r="21" spans="1:35">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="M21" s="19"/>
+      <c r="AE21" s="19"/>
+      <c r="AG21" s="9"/>
+    </row>
+    <row r="22" spans="1:35">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="M22" s="19"/>
+      <c r="AE22" s="19"/>
+      <c r="AG22" s="9"/>
+    </row>
+    <row r="23" spans="1:35">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="M23" s="19"/>
+      <c r="AE23" s="19"/>
+      <c r="AG23" s="9"/>
+    </row>
+    <row r="24" spans="1:35">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AE24" s="19"/>
+      <c r="AG24" s="9"/>
+    </row>
+    <row r="25" spans="1:35">
+      <c r="A25" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="48"/>
+      <c r="G25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="4"/>
+      <c r="AE25" s="19"/>
+      <c r="AG25" s="9"/>
+    </row>
+    <row r="26" spans="1:35">
+      <c r="A26" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="5"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="4"/>
+      <c r="AE26" s="19"/>
+      <c r="AG26" s="9"/>
+    </row>
+    <row r="27" spans="1:35">
+      <c r="A27" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="4"/>
+      <c r="AE27" s="19"/>
+      <c r="AG27" s="9"/>
+    </row>
+    <row r="28" spans="1:35">
+      <c r="A28" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="4"/>
+      <c r="AE28" s="19"/>
+      <c r="AG28" s="9"/>
+    </row>
+    <row r="29" spans="1:35">
+      <c r="A29" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AE29" s="19"/>
+      <c r="AG29" s="9"/>
+    </row>
+    <row r="30" spans="1:35">
+      <c r="A30" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="50"/>
+      <c r="G30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="AE30" s="19"/>
+      <c r="AG30" s="9"/>
+    </row>
+    <row r="31" spans="1:35">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="22"/>
+      <c r="AI31" s="22"/>
+    </row>
+    <row r="32" spans="1:35">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="AE32" s="19"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="22"/>
+      <c r="AI32" s="22"/>
+    </row>
+    <row r="33" spans="1:39">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="AE33" s="19"/>
+      <c r="AG33" s="9"/>
+      <c r="AJ33" s="22"/>
+    </row>
+    <row r="34" spans="1:39">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="AE34" s="19"/>
+      <c r="AG34" s="9"/>
+      <c r="AJ34" s="22"/>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="52"/>
+      <c r="G35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="AE35" s="19"/>
+      <c r="AG35" s="9"/>
+    </row>
+    <row r="36" spans="1:39">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="G36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="AE36" s="19"/>
+      <c r="AG36" s="9"/>
+    </row>
+    <row r="37" spans="1:39">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="G37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="AE37" s="19"/>
+      <c r="AG37" s="9"/>
+    </row>
+    <row r="38" spans="1:39">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="G38" s="31"/>
+      <c r="M38" s="19"/>
+      <c r="AE38" s="19"/>
+      <c r="AG38" s="9"/>
+    </row>
+    <row r="39" spans="1:39" s="4" customFormat="1">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="7"/>
+      <c r="AE39" s="21"/>
+      <c r="AG39" s="8"/>
+    </row>
+    <row r="40" spans="1:39">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="G40" s="21"/>
+      <c r="M40" s="19"/>
+      <c r="AE40" s="31"/>
+      <c r="AG40" s="9"/>
+    </row>
+    <row r="41" spans="1:39">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="AC41" s="8"/>
+      <c r="AD41" s="8"/>
+      <c r="AE41" s="19"/>
+      <c r="AG41" s="9"/>
+      <c r="AJ41" s="7"/>
+    </row>
+    <row r="42" spans="1:39">
+      <c r="A42" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="42"/>
+      <c r="G42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="AE42" s="19"/>
+      <c r="AG42" s="9"/>
+    </row>
+    <row r="43" spans="1:39">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="G43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="AE43" s="19"/>
+      <c r="AG43" s="9"/>
+    </row>
+    <row r="44" spans="1:39" s="9" customFormat="1">
+      <c r="A44" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44" s="19"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44" s="19"/>
+      <c r="N44"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44"/>
+      <c r="X44"/>
+      <c r="Y44"/>
+      <c r="Z44"/>
+      <c r="AA44"/>
+      <c r="AB44"/>
+      <c r="AC44"/>
+      <c r="AD44"/>
+      <c r="AE44" s="19"/>
+      <c r="AF44"/>
+      <c r="AM44" s="11"/>
+    </row>
+    <row r="45" spans="1:39" s="9" customFormat="1">
+      <c r="A45" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45" s="19"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45" s="19"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+      <c r="Y45"/>
+      <c r="Z45"/>
+      <c r="AA45"/>
+      <c r="AB45"/>
+      <c r="AC45"/>
+      <c r="AD45"/>
+      <c r="AE45" s="19"/>
+      <c r="AF45"/>
+    </row>
+    <row r="46" spans="1:39" s="9" customFormat="1">
+      <c r="A46" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46" s="19"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46" s="19"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+      <c r="Y46"/>
+      <c r="Z46"/>
+      <c r="AA46"/>
+      <c r="AB46"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="21"/>
+      <c r="AF46" s="3"/>
+      <c r="AG46" s="24"/>
+      <c r="AH46" s="24"/>
+      <c r="AI46" s="24"/>
+    </row>
+    <row r="47" spans="1:39" s="9" customFormat="1"/>
+    <row r="48" spans="1:39" s="9" customFormat="1"/>
+    <row r="49" s="9" customFormat="1"/>
+    <row r="50" s="9" customFormat="1"/>
+    <row r="51" s="9" customFormat="1"/>
+    <row r="52" s="9" customFormat="1"/>
+    <row r="53" s="9" customFormat="1"/>
+    <row r="54" s="9" customFormat="1"/>
+    <row r="55" s="9" customFormat="1"/>
+    <row r="56" s="9" customFormat="1"/>
+    <row r="57" s="9" customFormat="1"/>
+    <row r="58" s="9" customFormat="1"/>
+    <row r="59" s="9" customFormat="1"/>
+    <row r="60" s="9" customFormat="1"/>
+    <row r="61" s="9" customFormat="1"/>
+    <row r="62" s="9" customFormat="1"/>
+    <row r="63" s="9" customFormat="1"/>
+    <row r="64" s="9" customFormat="1"/>
+    <row r="65" spans="2:2" s="9" customFormat="1"/>
+    <row r="66" spans="2:2" s="9" customFormat="1"/>
+    <row r="67" spans="2:2" s="9" customFormat="1"/>
+    <row r="68" spans="2:2" s="9" customFormat="1"/>
+    <row r="69" spans="2:2" s="9" customFormat="1"/>
+    <row r="70" spans="2:2" s="9" customFormat="1"/>
+    <row r="71" spans="2:2" s="9" customFormat="1"/>
+    <row r="72" spans="2:2" s="9" customFormat="1"/>
+    <row r="73" spans="2:2" s="9" customFormat="1"/>
+    <row r="74" spans="2:2" s="9" customFormat="1"/>
+    <row r="75" spans="2:2" s="9" customFormat="1"/>
+    <row r="76" spans="2:2" s="9" customFormat="1"/>
+    <row r="77" spans="2:2">
+      <c r="B77" s="9"/>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="9"/>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A42:B42"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:AJ2">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B8D06D-6803-B645-A234-12FD1F5D03C7}">
   <dimension ref="A1:AM79"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
@@ -2069,11 +3276,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB78A94-45E5-D041-A9F3-CF4F27E90595}">
   <dimension ref="A1:AJ137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -4683,12 +5890,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A132:B132"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A63:B63"/>
@@ -4701,6 +5902,12 @@
     <mergeCell ref="A115:B115"/>
     <mergeCell ref="A120:B120"/>
     <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
Minor changes to workplan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leafeon/Desktop/G54IRP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D78F10-F4C1-154F-8A06-92001275E99D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60223A8-07D8-564B-BC59-5354486990D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="25600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="460" windowWidth="40960" windowHeight="25600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Active WorkPlan" sheetId="10" r:id="rId1"/>
@@ -20,12 +20,16 @@
     <sheet name="Project Proposal (Print)" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -493,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -666,11 +670,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -735,6 +842,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,30 +912,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1086,11 +1202,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13957A64-6344-8943-90F3-268E017FF0FC}">
   <dimension ref="A1:AM92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="110" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K50" sqref="K50"/>
+      <selection pane="bottomRight" activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1514,10 +1630,10 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="17" thickTop="1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="72"/>
       <c r="G5" s="19"/>
       <c r="M5" s="19"/>
       <c r="AE5" s="19"/>
@@ -1580,8 +1696,8 @@
       <c r="G9" s="21"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="69"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="19"/>
       <c r="AE9" s="19"/>
       <c r="AG9" s="9"/>
@@ -1597,11 +1713,11 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="21"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="55"/>
       <c r="AE10" s="19"/>
       <c r="AG10" s="9"/>
     </row>
@@ -1616,9 +1732,9 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="21"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="71"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="AE11" s="19"/>
       <c r="AG11" s="9"/>
     </row>
@@ -1646,7 +1762,7 @@
       </c>
       <c r="G13" s="19"/>
       <c r="M13" s="19"/>
-      <c r="AA13" s="2"/>
+      <c r="AA13" s="60"/>
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
@@ -1663,7 +1779,7 @@
       </c>
       <c r="G14" s="19"/>
       <c r="M14" s="19"/>
-      <c r="AA14" s="2"/>
+      <c r="AA14" s="61"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="4"/>
@@ -1723,10 +1839,10 @@
       <c r="AG17" s="9"/>
     </row>
     <row r="18" spans="1:33">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="74"/>
       <c r="G18" s="19"/>
       <c r="M18" s="19"/>
       <c r="AE18" s="19"/>
@@ -1801,10 +1917,10 @@
         <v>55</v>
       </c>
       <c r="G23" s="19"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="64"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
       <c r="AE23" s="19"/>
       <c r="AG23" s="9"/>
     </row>
@@ -1911,7 +2027,7 @@
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
-      <c r="Y27" s="6"/>
+      <c r="Y27" s="62"/>
       <c r="Z27" s="4"/>
       <c r="AE27" s="19"/>
       <c r="AG27" s="9"/>
@@ -1945,10 +2061,10 @@
       <c r="AG28" s="9"/>
     </row>
     <row r="29" spans="1:33">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="49"/>
+      <c r="B29" s="76"/>
       <c r="G29" s="19"/>
       <c r="M29" s="19"/>
       <c r="N29" s="4"/>
@@ -1996,9 +2112,9 @@
         <v>64</v>
       </c>
       <c r="G32" s="19"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
       <c r="M32" s="19"/>
       <c r="N32" s="4"/>
       <c r="AE32" s="19"/>
@@ -2146,9 +2262,9 @@
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="X38" s="4"/>
-      <c r="Y38" s="5"/>
-      <c r="Z38" s="5"/>
-      <c r="AA38" s="5"/>
+      <c r="Y38" s="63"/>
+      <c r="Z38" s="64"/>
+      <c r="AA38" s="65"/>
       <c r="AE38" s="19"/>
       <c r="AG38" s="9"/>
     </row>
@@ -2170,9 +2286,9 @@
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
       <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="5"/>
-      <c r="AA39" s="5"/>
+      <c r="Y39" s="66"/>
+      <c r="Z39" s="67"/>
+      <c r="AA39" s="68"/>
       <c r="AE39" s="19"/>
       <c r="AG39" s="9"/>
     </row>
@@ -2229,10 +2345,10 @@
       <c r="AG41" s="9"/>
     </row>
     <row r="42" spans="1:36">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="51"/>
+      <c r="B42" s="78"/>
       <c r="G42" s="19"/>
       <c r="M42" s="19"/>
       <c r="R42" s="4"/>
@@ -2297,10 +2413,10 @@
       <c r="AJ46" s="22"/>
     </row>
     <row r="47" spans="1:36">
-      <c r="A47" s="52" t="s">
+      <c r="A47" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="53"/>
+      <c r="B47" s="80"/>
       <c r="G47" s="19"/>
       <c r="M47" s="19"/>
       <c r="AE47" s="19"/>
@@ -2353,7 +2469,7 @@
         <v>89</v>
       </c>
       <c r="G51" s="21"/>
-      <c r="M51" s="61"/>
+      <c r="M51" s="48"/>
       <c r="N51" s="8"/>
       <c r="AE51" s="21"/>
       <c r="AG51" s="8"/>
@@ -2391,10 +2507,10 @@
       <c r="AJ53" s="7"/>
     </row>
     <row r="54" spans="1:39">
-      <c r="A54" s="42" t="s">
+      <c r="A54" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="43"/>
+      <c r="B54" s="70"/>
       <c r="G54" s="19"/>
       <c r="M54" s="19"/>
       <c r="AE54" s="19"/>
@@ -2547,8 +2663,8 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
-      <c r="K59" s="60"/>
-      <c r="L59" s="55"/>
+      <c r="K59" s="47"/>
+      <c r="L59" s="42"/>
       <c r="M59" s="21"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
@@ -2568,11 +2684,11 @@
       <c r="AC59" s="4"/>
       <c r="AD59" s="4"/>
       <c r="AE59" s="21"/>
-      <c r="AF59" s="56"/>
-      <c r="AG59" s="57"/>
-      <c r="AH59" s="57"/>
-      <c r="AI59" s="57"/>
-      <c r="AJ59" s="57"/>
+      <c r="AF59" s="43"/>
+      <c r="AG59" s="44"/>
+      <c r="AH59" s="44"/>
+      <c r="AI59" s="44"/>
+      <c r="AJ59" s="44"/>
     </row>
     <row r="60" spans="1:39" s="9" customFormat="1">
       <c r="F60" s="8"/>
@@ -3143,10 +3259,10 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="17" thickTop="1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="72"/>
       <c r="G5" s="19"/>
       <c r="M5" s="19"/>
       <c r="AE5" s="19"/>
@@ -3209,8 +3325,8 @@
       <c r="G9" s="21"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="69"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="19"/>
       <c r="AE9" s="19"/>
       <c r="AG9" s="9"/>
@@ -3226,11 +3342,11 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="21"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="55"/>
       <c r="AE10" s="19"/>
       <c r="AG10" s="9"/>
     </row>
@@ -3245,9 +3361,9 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="21"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="71"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="AE11" s="19"/>
       <c r="AG11" s="9"/>
     </row>
@@ -3352,10 +3468,10 @@
       <c r="AG17" s="9"/>
     </row>
     <row r="18" spans="1:33">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="74"/>
       <c r="G18" s="19"/>
       <c r="M18" s="19"/>
       <c r="AE18" s="19"/>
@@ -3430,10 +3546,10 @@
         <v>55</v>
       </c>
       <c r="G23" s="19"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="64"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
       <c r="AE23" s="19"/>
       <c r="AG23" s="9"/>
     </row>
@@ -3574,10 +3690,10 @@
       <c r="AG28" s="9"/>
     </row>
     <row r="29" spans="1:33">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="49"/>
+      <c r="B29" s="76"/>
       <c r="G29" s="19"/>
       <c r="M29" s="19"/>
       <c r="N29" s="4"/>
@@ -3625,9 +3741,9 @@
         <v>64</v>
       </c>
       <c r="G32" s="19"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
       <c r="M32" s="19"/>
       <c r="N32" s="4"/>
       <c r="AE32" s="19"/>
@@ -3858,10 +3974,10 @@
       <c r="AG41" s="9"/>
     </row>
     <row r="42" spans="1:36">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="51"/>
+      <c r="B42" s="78"/>
       <c r="G42" s="19"/>
       <c r="M42" s="19"/>
       <c r="R42" s="4"/>
@@ -3926,10 +4042,10 @@
       <c r="AJ46" s="22"/>
     </row>
     <row r="47" spans="1:36">
-      <c r="A47" s="52" t="s">
+      <c r="A47" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="53"/>
+      <c r="B47" s="80"/>
       <c r="G47" s="19"/>
       <c r="M47" s="19"/>
       <c r="AE47" s="19"/>
@@ -3982,7 +4098,7 @@
         <v>89</v>
       </c>
       <c r="G51" s="21"/>
-      <c r="M51" s="61"/>
+      <c r="M51" s="48"/>
       <c r="N51" s="8"/>
       <c r="AE51" s="21"/>
       <c r="AG51" s="8"/>
@@ -4020,10 +4136,10 @@
       <c r="AJ53" s="7"/>
     </row>
     <row r="54" spans="1:39">
-      <c r="A54" s="42" t="s">
+      <c r="A54" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="43"/>
+      <c r="B54" s="70"/>
       <c r="G54" s="19"/>
       <c r="M54" s="19"/>
       <c r="AE54" s="19"/>
@@ -4176,8 +4292,8 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
-      <c r="K59" s="60"/>
-      <c r="L59" s="55"/>
+      <c r="K59" s="47"/>
+      <c r="L59" s="42"/>
       <c r="M59" s="21"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
@@ -4197,11 +4313,11 @@
       <c r="AC59" s="4"/>
       <c r="AD59" s="4"/>
       <c r="AE59" s="21"/>
-      <c r="AF59" s="56"/>
-      <c r="AG59" s="57"/>
-      <c r="AH59" s="57"/>
-      <c r="AI59" s="57"/>
-      <c r="AJ59" s="57"/>
+      <c r="AF59" s="43"/>
+      <c r="AG59" s="44"/>
+      <c r="AH59" s="44"/>
+      <c r="AI59" s="44"/>
+      <c r="AJ59" s="44"/>
     </row>
     <row r="60" spans="1:39" s="9" customFormat="1">
       <c r="F60" s="8"/>
@@ -4308,12 +4424,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A54:B54"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="colorScale" priority="1">
@@ -4427,10 +4543,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" thickTop="1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="72"/>
       <c r="G3" s="19"/>
       <c r="M3" s="19"/>
     </row>
@@ -4485,8 +4601,8 @@
       <c r="G7" s="21"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="69"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="56"/>
       <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:13" ht="17" thickBot="1">
@@ -4500,11 +4616,11 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="21"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="68"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="55"/>
     </row>
     <row r="9" spans="1:13" ht="17" thickBot="1">
       <c r="A9" t="s">
@@ -4517,9 +4633,9 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="21"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="71"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="58"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
@@ -4535,10 +4651,10 @@
       <c r="M10" s="20"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="74"/>
       <c r="G11" s="19"/>
       <c r="M11" s="19"/>
     </row>
@@ -4603,16 +4719,16 @@
         <v>55</v>
       </c>
       <c r="G16" s="19"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="64"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="51"/>
     </row>
     <row r="17" spans="1:38">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="49"/>
+      <c r="B17" s="76"/>
       <c r="G17" s="19"/>
       <c r="M17" s="19"/>
     </row>
@@ -4649,9 +4765,9 @@
         <v>64</v>
       </c>
       <c r="G20" s="19"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
       <c r="M20" s="19"/>
     </row>
     <row r="21" spans="1:38" ht="17" thickBot="1">
@@ -4666,10 +4782,10 @@
       <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:38">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="53"/>
+      <c r="B22" s="80"/>
       <c r="G22" s="19"/>
       <c r="M22" s="19"/>
     </row>
@@ -4714,13 +4830,13 @@
         <v>89</v>
       </c>
       <c r="G26" s="21"/>
-      <c r="M26" s="61"/>
+      <c r="M26" s="48"/>
     </row>
     <row r="27" spans="1:38">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="43"/>
+      <c r="B27" s="70"/>
       <c r="G27" s="19"/>
       <c r="M27" s="19"/>
     </row>
@@ -4751,8 +4867,8 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="55"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="42"/>
       <c r="M29" s="21"/>
     </row>
     <row r="30" spans="1:38" s="9" customFormat="1">
@@ -4871,37 +4987,37 @@
       <c r="M32" s="16">
         <v>43514</v>
       </c>
-      <c r="N32" s="72"/>
-      <c r="O32" s="72"/>
-      <c r="P32" s="72"/>
-      <c r="Q32" s="72"/>
-      <c r="R32" s="72"/>
-      <c r="S32" s="72"/>
-      <c r="T32" s="72"/>
-      <c r="U32" s="72"/>
-      <c r="V32" s="72"/>
-      <c r="W32" s="72"/>
-      <c r="X32" s="72"/>
-      <c r="Y32" s="72"/>
-      <c r="Z32" s="72"/>
-      <c r="AA32" s="72"/>
-      <c r="AB32" s="72"/>
-      <c r="AC32" s="72"/>
-      <c r="AD32" s="72"/>
-      <c r="AE32" s="72"/>
-      <c r="AF32" s="72"/>
-      <c r="AG32" s="72"/>
-      <c r="AH32" s="72"/>
-      <c r="AI32" s="72"/>
-      <c r="AJ32" s="72"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="59"/>
+      <c r="P32" s="59"/>
+      <c r="Q32" s="59"/>
+      <c r="R32" s="59"/>
+      <c r="S32" s="59"/>
+      <c r="T32" s="59"/>
+      <c r="U32" s="59"/>
+      <c r="V32" s="59"/>
+      <c r="W32" s="59"/>
+      <c r="X32" s="59"/>
+      <c r="Y32" s="59"/>
+      <c r="Z32" s="59"/>
+      <c r="AA32" s="59"/>
+      <c r="AB32" s="59"/>
+      <c r="AC32" s="59"/>
+      <c r="AD32" s="59"/>
+      <c r="AE32" s="59"/>
+      <c r="AF32" s="59"/>
+      <c r="AG32" s="59"/>
+      <c r="AH32" s="59"/>
+      <c r="AI32" s="59"/>
+      <c r="AJ32" s="59"/>
       <c r="AK32" s="8"/>
       <c r="AL32" s="8"/>
     </row>
     <row r="33" spans="1:39" ht="17" thickTop="1">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="47"/>
+      <c r="B33" s="74"/>
       <c r="M33"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
@@ -5062,10 +5178,10 @@
       <c r="AL36" s="8"/>
     </row>
     <row r="37" spans="1:39">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="49"/>
+      <c r="B37" s="76"/>
       <c r="C37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -5402,10 +5518,10 @@
       <c r="AL44" s="8"/>
     </row>
     <row r="45" spans="1:39">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="43"/>
+      <c r="B45" s="70"/>
       <c r="M45"/>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
@@ -5635,36 +5751,36 @@
       <c r="N50" s="16">
         <v>43598</v>
       </c>
-      <c r="O50" s="72"/>
-      <c r="P50" s="72"/>
-      <c r="Q50" s="72"/>
-      <c r="R50" s="72"/>
-      <c r="S50" s="72"/>
-      <c r="T50" s="72"/>
-      <c r="U50" s="72"/>
-      <c r="V50" s="72"/>
-      <c r="W50" s="72"/>
-      <c r="X50" s="72"/>
-      <c r="Y50" s="72"/>
-      <c r="Z50" s="72"/>
-      <c r="AA50" s="72"/>
-      <c r="AB50" s="72"/>
-      <c r="AC50" s="72"/>
-      <c r="AD50" s="72"/>
-      <c r="AE50" s="72"/>
-      <c r="AF50" s="72"/>
-      <c r="AG50" s="72"/>
-      <c r="AH50" s="72"/>
-      <c r="AI50" s="72"/>
-      <c r="AJ50" s="72"/>
+      <c r="O50" s="59"/>
+      <c r="P50" s="59"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="59"/>
+      <c r="T50" s="59"/>
+      <c r="U50" s="59"/>
+      <c r="V50" s="59"/>
+      <c r="W50" s="59"/>
+      <c r="X50" s="59"/>
+      <c r="Y50" s="59"/>
+      <c r="Z50" s="59"/>
+      <c r="AA50" s="59"/>
+      <c r="AB50" s="59"/>
+      <c r="AC50" s="59"/>
+      <c r="AD50" s="59"/>
+      <c r="AE50" s="59"/>
+      <c r="AF50" s="59"/>
+      <c r="AG50" s="59"/>
+      <c r="AH50" s="59"/>
+      <c r="AI50" s="59"/>
+      <c r="AJ50" s="59"/>
       <c r="AK50" s="8"/>
       <c r="AL50" s="8"/>
     </row>
     <row r="51" spans="1:38" ht="17" thickTop="1">
-      <c r="A51" s="44" t="s">
+      <c r="A51" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="45"/>
+      <c r="B51" s="72"/>
       <c r="I51" s="19"/>
       <c r="K51" s="9"/>
       <c r="M51"/>
@@ -5894,10 +6010,10 @@
       <c r="AL56" s="8"/>
     </row>
     <row r="57" spans="1:38">
-      <c r="A57" s="46" t="s">
+      <c r="A57" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="47"/>
+      <c r="B57" s="74"/>
       <c r="I57" s="19"/>
       <c r="K57" s="9"/>
       <c r="M57"/>
@@ -6039,10 +6155,10 @@
       <c r="AL60" s="8"/>
     </row>
     <row r="61" spans="1:38">
-      <c r="A61" s="48" t="s">
+      <c r="A61" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="49"/>
+      <c r="B61" s="76"/>
       <c r="I61" s="19"/>
       <c r="K61" s="9"/>
       <c r="M61"/>
@@ -6185,10 +6301,10 @@
       <c r="AL64" s="8"/>
     </row>
     <row r="65" spans="1:38">
-      <c r="A65" s="50" t="s">
+      <c r="A65" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="51"/>
+      <c r="B65" s="78"/>
       <c r="I65" s="19"/>
       <c r="K65" s="9"/>
       <c r="M65"/>
@@ -6362,10 +6478,10 @@
       <c r="AL69" s="8"/>
     </row>
     <row r="70" spans="1:38">
-      <c r="A70" s="52" t="s">
+      <c r="A70" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="53"/>
+      <c r="B70" s="80"/>
       <c r="I70" s="19"/>
       <c r="K70" s="9"/>
       <c r="M70"/>
@@ -6468,10 +6584,10 @@
       <c r="AL72" s="8"/>
     </row>
     <row r="73" spans="1:38">
-      <c r="A73" s="42" t="s">
+      <c r="A73" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B73" s="43"/>
+      <c r="B73" s="70"/>
       <c r="I73" s="19"/>
       <c r="K73" s="9"/>
       <c r="M73"/>
@@ -6760,103 +6876,103 @@
         <v>0.26470588235294118</v>
       </c>
       <c r="L2" s="32">
-        <f t="shared" ref="L2" si="1">SUM(100/$AJ$1*L1)/100</f>
+        <f t="shared" ref="L2:AJ2" si="1">SUM(100/$AJ$1*L1)/100</f>
         <v>0.29411764705882354</v>
       </c>
       <c r="M2" s="32">
-        <f t="shared" ref="M2" si="2">SUM(100/$AJ$1*M1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.32352941176470595</v>
       </c>
       <c r="N2" s="32">
-        <f t="shared" ref="N2" si="3">SUM(100/$AJ$1*N1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.35294117647058826</v>
       </c>
       <c r="O2" s="32">
-        <f t="shared" ref="O2" si="4">SUM(100/$AJ$1*O1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.38235294117647056</v>
       </c>
       <c r="P2" s="32">
-        <f t="shared" ref="P2" si="5">SUM(100/$AJ$1*P1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.41176470588235298</v>
       </c>
       <c r="Q2" s="32">
-        <f t="shared" ref="Q2" si="6">SUM(100/$AJ$1*Q1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.44117647058823534</v>
       </c>
       <c r="R2" s="32">
-        <f t="shared" ref="R2:S2" si="7">SUM(100/$AJ$1*R1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.4705882352941177</v>
       </c>
       <c r="S2" s="32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="T2" s="32">
-        <f t="shared" ref="T2" si="8">SUM(100/$AJ$1*T1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.52941176470588236</v>
       </c>
       <c r="U2" s="32">
-        <f t="shared" ref="U2" si="9">SUM(100/$AJ$1*U1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.55882352941176483</v>
       </c>
       <c r="V2" s="32">
-        <f t="shared" ref="V2" si="10">SUM(100/$AJ$1*V1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.58823529411764708</v>
       </c>
       <c r="W2" s="32">
-        <f t="shared" ref="W2" si="11">SUM(100/$AJ$1*W1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.61764705882352944</v>
       </c>
       <c r="X2" s="32">
-        <f t="shared" ref="X2" si="12">SUM(100/$AJ$1*X1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.64705882352941191</v>
       </c>
       <c r="Y2" s="32">
-        <f t="shared" ref="Y2" si="13">SUM(100/$AJ$1*Y1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.67647058823529416</v>
       </c>
       <c r="Z2" s="32">
-        <f t="shared" ref="Z2:AA2" si="14">SUM(100/$AJ$1*Z1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.70588235294117652</v>
       </c>
       <c r="AA2" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>0.73529411764705888</v>
       </c>
       <c r="AB2" s="32">
-        <f t="shared" ref="AB2" si="15">SUM(100/$AJ$1*AB1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.76470588235294112</v>
       </c>
       <c r="AC2" s="32">
-        <f t="shared" ref="AC2" si="16">SUM(100/$AJ$1*AC1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.79411764705882359</v>
       </c>
       <c r="AD2" s="32">
-        <f t="shared" ref="AD2" si="17">SUM(100/$AJ$1*AD1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.82352941176470595</v>
       </c>
       <c r="AE2" s="32">
-        <f t="shared" ref="AE2" si="18">SUM(100/$AJ$1*AE1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.85294117647058831</v>
       </c>
       <c r="AF2" s="32">
-        <f t="shared" ref="AF2" si="19">SUM(100/$AJ$1*AF1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.88235294117647067</v>
       </c>
       <c r="AG2" s="32">
-        <f t="shared" ref="AG2" si="20">SUM(100/$AJ$1*AG1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.91176470588235303</v>
       </c>
       <c r="AH2" s="32">
-        <f t="shared" ref="AH2:AI2" si="21">SUM(100/$AJ$1*AH1)/100</f>
+        <f t="shared" si="1"/>
         <v>0.94117647058823539</v>
       </c>
       <c r="AI2" s="32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="1"/>
         <v>0.97058823529411764</v>
       </c>
       <c r="AJ2" s="32">
-        <f t="shared" ref="AJ2" si="22">SUM(100/$AJ$1*AJ1)/100</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7023,10 +7139,10 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="17" thickTop="1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="72"/>
       <c r="G5" s="19"/>
       <c r="M5" s="19"/>
       <c r="AE5" s="19"/>
@@ -7230,10 +7346,10 @@
       <c r="AG17" s="9"/>
     </row>
     <row r="18" spans="1:35">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="74"/>
       <c r="G18" s="19"/>
       <c r="M18" s="19"/>
       <c r="AE18" s="19"/>
@@ -7342,10 +7458,10 @@
       <c r="AG24" s="9"/>
     </row>
     <row r="25" spans="1:35">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="49"/>
+      <c r="B25" s="76"/>
       <c r="G25" s="19"/>
       <c r="M25" s="19"/>
       <c r="N25" s="4"/>
@@ -7423,10 +7539,10 @@
       <c r="AG29" s="9"/>
     </row>
     <row r="30" spans="1:35">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="51"/>
+      <c r="B30" s="78"/>
       <c r="G30" s="19"/>
       <c r="M30" s="19"/>
       <c r="U30" s="4"/>
@@ -7489,10 +7605,10 @@
       <c r="AJ34" s="22"/>
     </row>
     <row r="35" spans="1:39">
-      <c r="A35" s="52" t="s">
+      <c r="A35" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="53"/>
+      <c r="B35" s="80"/>
       <c r="G35" s="19"/>
       <c r="M35" s="19"/>
       <c r="AE35" s="19"/>
@@ -7583,10 +7699,10 @@
       <c r="AJ41" s="7"/>
     </row>
     <row r="42" spans="1:39">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="70"/>
       <c r="G42" s="19"/>
       <c r="M42" s="19"/>
       <c r="AE42" s="19"/>
@@ -8157,10 +8273,10 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="17" thickTop="1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="72"/>
       <c r="G5" s="19"/>
       <c r="M5" s="19"/>
     </row>
@@ -8313,10 +8429,10 @@
       <c r="M17" s="19"/>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="74"/>
       <c r="G18" s="19"/>
       <c r="M18" s="19"/>
     </row>
@@ -8405,10 +8521,10 @@
       <c r="T24" s="6"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="49"/>
+      <c r="B25" s="76"/>
       <c r="G25" s="19"/>
       <c r="M25" s="19"/>
       <c r="N25" s="4"/>
@@ -8470,10 +8586,10 @@
       <c r="T29" s="5"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="51"/>
+      <c r="B30" s="78"/>
       <c r="G30" s="19"/>
       <c r="M30" s="19"/>
     </row>
@@ -8518,10 +8634,10 @@
       <c r="M34" s="19"/>
     </row>
     <row r="35" spans="1:30">
-      <c r="A35" s="52" t="s">
+      <c r="A35" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="53"/>
+      <c r="B35" s="80"/>
       <c r="G35" s="19"/>
       <c r="M35" s="19"/>
     </row>
@@ -8595,10 +8711,10 @@
       <c r="T41" s="4"/>
     </row>
     <row r="42" spans="1:30">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="70"/>
       <c r="G42" s="19"/>
       <c r="M42" s="19"/>
     </row>
@@ -8788,10 +8904,10 @@
       <c r="AD49"/>
     </row>
     <row r="50" spans="1:30" s="9" customFormat="1" ht="17" thickTop="1">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="45"/>
+      <c r="B50" s="72"/>
       <c r="C50"/>
       <c r="D50"/>
       <c r="E50"/>
@@ -9150,10 +9266,10 @@
       <c r="AD62"/>
     </row>
     <row r="63" spans="1:30" s="9" customFormat="1">
-      <c r="A63" s="46" t="s">
+      <c r="A63" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="47"/>
+      <c r="B63" s="74"/>
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63"/>
@@ -9344,10 +9460,10 @@
       <c r="AD69"/>
     </row>
     <row r="70" spans="1:30" s="9" customFormat="1">
-      <c r="A70" s="48" t="s">
+      <c r="A70" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B70" s="49"/>
+      <c r="B70" s="76"/>
       <c r="C70"/>
       <c r="D70"/>
       <c r="E70"/>
@@ -9482,10 +9598,10 @@
       <c r="AD74"/>
     </row>
     <row r="75" spans="1:30" s="9" customFormat="1">
-      <c r="A75" s="50" t="s">
+      <c r="A75" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="51"/>
+      <c r="B75" s="78"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75"/>
@@ -9570,10 +9686,10 @@
       <c r="R79" s="22"/>
     </row>
     <row r="80" spans="1:30">
-      <c r="A80" s="52" t="s">
+      <c r="A80" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B80" s="53"/>
+      <c r="B80" s="80"/>
       <c r="M80" s="19"/>
       <c r="O80" s="9"/>
     </row>
@@ -9660,10 +9776,10 @@
       <c r="R86" s="7"/>
     </row>
     <row r="87" spans="1:30">
-      <c r="A87" s="42" t="s">
+      <c r="A87" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="43"/>
+      <c r="B87" s="70"/>
       <c r="M87" s="19"/>
       <c r="O87" s="9"/>
     </row>
@@ -9765,8 +9881,8 @@
       <c r="M94" s="8"/>
     </row>
     <row r="95" spans="1:30">
-      <c r="A95" s="54"/>
-      <c r="B95" s="54"/>
+      <c r="A95" s="81"/>
+      <c r="B95" s="81"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
@@ -9960,8 +10076,8 @@
       <c r="M107" s="8"/>
     </row>
     <row r="108" spans="1:13">
-      <c r="A108" s="54"/>
-      <c r="B108" s="54"/>
+      <c r="A108" s="81"/>
+      <c r="B108" s="81"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="8"/>
@@ -10065,8 +10181,8 @@
       <c r="M114" s="8"/>
     </row>
     <row r="115" spans="1:13">
-      <c r="A115" s="54"/>
-      <c r="B115" s="54"/>
+      <c r="A115" s="81"/>
+      <c r="B115" s="81"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
       <c r="E115" s="8"/>
@@ -10140,8 +10256,8 @@
       <c r="M119" s="8"/>
     </row>
     <row r="120" spans="1:13">
-      <c r="A120" s="54"/>
-      <c r="B120" s="54"/>
+      <c r="A120" s="81"/>
+      <c r="B120" s="81"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
@@ -10215,8 +10331,8 @@
       <c r="M124" s="8"/>
     </row>
     <row r="125" spans="1:13">
-      <c r="A125" s="54"/>
-      <c r="B125" s="54"/>
+      <c r="A125" s="81"/>
+      <c r="B125" s="81"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
@@ -10320,8 +10436,8 @@
       <c r="M131" s="8"/>
     </row>
     <row r="132" spans="1:13">
-      <c r="A132" s="54"/>
-      <c r="B132" s="54"/>
+      <c r="A132" s="81"/>
+      <c r="B132" s="81"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
       <c r="E132" s="8"/>

</xml_diff>